<commit_message>
Introducing the weather map module forecasting
</commit_message>
<xml_diff>
--- a/RAAL/Production/Input.xlsx
+++ b/RAAL/Production/Input.xlsx
@@ -1,39 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27126"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mynexte-my.sharepoint.com/personal/andrei_ionita_mynexte_com/Documents/Desktop/ML/Forecast_app/RAAL/Production/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_63394035982C51948A70C3114A033000466F0056" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D8438E6D-4B1E-4A2D-AC4C-9D8EFECE9E34}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="11_23F921ED593BCD51E76540BBD1E32D894E4C8F3F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EA96B214-9E7D-40C9-8FD0-A31C23732CB0}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="78">
   <si>
     <t>Data</t>
   </si>
@@ -48,6 +35,225 @@
   </si>
   <si>
     <t>Nori</t>
+  </si>
+  <si>
+    <t>Lookup</t>
+  </si>
+  <si>
+    <t>4532315</t>
+  </si>
+  <si>
+    <t>4532316</t>
+  </si>
+  <si>
+    <t>4532317</t>
+  </si>
+  <si>
+    <t>4532318</t>
+  </si>
+  <si>
+    <t>4532319</t>
+  </si>
+  <si>
+    <t>4532320</t>
+  </si>
+  <si>
+    <t>4532321</t>
+  </si>
+  <si>
+    <t>4532322</t>
+  </si>
+  <si>
+    <t>4532323</t>
+  </si>
+  <si>
+    <t>453240</t>
+  </si>
+  <si>
+    <t>453241</t>
+  </si>
+  <si>
+    <t>453242</t>
+  </si>
+  <si>
+    <t>453243</t>
+  </si>
+  <si>
+    <t>453244</t>
+  </si>
+  <si>
+    <t>453245</t>
+  </si>
+  <si>
+    <t>453246</t>
+  </si>
+  <si>
+    <t>453247</t>
+  </si>
+  <si>
+    <t>453248</t>
+  </si>
+  <si>
+    <t>453249</t>
+  </si>
+  <si>
+    <t>4532410</t>
+  </si>
+  <si>
+    <t>4532411</t>
+  </si>
+  <si>
+    <t>4532412</t>
+  </si>
+  <si>
+    <t>4532413</t>
+  </si>
+  <si>
+    <t>4532414</t>
+  </si>
+  <si>
+    <t>4532415</t>
+  </si>
+  <si>
+    <t>4532416</t>
+  </si>
+  <si>
+    <t>4532417</t>
+  </si>
+  <si>
+    <t>4532418</t>
+  </si>
+  <si>
+    <t>4532419</t>
+  </si>
+  <si>
+    <t>4532420</t>
+  </si>
+  <si>
+    <t>4532421</t>
+  </si>
+  <si>
+    <t>4532422</t>
+  </si>
+  <si>
+    <t>4532423</t>
+  </si>
+  <si>
+    <t>453250</t>
+  </si>
+  <si>
+    <t>453251</t>
+  </si>
+  <si>
+    <t>453252</t>
+  </si>
+  <si>
+    <t>453253</t>
+  </si>
+  <si>
+    <t>453254</t>
+  </si>
+  <si>
+    <t>453255</t>
+  </si>
+  <si>
+    <t>453256</t>
+  </si>
+  <si>
+    <t>453257</t>
+  </si>
+  <si>
+    <t>453258</t>
+  </si>
+  <si>
+    <t>453259</t>
+  </si>
+  <si>
+    <t>4532510</t>
+  </si>
+  <si>
+    <t>4532511</t>
+  </si>
+  <si>
+    <t>4532512</t>
+  </si>
+  <si>
+    <t>4532513</t>
+  </si>
+  <si>
+    <t>4532514</t>
+  </si>
+  <si>
+    <t>4532515</t>
+  </si>
+  <si>
+    <t>4532516</t>
+  </si>
+  <si>
+    <t>4532517</t>
+  </si>
+  <si>
+    <t>4532518</t>
+  </si>
+  <si>
+    <t>4532519</t>
+  </si>
+  <si>
+    <t>4532520</t>
+  </si>
+  <si>
+    <t>4532521</t>
+  </si>
+  <si>
+    <t>4532522</t>
+  </si>
+  <si>
+    <t>4532523</t>
+  </si>
+  <si>
+    <t>453260</t>
+  </si>
+  <si>
+    <t>453261</t>
+  </si>
+  <si>
+    <t>453262</t>
+  </si>
+  <si>
+    <t>453263</t>
+  </si>
+  <si>
+    <t>453264</t>
+  </si>
+  <si>
+    <t>453265</t>
+  </si>
+  <si>
+    <t>453266</t>
+  </si>
+  <si>
+    <t>453267</t>
+  </si>
+  <si>
+    <t>453268</t>
+  </si>
+  <si>
+    <t>453269</t>
+  </si>
+  <si>
+    <t>4532610</t>
+  </si>
+  <si>
+    <t>4532611</t>
+  </si>
+  <si>
+    <t>4532612</t>
+  </si>
+  <si>
+    <t>4532613</t>
+  </si>
+  <si>
+    <t>4532614</t>
   </si>
 </sst>
 </file>
@@ -55,9 +261,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="dd\.mm\.yyyy"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -73,10 +279,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -86,7 +288,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -109,30 +311,18 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="2"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="2"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+  <cellXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="2" xfId="2"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="3">
-    <cellStyle name="data_style" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name="date_style" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -435,25 +625,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:F97"/>
+  <dimension ref="A1:F73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N14" sqref="N14"/>
+      <selection activeCell="S13" sqref="S13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -468,655 +653,1449 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="3">
+      <c r="A2" s="2">
         <v>45323</v>
       </c>
       <c r="B2">
         <v>15</v>
       </c>
-      <c r="F2" s="2"/>
+      <c r="C2">
+        <v>234</v>
+      </c>
+      <c r="D2">
+        <v>2.1800000000000002</v>
+      </c>
+      <c r="E2">
+        <v>32</v>
+      </c>
+      <c r="F2" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
+      <c r="A3" s="2">
         <v>45323</v>
       </c>
       <c r="B3">
         <v>16</v>
       </c>
+      <c r="C3">
+        <v>100.8</v>
+      </c>
+      <c r="D3">
+        <v>1.29</v>
+      </c>
+      <c r="E3">
+        <v>32</v>
+      </c>
+      <c r="F3" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
+      <c r="A4" s="2">
         <v>45323</v>
       </c>
       <c r="B4">
         <v>17</v>
       </c>
+      <c r="C4">
+        <v>6.07</v>
+      </c>
+      <c r="D4">
+        <v>0.69</v>
+      </c>
+      <c r="E4">
+        <v>39</v>
+      </c>
+      <c r="F4" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
+      <c r="A5" s="2">
         <v>45323</v>
       </c>
       <c r="B5">
         <v>18</v>
       </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0.35</v>
+      </c>
+      <c r="E5">
+        <v>49</v>
+      </c>
+      <c r="F5" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
+      <c r="A6" s="2">
         <v>45323</v>
       </c>
       <c r="B6">
         <v>19</v>
       </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>-0.2</v>
+      </c>
+      <c r="E6">
+        <v>100</v>
+      </c>
+      <c r="F6" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
+      <c r="A7" s="2">
         <v>45323</v>
       </c>
       <c r="B7">
         <v>20</v>
       </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>-0.87</v>
+      </c>
+      <c r="E7">
+        <v>100</v>
+      </c>
+      <c r="F7" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
+      <c r="A8" s="2">
         <v>45323</v>
       </c>
       <c r="B8">
         <v>21</v>
       </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>-0.21</v>
+      </c>
+      <c r="E8">
+        <v>100</v>
+      </c>
+      <c r="F8" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="3">
+      <c r="A9" s="2">
         <v>45323</v>
       </c>
       <c r="B9">
         <v>22</v>
       </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>-0.66</v>
+      </c>
+      <c r="E9">
+        <v>100</v>
+      </c>
+      <c r="F9" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="3">
+      <c r="A10" s="2">
         <v>45323</v>
       </c>
       <c r="B10">
         <v>23</v>
       </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>-1.29</v>
+      </c>
+      <c r="E10">
+        <v>100</v>
+      </c>
+      <c r="F10" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="3">
+      <c r="A11" s="2">
         <v>45324</v>
       </c>
       <c r="B11">
         <v>0</v>
       </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>-1.36</v>
+      </c>
+      <c r="E11">
+        <v>100</v>
+      </c>
+      <c r="F11" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="3">
+      <c r="A12" s="2">
         <v>45324</v>
       </c>
       <c r="B12">
         <v>1</v>
       </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>-1.36</v>
+      </c>
+      <c r="E12">
+        <v>100</v>
+      </c>
+      <c r="F12" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="3">
+      <c r="A13" s="2">
         <v>45324</v>
       </c>
       <c r="B13">
         <v>2</v>
       </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>-1.21</v>
+      </c>
+      <c r="E13">
+        <v>100</v>
+      </c>
+      <c r="F13" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="3">
+      <c r="A14" s="2">
         <v>45324</v>
       </c>
       <c r="B14">
         <v>3</v>
       </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>-0.7</v>
+      </c>
+      <c r="E14">
+        <v>100</v>
+      </c>
+      <c r="F14" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="3">
+      <c r="A15" s="2">
         <v>45324</v>
       </c>
       <c r="B15">
         <v>4</v>
       </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>-0.63</v>
+      </c>
+      <c r="E15">
+        <v>100</v>
+      </c>
+      <c r="F15" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="3">
+      <c r="A16" s="2">
         <v>45324</v>
       </c>
       <c r="B16">
         <v>5</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="3">
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>-0.59</v>
+      </c>
+      <c r="E16">
+        <v>100</v>
+      </c>
+      <c r="F16" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
         <v>45324</v>
       </c>
       <c r="B17">
         <v>6</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="3">
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>-0.76</v>
+      </c>
+      <c r="E17">
+        <v>100</v>
+      </c>
+      <c r="F17" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
         <v>45324</v>
       </c>
       <c r="B18">
         <v>7</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="3">
+      <c r="C18">
+        <v>0.25</v>
+      </c>
+      <c r="D18">
+        <v>-0.8</v>
+      </c>
+      <c r="E18">
+        <v>100</v>
+      </c>
+      <c r="F18" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
         <v>45324</v>
       </c>
       <c r="B19">
         <v>8</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="3">
+      <c r="C19">
+        <v>18.23</v>
+      </c>
+      <c r="D19">
+        <v>-0.6</v>
+      </c>
+      <c r="E19">
+        <v>100</v>
+      </c>
+      <c r="F19" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
         <v>45324</v>
       </c>
       <c r="B20">
         <v>9</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="3">
+      <c r="C20">
+        <v>51.87</v>
+      </c>
+      <c r="D20">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="E20">
+        <v>100</v>
+      </c>
+      <c r="F20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
         <v>45324</v>
       </c>
       <c r="B21">
         <v>10</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="3">
+      <c r="C21">
+        <v>82.96</v>
+      </c>
+      <c r="D21">
+        <v>0.67</v>
+      </c>
+      <c r="E21">
+        <v>99</v>
+      </c>
+      <c r="F21" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
         <v>45324</v>
       </c>
       <c r="B22">
         <v>11</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="3">
+      <c r="C22">
+        <v>106.83</v>
+      </c>
+      <c r="D22">
+        <v>0.63</v>
+      </c>
+      <c r="E22">
+        <v>99</v>
+      </c>
+      <c r="F22" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
         <v>45324</v>
       </c>
       <c r="B23">
         <v>12</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="3">
+      <c r="C23">
+        <v>115.54</v>
+      </c>
+      <c r="D23">
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="E23">
+        <v>98</v>
+      </c>
+      <c r="F23" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="2">
         <v>45324</v>
       </c>
       <c r="B24">
         <v>13</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="3">
+      <c r="C24">
+        <v>114.53</v>
+      </c>
+      <c r="D24">
+        <v>1.64</v>
+      </c>
+      <c r="E24">
+        <v>92</v>
+      </c>
+      <c r="F24" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="2">
         <v>45324</v>
       </c>
       <c r="B25">
         <v>14</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="3">
+      <c r="C25">
+        <v>119.05</v>
+      </c>
+      <c r="D25">
+        <v>1.69</v>
+      </c>
+      <c r="E25">
+        <v>94</v>
+      </c>
+      <c r="F25" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="2">
         <v>45324</v>
       </c>
       <c r="B26">
         <v>15</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="3">
+      <c r="C26">
+        <v>95.68</v>
+      </c>
+      <c r="D26">
+        <v>0.04</v>
+      </c>
+      <c r="E26">
+        <v>93</v>
+      </c>
+      <c r="F26" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="2">
         <v>45324</v>
       </c>
       <c r="B27">
         <v>16</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="3">
+      <c r="C27">
+        <v>37.15</v>
+      </c>
+      <c r="D27">
+        <v>-1.92</v>
+      </c>
+      <c r="E27">
+        <v>83</v>
+      </c>
+      <c r="F27" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="2">
         <v>45324</v>
       </c>
       <c r="B28">
         <v>17</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="3">
+      <c r="C28">
+        <v>1.72</v>
+      </c>
+      <c r="D28">
+        <v>-2.35</v>
+      </c>
+      <c r="E28">
+        <v>78</v>
+      </c>
+      <c r="F28" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="2">
         <v>45324</v>
       </c>
       <c r="B29">
         <v>18</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="3">
+      <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="D29">
+        <v>-2.37</v>
+      </c>
+      <c r="E29">
+        <v>78</v>
+      </c>
+      <c r="F29" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="2">
         <v>45324</v>
       </c>
       <c r="B30">
         <v>19</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="3">
+      <c r="C30">
+        <v>0</v>
+      </c>
+      <c r="D30">
+        <v>-2.65</v>
+      </c>
+      <c r="E30">
+        <v>52</v>
+      </c>
+      <c r="F30" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="2">
         <v>45324</v>
       </c>
       <c r="B31">
         <v>20</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="3">
+      <c r="C31">
+        <v>0</v>
+      </c>
+      <c r="D31">
+        <v>-2.78</v>
+      </c>
+      <c r="E31">
+        <v>50</v>
+      </c>
+      <c r="F31" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="2">
         <v>45324</v>
       </c>
       <c r="B32">
         <v>21</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="3">
+      <c r="C32">
+        <v>0</v>
+      </c>
+      <c r="D32">
+        <v>-2.4500000000000002</v>
+      </c>
+      <c r="E32">
+        <v>67</v>
+      </c>
+      <c r="F32" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="2">
         <v>45324</v>
       </c>
       <c r="B33">
         <v>22</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="3">
+      <c r="C33">
+        <v>0</v>
+      </c>
+      <c r="D33">
+        <v>-1.83</v>
+      </c>
+      <c r="E33">
+        <v>75</v>
+      </c>
+      <c r="F33" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="2">
         <v>45324</v>
       </c>
       <c r="B34">
         <v>23</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="3">
+      <c r="C34">
+        <v>0</v>
+      </c>
+      <c r="D34">
+        <v>-1.54</v>
+      </c>
+      <c r="E34">
+        <v>80</v>
+      </c>
+      <c r="F34" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="2">
         <v>45325</v>
       </c>
       <c r="B35">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="3">
+      <c r="C35">
+        <v>0</v>
+      </c>
+      <c r="D35">
+        <v>-2.2400000000000002</v>
+      </c>
+      <c r="E35">
+        <v>83</v>
+      </c>
+      <c r="F35" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="2">
         <v>45325</v>
       </c>
       <c r="B36">
         <v>1</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="3">
+      <c r="C36">
+        <v>0</v>
+      </c>
+      <c r="D36">
+        <v>-2.25</v>
+      </c>
+      <c r="E36">
+        <v>100</v>
+      </c>
+      <c r="F36" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="2">
         <v>45325</v>
       </c>
       <c r="B37">
         <v>2</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="3">
+      <c r="C37">
+        <v>0</v>
+      </c>
+      <c r="D37">
+        <v>-2.1</v>
+      </c>
+      <c r="E37">
+        <v>98</v>
+      </c>
+      <c r="F37" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="2">
         <v>45325</v>
       </c>
       <c r="B38">
         <v>3</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="3">
+      <c r="C38">
+        <v>0</v>
+      </c>
+      <c r="D38">
+        <v>-2.25</v>
+      </c>
+      <c r="E38">
+        <v>94</v>
+      </c>
+      <c r="F38" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="2">
         <v>45325</v>
       </c>
       <c r="B39">
         <v>4</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="3">
+      <c r="C39">
+        <v>0</v>
+      </c>
+      <c r="D39">
+        <v>-0.67</v>
+      </c>
+      <c r="E39">
+        <v>95</v>
+      </c>
+      <c r="F39" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="2">
         <v>45325</v>
       </c>
       <c r="B40">
         <v>5</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="3">
+      <c r="C40">
+        <v>0</v>
+      </c>
+      <c r="D40">
+        <v>-0.18</v>
+      </c>
+      <c r="E40">
+        <v>96</v>
+      </c>
+      <c r="F40" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="2">
         <v>45325</v>
       </c>
       <c r="B41">
         <v>6</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="3">
+      <c r="C41">
+        <v>0</v>
+      </c>
+      <c r="D41">
+        <v>-0.14000000000000001</v>
+      </c>
+      <c r="E41">
+        <v>96</v>
+      </c>
+      <c r="F41" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="2">
         <v>45325</v>
       </c>
       <c r="B42">
         <v>7</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="3">
+      <c r="C42">
+        <v>0.45</v>
+      </c>
+      <c r="D42">
+        <v>-0.37</v>
+      </c>
+      <c r="E42">
+        <v>100</v>
+      </c>
+      <c r="F42" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="2">
         <v>45325</v>
       </c>
       <c r="B43">
         <v>8</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="3">
+      <c r="C43">
+        <v>22.36</v>
+      </c>
+      <c r="D43">
+        <v>-0.04</v>
+      </c>
+      <c r="E43">
+        <v>100</v>
+      </c>
+      <c r="F43" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="2">
         <v>45325</v>
       </c>
       <c r="B44">
         <v>9</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="3">
+      <c r="C44">
+        <v>52.91</v>
+      </c>
+      <c r="D44">
+        <v>0.7</v>
+      </c>
+      <c r="E44">
+        <v>100</v>
+      </c>
+      <c r="F44" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="2">
         <v>45325</v>
       </c>
       <c r="B45">
         <v>10</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" s="3">
+      <c r="C45">
+        <v>82.6</v>
+      </c>
+      <c r="D45">
+        <v>1.28</v>
+      </c>
+      <c r="E45">
+        <v>100</v>
+      </c>
+      <c r="F45" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" s="2">
         <v>45325</v>
       </c>
       <c r="B46">
         <v>11</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="3">
+      <c r="C46">
+        <v>102.6</v>
+      </c>
+      <c r="D46">
+        <v>1.71</v>
+      </c>
+      <c r="E46">
+        <v>100</v>
+      </c>
+      <c r="F46" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="2">
         <v>45325</v>
       </c>
       <c r="B47">
         <v>12</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" s="3">
+      <c r="C47">
+        <v>110.31</v>
+      </c>
+      <c r="D47">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="E47">
+        <v>100</v>
+      </c>
+      <c r="F47" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="2">
         <v>45325</v>
       </c>
       <c r="B48">
         <v>13</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="3">
+      <c r="C48">
+        <v>104.9</v>
+      </c>
+      <c r="D48">
+        <v>2.31</v>
+      </c>
+      <c r="E48">
+        <v>100</v>
+      </c>
+      <c r="F48" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="2">
         <v>45325</v>
       </c>
       <c r="B49">
         <v>14</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="3">
+      <c r="C49">
+        <v>87.56</v>
+      </c>
+      <c r="D49">
+        <v>2.14</v>
+      </c>
+      <c r="E49">
+        <v>100</v>
+      </c>
+      <c r="F49" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="2">
         <v>45325</v>
       </c>
       <c r="B50">
         <v>15</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="3">
+      <c r="C50">
+        <v>60.17</v>
+      </c>
+      <c r="D50">
+        <v>1.81</v>
+      </c>
+      <c r="E50">
+        <v>100</v>
+      </c>
+      <c r="F50" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" s="2">
         <v>45325</v>
       </c>
       <c r="B51">
         <v>16</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="3">
+      <c r="C51">
+        <v>25.67</v>
+      </c>
+      <c r="D51">
+        <v>1.67</v>
+      </c>
+      <c r="E51">
+        <v>100</v>
+      </c>
+      <c r="F51" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" s="2">
         <v>45325</v>
       </c>
       <c r="B52">
         <v>17</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" s="3">
+      <c r="C52">
+        <v>1.27</v>
+      </c>
+      <c r="D52">
+        <v>1.61</v>
+      </c>
+      <c r="E52">
+        <v>100</v>
+      </c>
+      <c r="F52" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" s="2">
         <v>45325</v>
       </c>
       <c r="B53">
         <v>18</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" s="3">
+      <c r="C53">
+        <v>0</v>
+      </c>
+      <c r="D53">
+        <v>1.67</v>
+      </c>
+      <c r="E53">
+        <v>100</v>
+      </c>
+      <c r="F53" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" s="2">
         <v>45325</v>
       </c>
       <c r="B54">
         <v>19</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" s="3">
+      <c r="C54">
+        <v>0</v>
+      </c>
+      <c r="D54">
+        <v>1.8</v>
+      </c>
+      <c r="E54">
+        <v>98</v>
+      </c>
+      <c r="F54" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" s="2">
         <v>45325</v>
       </c>
       <c r="B55">
         <v>20</v>
       </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" s="3">
+      <c r="C55">
+        <v>0</v>
+      </c>
+      <c r="D55">
+        <v>1.83</v>
+      </c>
+      <c r="E55">
+        <v>99</v>
+      </c>
+      <c r="F55" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" s="2">
         <v>45325</v>
       </c>
       <c r="B56">
         <v>21</v>
       </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" s="3">
+      <c r="C56">
+        <v>0</v>
+      </c>
+      <c r="D56">
+        <v>2.1</v>
+      </c>
+      <c r="E56">
+        <v>99</v>
+      </c>
+      <c r="F56" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" s="2">
         <v>45325</v>
       </c>
       <c r="B57">
         <v>22</v>
       </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" s="3">
+      <c r="C57">
+        <v>0</v>
+      </c>
+      <c r="D57">
+        <v>2.19</v>
+      </c>
+      <c r="E57">
+        <v>100</v>
+      </c>
+      <c r="F57" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" s="2">
         <v>45325</v>
       </c>
       <c r="B58">
         <v>23</v>
       </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" s="3">
+      <c r="C58">
+        <v>0</v>
+      </c>
+      <c r="D58">
+        <v>2.4700000000000002</v>
+      </c>
+      <c r="E58">
+        <v>100</v>
+      </c>
+      <c r="F58" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" s="2">
         <v>45326</v>
       </c>
       <c r="B59">
         <v>0</v>
       </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" s="3">
+      <c r="C59">
+        <v>0</v>
+      </c>
+      <c r="D59">
+        <v>2.42</v>
+      </c>
+      <c r="E59">
+        <v>99</v>
+      </c>
+      <c r="F59" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" s="2">
         <v>45326</v>
       </c>
       <c r="B60">
         <v>1</v>
       </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" s="3">
+      <c r="C60">
+        <v>0</v>
+      </c>
+      <c r="D60">
+        <v>1.56</v>
+      </c>
+      <c r="E60">
+        <v>90</v>
+      </c>
+      <c r="F60" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" s="2">
         <v>45326</v>
       </c>
       <c r="B61">
         <v>2</v>
       </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" s="3">
+      <c r="C61">
+        <v>0</v>
+      </c>
+      <c r="D61">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="E61">
+        <v>95</v>
+      </c>
+      <c r="F61" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" s="2">
         <v>45326</v>
       </c>
       <c r="B62">
         <v>3</v>
       </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" s="3">
+      <c r="C62">
+        <v>0</v>
+      </c>
+      <c r="D62">
+        <v>2.81</v>
+      </c>
+      <c r="E62">
+        <v>97</v>
+      </c>
+      <c r="F62" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" s="2">
         <v>45326</v>
       </c>
       <c r="B63">
         <v>4</v>
       </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" s="3">
+      <c r="C63">
+        <v>0</v>
+      </c>
+      <c r="D63">
+        <v>2.92</v>
+      </c>
+      <c r="E63">
+        <v>97</v>
+      </c>
+      <c r="F63" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" s="2">
         <v>45326</v>
       </c>
       <c r="B64">
         <v>5</v>
       </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" s="3">
+      <c r="C64">
+        <v>0</v>
+      </c>
+      <c r="D64">
+        <v>3.08</v>
+      </c>
+      <c r="E64">
+        <v>98</v>
+      </c>
+      <c r="F64" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65" s="2">
         <v>45326</v>
       </c>
       <c r="B65">
         <v>6</v>
       </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" s="3">
+      <c r="C65">
+        <v>0</v>
+      </c>
+      <c r="D65">
+        <v>3.24</v>
+      </c>
+      <c r="E65">
+        <v>98</v>
+      </c>
+      <c r="F65" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66" s="2">
         <v>45326</v>
       </c>
       <c r="B66">
         <v>7</v>
       </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" s="3">
+      <c r="C66">
+        <v>0.15</v>
+      </c>
+      <c r="D66">
+        <v>3.71</v>
+      </c>
+      <c r="E66">
+        <v>100</v>
+      </c>
+      <c r="F66" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67" s="2">
         <v>45326</v>
       </c>
       <c r="B67">
         <v>8</v>
       </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68" s="3">
+      <c r="C67">
+        <v>18.05</v>
+      </c>
+      <c r="D67">
+        <v>4.47</v>
+      </c>
+      <c r="E67">
+        <v>100</v>
+      </c>
+      <c r="F67" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A68" s="2">
         <v>45326</v>
       </c>
       <c r="B68">
         <v>9</v>
       </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" s="3">
+      <c r="C68">
+        <v>51.42</v>
+      </c>
+      <c r="D68">
+        <v>5.15</v>
+      </c>
+      <c r="E68">
+        <v>100</v>
+      </c>
+      <c r="F68" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A69" s="2">
         <v>45326</v>
       </c>
       <c r="B69">
         <v>10</v>
       </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70" s="3">
+      <c r="C69">
+        <v>81.81</v>
+      </c>
+      <c r="D69">
+        <v>5.96</v>
+      </c>
+      <c r="E69">
+        <v>100</v>
+      </c>
+      <c r="F69" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A70" s="2">
         <v>45326</v>
       </c>
       <c r="B70">
         <v>11</v>
       </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71" s="3">
+      <c r="C70">
+        <v>102.75</v>
+      </c>
+      <c r="D70">
+        <v>6.18</v>
+      </c>
+      <c r="E70">
+        <v>100</v>
+      </c>
+      <c r="F70" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A71" s="2">
         <v>45326</v>
       </c>
       <c r="B71">
         <v>12</v>
       </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A72" s="3">
+      <c r="C71">
+        <v>111.49</v>
+      </c>
+      <c r="D71">
+        <v>5.95</v>
+      </c>
+      <c r="E71">
+        <v>100</v>
+      </c>
+      <c r="F71" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A72" s="2">
         <v>45326</v>
       </c>
       <c r="B72">
         <v>13</v>
       </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A73" s="3">
+      <c r="C72">
+        <v>107.01</v>
+      </c>
+      <c r="D72">
+        <v>5.54</v>
+      </c>
+      <c r="E72">
+        <v>100</v>
+      </c>
+      <c r="F72" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A73" s="2">
         <v>45326</v>
       </c>
       <c r="B73">
         <v>14</v>
       </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A74" s="3"/>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75" s="3"/>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A76" s="3"/>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77" s="3"/>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A78" s="3"/>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A79" s="3"/>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A80" s="3"/>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A81" s="3"/>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A82" s="3"/>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A83" s="3"/>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A84" s="3"/>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A85" s="3"/>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A86" s="3"/>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A87" s="3"/>
-    </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A88" s="3"/>
-    </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A89" s="3"/>
-    </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A90" s="3"/>
-    </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A91" s="3"/>
-    </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A92" s="3"/>
-    </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A93" s="3"/>
-    </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A94" s="3"/>
-    </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A95" s="3"/>
-    </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A96" s="3"/>
-    </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A97" s="3"/>
+      <c r="C73">
+        <v>89.84</v>
+      </c>
+      <c r="D73">
+        <v>5.03</v>
+      </c>
+      <c r="E73">
+        <v>100</v>
+      </c>
+      <c r="F73" t="s">
+        <v>77</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Adding the weathermap forecast for RAAL
</commit_message>
<xml_diff>
--- a/RAAL/Production/Input.xlsx
+++ b/RAAL/Production/Input.xlsx
@@ -1,26 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27126"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mynexte-my.sharepoint.com/personal/andrei_ionita_mynexte_com/Documents/Desktop/ML/Forecast_app/RAAL/Production/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="11_23F921ED593BCD51E76540BBD1E32D894E4C8F3F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EA96B214-9E7D-40C9-8FD0-A31C23732CB0}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="102">
   <si>
     <t>Data</t>
   </si>
@@ -40,230 +34,302 @@
     <t>Lookup</t>
   </si>
   <si>
-    <t>4532315</t>
-  </si>
-  <si>
-    <t>4532316</t>
-  </si>
-  <si>
-    <t>4532317</t>
-  </si>
-  <si>
-    <t>4532318</t>
-  </si>
-  <si>
-    <t>4532319</t>
-  </si>
-  <si>
-    <t>4532320</t>
-  </si>
-  <si>
-    <t>4532321</t>
-  </si>
-  <si>
-    <t>4532322</t>
-  </si>
-  <si>
-    <t>4532323</t>
-  </si>
-  <si>
-    <t>453240</t>
-  </si>
-  <si>
-    <t>453241</t>
-  </si>
-  <si>
-    <t>453242</t>
-  </si>
-  <si>
-    <t>453243</t>
-  </si>
-  <si>
-    <t>453244</t>
-  </si>
-  <si>
-    <t>453245</t>
-  </si>
-  <si>
-    <t>453246</t>
-  </si>
-  <si>
-    <t>453247</t>
-  </si>
-  <si>
-    <t>453248</t>
-  </si>
-  <si>
-    <t>453249</t>
-  </si>
-  <si>
-    <t>4532410</t>
-  </si>
-  <si>
-    <t>4532411</t>
-  </si>
-  <si>
-    <t>4532412</t>
-  </si>
-  <si>
-    <t>4532413</t>
-  </si>
-  <si>
-    <t>4532414</t>
-  </si>
-  <si>
-    <t>4532415</t>
-  </si>
-  <si>
-    <t>4532416</t>
-  </si>
-  <si>
-    <t>4532417</t>
-  </si>
-  <si>
-    <t>4532418</t>
-  </si>
-  <si>
-    <t>4532419</t>
-  </si>
-  <si>
-    <t>4532420</t>
-  </si>
-  <si>
-    <t>4532421</t>
-  </si>
-  <si>
-    <t>4532422</t>
-  </si>
-  <si>
-    <t>4532423</t>
-  </si>
-  <si>
-    <t>453250</t>
-  </si>
-  <si>
-    <t>453251</t>
-  </si>
-  <si>
-    <t>453252</t>
-  </si>
-  <si>
-    <t>453253</t>
-  </si>
-  <si>
-    <t>453254</t>
-  </si>
-  <si>
-    <t>453255</t>
-  </si>
-  <si>
-    <t>453256</t>
-  </si>
-  <si>
-    <t>453257</t>
-  </si>
-  <si>
-    <t>453258</t>
-  </si>
-  <si>
-    <t>453259</t>
-  </si>
-  <si>
-    <t>4532510</t>
-  </si>
-  <si>
-    <t>4532511</t>
-  </si>
-  <si>
-    <t>4532512</t>
-  </si>
-  <si>
-    <t>4532513</t>
-  </si>
-  <si>
-    <t>4532514</t>
-  </si>
-  <si>
-    <t>4532515</t>
-  </si>
-  <si>
-    <t>4532516</t>
-  </si>
-  <si>
-    <t>4532517</t>
-  </si>
-  <si>
-    <t>4532518</t>
-  </si>
-  <si>
-    <t>4532519</t>
-  </si>
-  <si>
-    <t>4532520</t>
-  </si>
-  <si>
-    <t>4532521</t>
-  </si>
-  <si>
-    <t>4532522</t>
-  </si>
-  <si>
-    <t>4532523</t>
-  </si>
-  <si>
-    <t>453260</t>
-  </si>
-  <si>
-    <t>453261</t>
-  </si>
-  <si>
-    <t>453262</t>
-  </si>
-  <si>
-    <t>453263</t>
-  </si>
-  <si>
-    <t>453264</t>
-  </si>
-  <si>
-    <t>453265</t>
-  </si>
-  <si>
-    <t>453266</t>
-  </si>
-  <si>
-    <t>453267</t>
-  </si>
-  <si>
-    <t>453268</t>
-  </si>
-  <si>
-    <t>453269</t>
-  </si>
-  <si>
-    <t>4532610</t>
-  </si>
-  <si>
-    <t>4532611</t>
-  </si>
-  <si>
-    <t>4532612</t>
-  </si>
-  <si>
-    <t>4532613</t>
-  </si>
-  <si>
-    <t>4532614</t>
+    <t>05.02.202413</t>
+  </si>
+  <si>
+    <t>05.02.202414</t>
+  </si>
+  <si>
+    <t>05.02.202415</t>
+  </si>
+  <si>
+    <t>05.02.202416</t>
+  </si>
+  <si>
+    <t>05.02.202417</t>
+  </si>
+  <si>
+    <t>05.02.202418</t>
+  </si>
+  <si>
+    <t>05.02.202419</t>
+  </si>
+  <si>
+    <t>05.02.202420</t>
+  </si>
+  <si>
+    <t>05.02.202421</t>
+  </si>
+  <si>
+    <t>05.02.202422</t>
+  </si>
+  <si>
+    <t>05.02.202423</t>
+  </si>
+  <si>
+    <t>06.02.20240</t>
+  </si>
+  <si>
+    <t>06.02.20241</t>
+  </si>
+  <si>
+    <t>06.02.20242</t>
+  </si>
+  <si>
+    <t>06.02.20243</t>
+  </si>
+  <si>
+    <t>06.02.20244</t>
+  </si>
+  <si>
+    <t>06.02.20245</t>
+  </si>
+  <si>
+    <t>06.02.20246</t>
+  </si>
+  <si>
+    <t>06.02.20247</t>
+  </si>
+  <si>
+    <t>06.02.20248</t>
+  </si>
+  <si>
+    <t>06.02.20249</t>
+  </si>
+  <si>
+    <t>06.02.202410</t>
+  </si>
+  <si>
+    <t>06.02.202411</t>
+  </si>
+  <si>
+    <t>06.02.202412</t>
+  </si>
+  <si>
+    <t>06.02.202413</t>
+  </si>
+  <si>
+    <t>06.02.202414</t>
+  </si>
+  <si>
+    <t>06.02.202415</t>
+  </si>
+  <si>
+    <t>06.02.202416</t>
+  </si>
+  <si>
+    <t>06.02.202417</t>
+  </si>
+  <si>
+    <t>06.02.202418</t>
+  </si>
+  <si>
+    <t>06.02.202419</t>
+  </si>
+  <si>
+    <t>06.02.202420</t>
+  </si>
+  <si>
+    <t>06.02.202421</t>
+  </si>
+  <si>
+    <t>06.02.202422</t>
+  </si>
+  <si>
+    <t>06.02.202423</t>
+  </si>
+  <si>
+    <t>07.02.20240</t>
+  </si>
+  <si>
+    <t>07.02.20241</t>
+  </si>
+  <si>
+    <t>07.02.20242</t>
+  </si>
+  <si>
+    <t>07.02.20243</t>
+  </si>
+  <si>
+    <t>07.02.20244</t>
+  </si>
+  <si>
+    <t>07.02.20245</t>
+  </si>
+  <si>
+    <t>07.02.20246</t>
+  </si>
+  <si>
+    <t>07.02.20247</t>
+  </si>
+  <si>
+    <t>07.02.20248</t>
+  </si>
+  <si>
+    <t>07.02.20249</t>
+  </si>
+  <si>
+    <t>07.02.202410</t>
+  </si>
+  <si>
+    <t>07.02.202411</t>
+  </si>
+  <si>
+    <t>07.02.202412</t>
+  </si>
+  <si>
+    <t>07.02.202413</t>
+  </si>
+  <si>
+    <t>07.02.202414</t>
+  </si>
+  <si>
+    <t>07.02.202415</t>
+  </si>
+  <si>
+    <t>07.02.202416</t>
+  </si>
+  <si>
+    <t>07.02.202417</t>
+  </si>
+  <si>
+    <t>07.02.202418</t>
+  </si>
+  <si>
+    <t>07.02.202419</t>
+  </si>
+  <si>
+    <t>07.02.202420</t>
+  </si>
+  <si>
+    <t>07.02.202421</t>
+  </si>
+  <si>
+    <t>07.02.202422</t>
+  </si>
+  <si>
+    <t>07.02.202423</t>
+  </si>
+  <si>
+    <t>08.02.20240</t>
+  </si>
+  <si>
+    <t>08.02.20241</t>
+  </si>
+  <si>
+    <t>08.02.20242</t>
+  </si>
+  <si>
+    <t>08.02.20243</t>
+  </si>
+  <si>
+    <t>08.02.20244</t>
+  </si>
+  <si>
+    <t>08.02.20245</t>
+  </si>
+  <si>
+    <t>08.02.20246</t>
+  </si>
+  <si>
+    <t>08.02.20247</t>
+  </si>
+  <si>
+    <t>08.02.20248</t>
+  </si>
+  <si>
+    <t>08.02.20249</t>
+  </si>
+  <si>
+    <t>08.02.202410</t>
+  </si>
+  <si>
+    <t>08.02.202411</t>
+  </si>
+  <si>
+    <t>08.02.202412</t>
+  </si>
+  <si>
+    <t>08.02.202413</t>
+  </si>
+  <si>
+    <t>08.02.202414</t>
+  </si>
+  <si>
+    <t>08.02.202415</t>
+  </si>
+  <si>
+    <t>08.02.202416</t>
+  </si>
+  <si>
+    <t>08.02.202417</t>
+  </si>
+  <si>
+    <t>08.02.202418</t>
+  </si>
+  <si>
+    <t>08.02.202419</t>
+  </si>
+  <si>
+    <t>08.02.202420</t>
+  </si>
+  <si>
+    <t>08.02.202421</t>
+  </si>
+  <si>
+    <t>08.02.202422</t>
+  </si>
+  <si>
+    <t>08.02.202423</t>
+  </si>
+  <si>
+    <t>09.02.20240</t>
+  </si>
+  <si>
+    <t>09.02.20241</t>
+  </si>
+  <si>
+    <t>09.02.20242</t>
+  </si>
+  <si>
+    <t>09.02.20243</t>
+  </si>
+  <si>
+    <t>09.02.20244</t>
+  </si>
+  <si>
+    <t>09.02.20245</t>
+  </si>
+  <si>
+    <t>09.02.20246</t>
+  </si>
+  <si>
+    <t>09.02.20247</t>
+  </si>
+  <si>
+    <t>09.02.20248</t>
+  </si>
+  <si>
+    <t>09.02.20249</t>
+  </si>
+  <si>
+    <t>09.02.202410</t>
+  </si>
+  <si>
+    <t>09.02.202411</t>
+  </si>
+  <si>
+    <t>09.02.202412</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -327,21 +393,13 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -379,7 +437,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -413,7 +471,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -448,10 +505,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -624,20 +680,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F73"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F97"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S13" sqref="S13"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -657,98 +707,98 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" s="2">
-        <v>45323</v>
+        <v>45327</v>
       </c>
       <c r="B2">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C2">
-        <v>234</v>
+        <v>108.41</v>
       </c>
       <c r="D2">
-        <v>2.1800000000000002</v>
+        <v>8.76</v>
       </c>
       <c r="E2">
-        <v>32</v>
+        <v>100</v>
       </c>
       <c r="F2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" s="2">
-        <v>45323</v>
+        <v>45327</v>
       </c>
       <c r="B3">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C3">
-        <v>100.8</v>
+        <v>91.38</v>
       </c>
       <c r="D3">
-        <v>1.29</v>
+        <v>8.32</v>
       </c>
       <c r="E3">
-        <v>32</v>
+        <v>100</v>
       </c>
       <c r="F3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" s="2">
-        <v>45323</v>
+        <v>45327</v>
       </c>
       <c r="B4">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C4">
-        <v>6.07</v>
+        <v>63.85</v>
       </c>
       <c r="D4">
-        <v>0.69</v>
+        <v>7.79</v>
       </c>
       <c r="E4">
-        <v>39</v>
+        <v>100</v>
       </c>
       <c r="F4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" s="2">
-        <v>45323</v>
+        <v>45327</v>
       </c>
       <c r="B5">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>29.65</v>
       </c>
       <c r="D5">
-        <v>0.35</v>
+        <v>7.21</v>
       </c>
       <c r="E5">
-        <v>49</v>
+        <v>100</v>
       </c>
       <c r="F5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6" s="2">
-        <v>45323</v>
+        <v>45327</v>
       </c>
       <c r="B6">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>2.69</v>
       </c>
       <c r="D6">
-        <v>-0.2</v>
+        <v>6.66</v>
       </c>
       <c r="E6">
         <v>100</v>
@@ -757,18 +807,18 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6">
       <c r="A7" s="2">
-        <v>45323</v>
+        <v>45327</v>
       </c>
       <c r="B7">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C7">
         <v>0</v>
       </c>
       <c r="D7">
-        <v>-0.87</v>
+        <v>6.08</v>
       </c>
       <c r="E7">
         <v>100</v>
@@ -777,18 +827,18 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6">
       <c r="A8" s="2">
-        <v>45323</v>
+        <v>45327</v>
       </c>
       <c r="B8">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C8">
         <v>0</v>
       </c>
       <c r="D8">
-        <v>-0.21</v>
+        <v>5.84</v>
       </c>
       <c r="E8">
         <v>100</v>
@@ -797,18 +847,18 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6">
       <c r="A9" s="2">
-        <v>45323</v>
+        <v>45327</v>
       </c>
       <c r="B9">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C9">
         <v>0</v>
       </c>
       <c r="D9">
-        <v>-0.66</v>
+        <v>5.61</v>
       </c>
       <c r="E9">
         <v>100</v>
@@ -817,18 +867,18 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6">
       <c r="A10" s="2">
-        <v>45323</v>
+        <v>45327</v>
       </c>
       <c r="B10">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C10">
         <v>0</v>
       </c>
       <c r="D10">
-        <v>-1.29</v>
+        <v>5.3</v>
       </c>
       <c r="E10">
         <v>100</v>
@@ -837,18 +887,18 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6">
       <c r="A11" s="2">
-        <v>45324</v>
+        <v>45327</v>
       </c>
       <c r="B11">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="C11">
         <v>0</v>
       </c>
       <c r="D11">
-        <v>-1.36</v>
+        <v>5.05</v>
       </c>
       <c r="E11">
         <v>100</v>
@@ -857,18 +907,18 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6">
       <c r="A12" s="2">
-        <v>45324</v>
+        <v>45327</v>
       </c>
       <c r="B12">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="C12">
         <v>0</v>
       </c>
       <c r="D12">
-        <v>-1.36</v>
+        <v>5.01</v>
       </c>
       <c r="E12">
         <v>100</v>
@@ -877,18 +927,18 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6">
       <c r="A13" s="2">
-        <v>45324</v>
+        <v>45328</v>
       </c>
       <c r="B13">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C13">
         <v>0</v>
       </c>
       <c r="D13">
-        <v>-1.21</v>
+        <v>4.96</v>
       </c>
       <c r="E13">
         <v>100</v>
@@ -897,538 +947,538 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6">
       <c r="A14" s="2">
-        <v>45324</v>
+        <v>45328</v>
       </c>
       <c r="B14">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C14">
         <v>0</v>
       </c>
       <c r="D14">
-        <v>-0.7</v>
+        <v>4.62</v>
       </c>
       <c r="E14">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F14" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6">
       <c r="A15" s="2">
-        <v>45324</v>
+        <v>45328</v>
       </c>
       <c r="B15">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C15">
         <v>0</v>
       </c>
       <c r="D15">
-        <v>-0.63</v>
+        <v>4.27</v>
       </c>
       <c r="E15">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="F15" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6">
       <c r="A16" s="2">
-        <v>45324</v>
+        <v>45328</v>
       </c>
       <c r="B16">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C16">
         <v>0</v>
       </c>
       <c r="D16">
-        <v>-0.59</v>
+        <v>4.13</v>
       </c>
       <c r="E16">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="F16" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6">
       <c r="A17" s="2">
-        <v>45324</v>
+        <v>45328</v>
       </c>
       <c r="B17">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C17">
         <v>0</v>
       </c>
       <c r="D17">
-        <v>-0.76</v>
+        <v>4.03</v>
       </c>
       <c r="E17">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="F17" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6">
       <c r="A18" s="2">
-        <v>45324</v>
+        <v>45328</v>
       </c>
       <c r="B18">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C18">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="D18">
-        <v>-0.8</v>
+        <v>3.95</v>
       </c>
       <c r="E18">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="F18" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6">
       <c r="A19" s="2">
-        <v>45324</v>
+        <v>45328</v>
       </c>
       <c r="B19">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C19">
-        <v>18.23</v>
+        <v>0</v>
       </c>
       <c r="D19">
-        <v>-0.6</v>
+        <v>3.3</v>
       </c>
       <c r="E19">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="F19" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6">
       <c r="A20" s="2">
-        <v>45324</v>
+        <v>45328</v>
       </c>
       <c r="B20">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C20">
-        <v>51.87</v>
+        <v>0.62</v>
       </c>
       <c r="D20">
-        <v>0.56000000000000005</v>
+        <v>4.2</v>
       </c>
       <c r="E20">
-        <v>100</v>
+        <v>87</v>
       </c>
       <c r="F20" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6">
       <c r="A21" s="2">
-        <v>45324</v>
+        <v>45328</v>
       </c>
       <c r="B21">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C21">
-        <v>82.96</v>
+        <v>36.72</v>
       </c>
       <c r="D21">
-        <v>0.67</v>
+        <v>5.63</v>
       </c>
       <c r="E21">
-        <v>99</v>
+        <v>84</v>
       </c>
       <c r="F21" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6">
       <c r="A22" s="2">
-        <v>45324</v>
+        <v>45328</v>
       </c>
       <c r="B22">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C22">
-        <v>106.83</v>
+        <v>117.51</v>
       </c>
       <c r="D22">
-        <v>0.63</v>
+        <v>6.47</v>
       </c>
       <c r="E22">
-        <v>99</v>
+        <v>79</v>
       </c>
       <c r="F22" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6">
       <c r="A23" s="2">
-        <v>45324</v>
+        <v>45328</v>
       </c>
       <c r="B23">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C23">
-        <v>115.54</v>
+        <v>200.92</v>
       </c>
       <c r="D23">
-        <v>1.0900000000000001</v>
+        <v>7.45</v>
       </c>
       <c r="E23">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="F23" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6">
       <c r="A24" s="2">
-        <v>45324</v>
+        <v>45328</v>
       </c>
       <c r="B24">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C24">
-        <v>114.53</v>
+        <v>263.89</v>
       </c>
       <c r="D24">
-        <v>1.64</v>
+        <v>8.52</v>
       </c>
       <c r="E24">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="F24" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6">
       <c r="A25" s="2">
-        <v>45324</v>
+        <v>45328</v>
       </c>
       <c r="B25">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C25">
-        <v>119.05</v>
+        <v>277.56</v>
       </c>
       <c r="D25">
-        <v>1.69</v>
+        <v>8.800000000000001</v>
       </c>
       <c r="E25">
-        <v>94</v>
+        <v>81</v>
       </c>
       <c r="F25" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6">
       <c r="A26" s="2">
-        <v>45324</v>
+        <v>45328</v>
       </c>
       <c r="B26">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C26">
-        <v>95.68</v>
+        <v>264.77</v>
       </c>
       <c r="D26">
-        <v>0.04</v>
+        <v>8.98</v>
       </c>
       <c r="E26">
-        <v>93</v>
+        <v>73</v>
       </c>
       <c r="F26" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6">
       <c r="A27" s="2">
-        <v>45324</v>
+        <v>45328</v>
       </c>
       <c r="B27">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C27">
-        <v>37.15</v>
+        <v>234.29</v>
       </c>
       <c r="D27">
-        <v>-1.92</v>
+        <v>8.25</v>
       </c>
       <c r="E27">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F27" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6">
       <c r="A28" s="2">
-        <v>45324</v>
+        <v>45328</v>
       </c>
       <c r="B28">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C28">
-        <v>1.72</v>
+        <v>166.71</v>
       </c>
       <c r="D28">
-        <v>-2.35</v>
+        <v>7.3</v>
       </c>
       <c r="E28">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="F28" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6">
       <c r="A29" s="2">
-        <v>45324</v>
+        <v>45328</v>
       </c>
       <c r="B29">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C29">
-        <v>0</v>
+        <v>62.96</v>
       </c>
       <c r="D29">
-        <v>-2.37</v>
+        <v>6.3</v>
       </c>
       <c r="E29">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="F29" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6">
       <c r="A30" s="2">
-        <v>45324</v>
+        <v>45328</v>
       </c>
       <c r="B30">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C30">
-        <v>0</v>
+        <v>3.58</v>
       </c>
       <c r="D30">
-        <v>-2.65</v>
+        <v>6.16</v>
       </c>
       <c r="E30">
-        <v>52</v>
+        <v>90</v>
       </c>
       <c r="F30" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6">
       <c r="A31" s="2">
-        <v>45324</v>
+        <v>45328</v>
       </c>
       <c r="B31">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C31">
         <v>0</v>
       </c>
       <c r="D31">
-        <v>-2.78</v>
+        <v>6.12</v>
       </c>
       <c r="E31">
-        <v>50</v>
+        <v>91</v>
       </c>
       <c r="F31" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6">
       <c r="A32" s="2">
-        <v>45324</v>
+        <v>45328</v>
       </c>
       <c r="B32">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C32">
         <v>0</v>
       </c>
       <c r="D32">
-        <v>-2.4500000000000002</v>
+        <v>5.79</v>
       </c>
       <c r="E32">
-        <v>67</v>
+        <v>89</v>
       </c>
       <c r="F32" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6">
       <c r="A33" s="2">
-        <v>45324</v>
+        <v>45328</v>
       </c>
       <c r="B33">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C33">
         <v>0</v>
       </c>
       <c r="D33">
-        <v>-1.83</v>
+        <v>5.68</v>
       </c>
       <c r="E33">
-        <v>75</v>
+        <v>89</v>
       </c>
       <c r="F33" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6">
       <c r="A34" s="2">
-        <v>45324</v>
+        <v>45328</v>
       </c>
       <c r="B34">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C34">
         <v>0</v>
       </c>
       <c r="D34">
-        <v>-1.54</v>
+        <v>5.6</v>
       </c>
       <c r="E34">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="F34" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6">
       <c r="A35" s="2">
-        <v>45325</v>
+        <v>45328</v>
       </c>
       <c r="B35">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="C35">
         <v>0</v>
       </c>
       <c r="D35">
-        <v>-2.2400000000000002</v>
+        <v>5.62</v>
       </c>
       <c r="E35">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="F35" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6">
       <c r="A36" s="2">
-        <v>45325</v>
+        <v>45328</v>
       </c>
       <c r="B36">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="C36">
         <v>0</v>
       </c>
       <c r="D36">
-        <v>-2.25</v>
+        <v>5.75</v>
       </c>
       <c r="E36">
-        <v>100</v>
+        <v>87</v>
       </c>
       <c r="F36" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6">
       <c r="A37" s="2">
-        <v>45325</v>
+        <v>45329</v>
       </c>
       <c r="B37">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C37">
         <v>0</v>
       </c>
       <c r="D37">
-        <v>-2.1</v>
+        <v>5.66</v>
       </c>
       <c r="E37">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="F37" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6">
       <c r="A38" s="2">
-        <v>45325</v>
+        <v>45329</v>
       </c>
       <c r="B38">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C38">
         <v>0</v>
       </c>
       <c r="D38">
-        <v>-2.25</v>
+        <v>5.43</v>
       </c>
       <c r="E38">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="F38" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6">
       <c r="A39" s="2">
-        <v>45325</v>
+        <v>45329</v>
       </c>
       <c r="B39">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C39">
         <v>0</v>
       </c>
       <c r="D39">
-        <v>-0.67</v>
+        <v>5.15</v>
       </c>
       <c r="E39">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="F39" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6">
       <c r="A40" s="2">
-        <v>45325</v>
+        <v>45329</v>
       </c>
       <c r="B40">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C40">
         <v>0</v>
       </c>
       <c r="D40">
-        <v>-0.18</v>
+        <v>5.16</v>
       </c>
       <c r="E40">
         <v>96</v>
@@ -1437,18 +1487,18 @@
         <v>44</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6">
       <c r="A41" s="2">
-        <v>45325</v>
+        <v>45329</v>
       </c>
       <c r="B41">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C41">
         <v>0</v>
       </c>
       <c r="D41">
-        <v>-0.14000000000000001</v>
+        <v>4.98</v>
       </c>
       <c r="E41">
         <v>96</v>
@@ -1457,644 +1507,1085 @@
         <v>45</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6">
       <c r="A42" s="2">
-        <v>45325</v>
+        <v>45329</v>
       </c>
       <c r="B42">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C42">
-        <v>0.45</v>
+        <v>0</v>
       </c>
       <c r="D42">
-        <v>-0.37</v>
+        <v>4.6</v>
       </c>
       <c r="E42">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="F42" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6">
       <c r="A43" s="2">
-        <v>45325</v>
+        <v>45329</v>
       </c>
       <c r="B43">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C43">
-        <v>22.36</v>
+        <v>0</v>
       </c>
       <c r="D43">
-        <v>-0.04</v>
+        <v>4.65</v>
       </c>
       <c r="E43">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="F43" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6">
       <c r="A44" s="2">
-        <v>45325</v>
+        <v>45329</v>
       </c>
       <c r="B44">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C44">
-        <v>52.91</v>
+        <v>0.73</v>
       </c>
       <c r="D44">
-        <v>0.7</v>
+        <v>4.99</v>
       </c>
       <c r="E44">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="F44" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6">
       <c r="A45" s="2">
-        <v>45325</v>
+        <v>45329</v>
       </c>
       <c r="B45">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C45">
-        <v>82.6</v>
+        <v>26.79</v>
       </c>
       <c r="D45">
-        <v>1.28</v>
+        <v>5.39</v>
       </c>
       <c r="E45">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="F45" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6">
       <c r="A46" s="2">
-        <v>45325</v>
+        <v>45329</v>
       </c>
       <c r="B46">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C46">
-        <v>102.6</v>
+        <v>69.95</v>
       </c>
       <c r="D46">
-        <v>1.71</v>
+        <v>6.25</v>
       </c>
       <c r="E46">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="F46" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6">
       <c r="A47" s="2">
-        <v>45325</v>
+        <v>45329</v>
       </c>
       <c r="B47">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C47">
-        <v>110.31</v>
+        <v>115.28</v>
       </c>
       <c r="D47">
-        <v>2.2999999999999998</v>
+        <v>7.55</v>
       </c>
       <c r="E47">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="F47" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6">
       <c r="A48" s="2">
-        <v>45325</v>
+        <v>45329</v>
       </c>
       <c r="B48">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C48">
-        <v>104.9</v>
+        <v>143.85</v>
       </c>
       <c r="D48">
-        <v>2.31</v>
+        <v>8.83</v>
       </c>
       <c r="E48">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="F48" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6">
       <c r="A49" s="2">
-        <v>45325</v>
+        <v>45329</v>
       </c>
       <c r="B49">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C49">
-        <v>87.56</v>
+        <v>156.25</v>
       </c>
       <c r="D49">
-        <v>2.14</v>
+        <v>9.34</v>
       </c>
       <c r="E49">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="F49" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6">
       <c r="A50" s="2">
-        <v>45325</v>
+        <v>45329</v>
       </c>
       <c r="B50">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C50">
-        <v>60.17</v>
+        <v>143.72</v>
       </c>
       <c r="D50">
-        <v>1.81</v>
+        <v>9.369999999999999</v>
       </c>
       <c r="E50">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="F50" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6">
       <c r="A51" s="2">
-        <v>45325</v>
+        <v>45329</v>
       </c>
       <c r="B51">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C51">
-        <v>25.67</v>
+        <v>115.26</v>
       </c>
       <c r="D51">
-        <v>1.67</v>
+        <v>8.93</v>
       </c>
       <c r="E51">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="F51" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6">
       <c r="A52" s="2">
-        <v>45325</v>
+        <v>45329</v>
       </c>
       <c r="B52">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C52">
-        <v>1.27</v>
+        <v>84.06999999999999</v>
       </c>
       <c r="D52">
-        <v>1.61</v>
+        <v>8.1</v>
       </c>
       <c r="E52">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="F52" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6">
       <c r="A53" s="2">
-        <v>45325</v>
+        <v>45329</v>
       </c>
       <c r="B53">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C53">
-        <v>0</v>
+        <v>43.56</v>
       </c>
       <c r="D53">
-        <v>1.67</v>
+        <v>6.25</v>
       </c>
       <c r="E53">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="F53" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6">
       <c r="A54" s="2">
-        <v>45325</v>
+        <v>45329</v>
       </c>
       <c r="B54">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C54">
-        <v>0</v>
+        <v>3.16</v>
       </c>
       <c r="D54">
-        <v>1.8</v>
+        <v>5.31</v>
       </c>
       <c r="E54">
-        <v>98</v>
+        <v>71</v>
       </c>
       <c r="F54" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6">
       <c r="A55" s="2">
-        <v>45325</v>
+        <v>45329</v>
       </c>
       <c r="B55">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C55">
         <v>0</v>
       </c>
       <c r="D55">
-        <v>1.83</v>
+        <v>4.99</v>
       </c>
       <c r="E55">
-        <v>99</v>
+        <v>69</v>
       </c>
       <c r="F55" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6">
       <c r="A56" s="2">
-        <v>45325</v>
+        <v>45329</v>
       </c>
       <c r="B56">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C56">
         <v>0</v>
       </c>
       <c r="D56">
-        <v>2.1</v>
+        <v>4.86</v>
       </c>
       <c r="E56">
-        <v>99</v>
+        <v>63</v>
       </c>
       <c r="F56" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6">
       <c r="A57" s="2">
-        <v>45325</v>
+        <v>45329</v>
       </c>
       <c r="B57">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C57">
         <v>0</v>
       </c>
       <c r="D57">
-        <v>2.19</v>
+        <v>4.55</v>
       </c>
       <c r="E57">
-        <v>100</v>
+        <v>53</v>
       </c>
       <c r="F57" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6">
       <c r="A58" s="2">
-        <v>45325</v>
+        <v>45329</v>
       </c>
       <c r="B58">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C58">
         <v>0</v>
       </c>
       <c r="D58">
-        <v>2.4700000000000002</v>
+        <v>4.33</v>
       </c>
       <c r="E58">
-        <v>100</v>
+        <v>52</v>
       </c>
       <c r="F58" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6">
       <c r="A59" s="2">
-        <v>45326</v>
+        <v>45329</v>
       </c>
       <c r="B59">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="C59">
         <v>0</v>
       </c>
       <c r="D59">
-        <v>2.42</v>
+        <v>4.46</v>
       </c>
       <c r="E59">
-        <v>99</v>
+        <v>57</v>
       </c>
       <c r="F59" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6">
       <c r="A60" s="2">
-        <v>45326</v>
+        <v>45329</v>
       </c>
       <c r="B60">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="C60">
         <v>0</v>
       </c>
       <c r="D60">
-        <v>1.56</v>
+        <v>4.67</v>
       </c>
       <c r="E60">
-        <v>90</v>
+        <v>63</v>
       </c>
       <c r="F60" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6">
       <c r="A61" s="2">
-        <v>45326</v>
+        <v>45330</v>
       </c>
       <c r="B61">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C61">
         <v>0</v>
       </c>
       <c r="D61">
-        <v>2.2000000000000002</v>
+        <v>4.71</v>
       </c>
       <c r="E61">
-        <v>95</v>
+        <v>67</v>
       </c>
       <c r="F61" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6">
       <c r="A62" s="2">
-        <v>45326</v>
+        <v>45330</v>
       </c>
       <c r="B62">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C62">
         <v>0</v>
       </c>
       <c r="D62">
-        <v>2.81</v>
+        <v>4.66</v>
       </c>
       <c r="E62">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="F62" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6">
       <c r="A63" s="2">
-        <v>45326</v>
+        <v>45330</v>
       </c>
       <c r="B63">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C63">
         <v>0</v>
       </c>
       <c r="D63">
-        <v>2.92</v>
+        <v>4.66</v>
       </c>
       <c r="E63">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="F63" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6">
       <c r="A64" s="2">
-        <v>45326</v>
+        <v>45330</v>
       </c>
       <c r="B64">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C64">
         <v>0</v>
       </c>
       <c r="D64">
-        <v>3.08</v>
+        <v>4.83</v>
       </c>
       <c r="E64">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="F64" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6">
       <c r="A65" s="2">
-        <v>45326</v>
+        <v>45330</v>
       </c>
       <c r="B65">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C65">
         <v>0</v>
       </c>
       <c r="D65">
-        <v>3.24</v>
+        <v>4.85</v>
       </c>
       <c r="E65">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="F65" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6">
       <c r="A66" s="2">
-        <v>45326</v>
+        <v>45330</v>
       </c>
       <c r="B66">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C66">
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="D66">
-        <v>3.71</v>
+        <v>4.7</v>
       </c>
       <c r="E66">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="F66" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6">
       <c r="A67" s="2">
-        <v>45326</v>
+        <v>45330</v>
       </c>
       <c r="B67">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C67">
-        <v>18.05</v>
+        <v>0</v>
       </c>
       <c r="D67">
-        <v>4.47</v>
+        <v>4.69</v>
       </c>
       <c r="E67">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="F67" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6">
       <c r="A68" s="2">
-        <v>45326</v>
+        <v>45330</v>
       </c>
       <c r="B68">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C68">
-        <v>51.42</v>
+        <v>0.88</v>
       </c>
       <c r="D68">
-        <v>5.15</v>
+        <v>5.14</v>
       </c>
       <c r="E68">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="F68" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6">
       <c r="A69" s="2">
-        <v>45326</v>
+        <v>45330</v>
       </c>
       <c r="B69">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C69">
-        <v>81.81</v>
+        <v>30.6</v>
       </c>
       <c r="D69">
-        <v>5.96</v>
+        <v>5.8</v>
       </c>
       <c r="E69">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="F69" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6">
       <c r="A70" s="2">
-        <v>45326</v>
+        <v>45330</v>
       </c>
       <c r="B70">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C70">
-        <v>102.75</v>
+        <v>82.94</v>
       </c>
       <c r="D70">
-        <v>6.18</v>
+        <v>5.98</v>
       </c>
       <c r="E70">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="F70" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6">
       <c r="A71" s="2">
-        <v>45326</v>
+        <v>45330</v>
       </c>
       <c r="B71">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C71">
-        <v>111.49</v>
+        <v>122</v>
       </c>
       <c r="D71">
-        <v>5.95</v>
+        <v>6.34</v>
       </c>
       <c r="E71">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="F71" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6">
       <c r="A72" s="2">
-        <v>45326</v>
+        <v>45330</v>
       </c>
       <c r="B72">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C72">
-        <v>107.01</v>
+        <v>142.53</v>
       </c>
       <c r="D72">
-        <v>5.54</v>
+        <v>7.14</v>
       </c>
       <c r="E72">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="F72" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6">
       <c r="A73" s="2">
-        <v>45326</v>
+        <v>45330</v>
       </c>
       <c r="B73">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C73">
-        <v>89.84</v>
+        <v>146.14</v>
       </c>
       <c r="D73">
-        <v>5.03</v>
+        <v>7.8</v>
       </c>
       <c r="E73">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="F73" t="s">
         <v>77</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6">
+      <c r="A74" s="2">
+        <v>45330</v>
+      </c>
+      <c r="B74">
+        <v>13</v>
+      </c>
+      <c r="C74">
+        <v>133.21</v>
+      </c>
+      <c r="D74">
+        <v>7.57</v>
+      </c>
+      <c r="E74">
+        <v>100</v>
+      </c>
+      <c r="F74" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6">
+      <c r="A75" s="2">
+        <v>45330</v>
+      </c>
+      <c r="B75">
+        <v>14</v>
+      </c>
+      <c r="C75">
+        <v>101.71</v>
+      </c>
+      <c r="D75">
+        <v>7.61</v>
+      </c>
+      <c r="E75">
+        <v>99</v>
+      </c>
+      <c r="F75" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6">
+      <c r="A76" s="2">
+        <v>45330</v>
+      </c>
+      <c r="B76">
+        <v>15</v>
+      </c>
+      <c r="C76">
+        <v>62.05</v>
+      </c>
+      <c r="D76">
+        <v>7.26</v>
+      </c>
+      <c r="E76">
+        <v>100</v>
+      </c>
+      <c r="F76" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6">
+      <c r="A77" s="2">
+        <v>45330</v>
+      </c>
+      <c r="B77">
+        <v>16</v>
+      </c>
+      <c r="C77">
+        <v>28.56</v>
+      </c>
+      <c r="D77">
+        <v>6.84</v>
+      </c>
+      <c r="E77">
+        <v>100</v>
+      </c>
+      <c r="F77" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6">
+      <c r="A78" s="2">
+        <v>45330</v>
+      </c>
+      <c r="B78">
+        <v>17</v>
+      </c>
+      <c r="C78">
+        <v>2.15</v>
+      </c>
+      <c r="D78">
+        <v>6.58</v>
+      </c>
+      <c r="E78">
+        <v>100</v>
+      </c>
+      <c r="F78" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6">
+      <c r="A79" s="2">
+        <v>45330</v>
+      </c>
+      <c r="B79">
+        <v>18</v>
+      </c>
+      <c r="C79">
+        <v>0</v>
+      </c>
+      <c r="D79">
+        <v>6.21</v>
+      </c>
+      <c r="E79">
+        <v>100</v>
+      </c>
+      <c r="F79" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6">
+      <c r="A80" s="2">
+        <v>45330</v>
+      </c>
+      <c r="B80">
+        <v>19</v>
+      </c>
+      <c r="C80">
+        <v>0</v>
+      </c>
+      <c r="D80">
+        <v>6.08</v>
+      </c>
+      <c r="E80">
+        <v>100</v>
+      </c>
+      <c r="F80" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6">
+      <c r="A81" s="2">
+        <v>45330</v>
+      </c>
+      <c r="B81">
+        <v>20</v>
+      </c>
+      <c r="C81">
+        <v>0</v>
+      </c>
+      <c r="D81">
+        <v>6.08</v>
+      </c>
+      <c r="E81">
+        <v>100</v>
+      </c>
+      <c r="F81" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6">
+      <c r="A82" s="2">
+        <v>45330</v>
+      </c>
+      <c r="B82">
+        <v>21</v>
+      </c>
+      <c r="C82">
+        <v>0</v>
+      </c>
+      <c r="D82">
+        <v>6.03</v>
+      </c>
+      <c r="E82">
+        <v>100</v>
+      </c>
+      <c r="F82" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6">
+      <c r="A83" s="2">
+        <v>45330</v>
+      </c>
+      <c r="B83">
+        <v>22</v>
+      </c>
+      <c r="C83">
+        <v>0</v>
+      </c>
+      <c r="D83">
+        <v>5.98</v>
+      </c>
+      <c r="E83">
+        <v>100</v>
+      </c>
+      <c r="F83" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6">
+      <c r="A84" s="2">
+        <v>45330</v>
+      </c>
+      <c r="B84">
+        <v>23</v>
+      </c>
+      <c r="C84">
+        <v>0</v>
+      </c>
+      <c r="D84">
+        <v>5.94</v>
+      </c>
+      <c r="E84">
+        <v>100</v>
+      </c>
+      <c r="F84" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6">
+      <c r="A85" s="2">
+        <v>45331</v>
+      </c>
+      <c r="B85">
+        <v>0</v>
+      </c>
+      <c r="D85">
+        <v>5.86</v>
+      </c>
+      <c r="E85">
+        <v>100</v>
+      </c>
+      <c r="F85" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6">
+      <c r="A86" s="2">
+        <v>45331</v>
+      </c>
+      <c r="B86">
+        <v>1</v>
+      </c>
+      <c r="D86">
+        <v>5.71</v>
+      </c>
+      <c r="E86">
+        <v>100</v>
+      </c>
+      <c r="F86" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6">
+      <c r="A87" s="2">
+        <v>45331</v>
+      </c>
+      <c r="B87">
+        <v>2</v>
+      </c>
+      <c r="D87">
+        <v>5.7</v>
+      </c>
+      <c r="E87">
+        <v>100</v>
+      </c>
+      <c r="F87" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6">
+      <c r="A88" s="2">
+        <v>45331</v>
+      </c>
+      <c r="B88">
+        <v>3</v>
+      </c>
+      <c r="D88">
+        <v>5.4</v>
+      </c>
+      <c r="E88">
+        <v>99</v>
+      </c>
+      <c r="F88" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6">
+      <c r="A89" s="2">
+        <v>45331</v>
+      </c>
+      <c r="B89">
+        <v>4</v>
+      </c>
+      <c r="D89">
+        <v>5.5</v>
+      </c>
+      <c r="E89">
+        <v>99</v>
+      </c>
+      <c r="F89" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6">
+      <c r="A90" s="2">
+        <v>45331</v>
+      </c>
+      <c r="B90">
+        <v>5</v>
+      </c>
+      <c r="D90">
+        <v>5.19</v>
+      </c>
+      <c r="E90">
+        <v>99</v>
+      </c>
+      <c r="F90" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6">
+      <c r="A91" s="2">
+        <v>45331</v>
+      </c>
+      <c r="B91">
+        <v>6</v>
+      </c>
+      <c r="D91">
+        <v>5.66</v>
+      </c>
+      <c r="E91">
+        <v>99</v>
+      </c>
+      <c r="F91" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6">
+      <c r="A92" s="2">
+        <v>45331</v>
+      </c>
+      <c r="B92">
+        <v>7</v>
+      </c>
+      <c r="D92">
+        <v>6.24</v>
+      </c>
+      <c r="E92">
+        <v>100</v>
+      </c>
+      <c r="F92" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6">
+      <c r="A93" s="2">
+        <v>45331</v>
+      </c>
+      <c r="B93">
+        <v>8</v>
+      </c>
+      <c r="D93">
+        <v>7.01</v>
+      </c>
+      <c r="E93">
+        <v>100</v>
+      </c>
+      <c r="F93" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6">
+      <c r="A94" s="2">
+        <v>45331</v>
+      </c>
+      <c r="B94">
+        <v>9</v>
+      </c>
+      <c r="D94">
+        <v>7.6</v>
+      </c>
+      <c r="E94">
+        <v>100</v>
+      </c>
+      <c r="F94" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6">
+      <c r="A95" s="2">
+        <v>45331</v>
+      </c>
+      <c r="B95">
+        <v>10</v>
+      </c>
+      <c r="D95">
+        <v>8.01</v>
+      </c>
+      <c r="E95">
+        <v>100</v>
+      </c>
+      <c r="F95" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6">
+      <c r="A96" s="2">
+        <v>45331</v>
+      </c>
+      <c r="B96">
+        <v>11</v>
+      </c>
+      <c r="D96">
+        <v>8.33</v>
+      </c>
+      <c r="E96">
+        <v>100</v>
+      </c>
+      <c r="F96" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6">
+      <c r="A97" s="2">
+        <v>45331</v>
+      </c>
+      <c r="B97">
+        <v>12</v>
+      </c>
+      <c r="D97">
+        <v>7.99</v>
+      </c>
+      <c r="E97">
+        <v>100</v>
+      </c>
+      <c r="F97" t="s">
+        <v>101</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Setting up the Forecasting env for Solina and RAAL PVPPs
</commit_message>
<xml_diff>
--- a/RAAL/Production/Input.xlsx
+++ b/RAAL/Production/Input.xlsx
@@ -34,147 +34,6 @@
     <t>Lookup</t>
   </si>
   <si>
-    <t>05.02.202413</t>
-  </si>
-  <si>
-    <t>05.02.202414</t>
-  </si>
-  <si>
-    <t>05.02.202415</t>
-  </si>
-  <si>
-    <t>05.02.202416</t>
-  </si>
-  <si>
-    <t>05.02.202417</t>
-  </si>
-  <si>
-    <t>05.02.202418</t>
-  </si>
-  <si>
-    <t>05.02.202419</t>
-  </si>
-  <si>
-    <t>05.02.202420</t>
-  </si>
-  <si>
-    <t>05.02.202421</t>
-  </si>
-  <si>
-    <t>05.02.202422</t>
-  </si>
-  <si>
-    <t>05.02.202423</t>
-  </si>
-  <si>
-    <t>06.02.20240</t>
-  </si>
-  <si>
-    <t>06.02.20241</t>
-  </si>
-  <si>
-    <t>06.02.20242</t>
-  </si>
-  <si>
-    <t>06.02.20243</t>
-  </si>
-  <si>
-    <t>06.02.20244</t>
-  </si>
-  <si>
-    <t>06.02.20245</t>
-  </si>
-  <si>
-    <t>06.02.20246</t>
-  </si>
-  <si>
-    <t>06.02.20247</t>
-  </si>
-  <si>
-    <t>06.02.20248</t>
-  </si>
-  <si>
-    <t>06.02.20249</t>
-  </si>
-  <si>
-    <t>06.02.202410</t>
-  </si>
-  <si>
-    <t>06.02.202411</t>
-  </si>
-  <si>
-    <t>06.02.202412</t>
-  </si>
-  <si>
-    <t>06.02.202413</t>
-  </si>
-  <si>
-    <t>06.02.202414</t>
-  </si>
-  <si>
-    <t>06.02.202415</t>
-  </si>
-  <si>
-    <t>06.02.202416</t>
-  </si>
-  <si>
-    <t>06.02.202417</t>
-  </si>
-  <si>
-    <t>06.02.202418</t>
-  </si>
-  <si>
-    <t>06.02.202419</t>
-  </si>
-  <si>
-    <t>06.02.202420</t>
-  </si>
-  <si>
-    <t>06.02.202421</t>
-  </si>
-  <si>
-    <t>06.02.202422</t>
-  </si>
-  <si>
-    <t>06.02.202423</t>
-  </si>
-  <si>
-    <t>07.02.20240</t>
-  </si>
-  <si>
-    <t>07.02.20241</t>
-  </si>
-  <si>
-    <t>07.02.20242</t>
-  </si>
-  <si>
-    <t>07.02.20243</t>
-  </si>
-  <si>
-    <t>07.02.20244</t>
-  </si>
-  <si>
-    <t>07.02.20245</t>
-  </si>
-  <si>
-    <t>07.02.20246</t>
-  </si>
-  <si>
-    <t>07.02.20247</t>
-  </si>
-  <si>
-    <t>07.02.20248</t>
-  </si>
-  <si>
-    <t>07.02.20249</t>
-  </si>
-  <si>
-    <t>07.02.202410</t>
-  </si>
-  <si>
-    <t>07.02.202411</t>
-  </si>
-  <si>
     <t>07.02.202412</t>
   </si>
   <si>
@@ -320,6 +179,147 @@
   </si>
   <si>
     <t>09.02.202412</t>
+  </si>
+  <si>
+    <t>09.02.202413</t>
+  </si>
+  <si>
+    <t>09.02.202414</t>
+  </si>
+  <si>
+    <t>09.02.202415</t>
+  </si>
+  <si>
+    <t>09.02.202416</t>
+  </si>
+  <si>
+    <t>09.02.202417</t>
+  </si>
+  <si>
+    <t>09.02.202418</t>
+  </si>
+  <si>
+    <t>09.02.202419</t>
+  </si>
+  <si>
+    <t>09.02.202420</t>
+  </si>
+  <si>
+    <t>09.02.202421</t>
+  </si>
+  <si>
+    <t>09.02.202422</t>
+  </si>
+  <si>
+    <t>09.02.202423</t>
+  </si>
+  <si>
+    <t>10.02.20240</t>
+  </si>
+  <si>
+    <t>10.02.20241</t>
+  </si>
+  <si>
+    <t>10.02.20242</t>
+  </si>
+  <si>
+    <t>10.02.20243</t>
+  </si>
+  <si>
+    <t>10.02.20244</t>
+  </si>
+  <si>
+    <t>10.02.20245</t>
+  </si>
+  <si>
+    <t>10.02.20246</t>
+  </si>
+  <si>
+    <t>10.02.20247</t>
+  </si>
+  <si>
+    <t>10.02.20248</t>
+  </si>
+  <si>
+    <t>10.02.20249</t>
+  </si>
+  <si>
+    <t>10.02.202410</t>
+  </si>
+  <si>
+    <t>10.02.202411</t>
+  </si>
+  <si>
+    <t>10.02.202412</t>
+  </si>
+  <si>
+    <t>10.02.202413</t>
+  </si>
+  <si>
+    <t>10.02.202414</t>
+  </si>
+  <si>
+    <t>10.02.202415</t>
+  </si>
+  <si>
+    <t>10.02.202416</t>
+  </si>
+  <si>
+    <t>10.02.202417</t>
+  </si>
+  <si>
+    <t>10.02.202418</t>
+  </si>
+  <si>
+    <t>10.02.202419</t>
+  </si>
+  <si>
+    <t>10.02.202420</t>
+  </si>
+  <si>
+    <t>10.02.202421</t>
+  </si>
+  <si>
+    <t>10.02.202422</t>
+  </si>
+  <si>
+    <t>10.02.202423</t>
+  </si>
+  <si>
+    <t>11.02.20240</t>
+  </si>
+  <si>
+    <t>11.02.20241</t>
+  </si>
+  <si>
+    <t>11.02.20242</t>
+  </si>
+  <si>
+    <t>11.02.20243</t>
+  </si>
+  <si>
+    <t>11.02.20244</t>
+  </si>
+  <si>
+    <t>11.02.20245</t>
+  </si>
+  <si>
+    <t>11.02.20246</t>
+  </si>
+  <si>
+    <t>11.02.20247</t>
+  </si>
+  <si>
+    <t>11.02.20248</t>
+  </si>
+  <si>
+    <t>11.02.20249</t>
+  </si>
+  <si>
+    <t>11.02.202410</t>
+  </si>
+  <si>
+    <t>11.02.202411</t>
   </si>
 </sst>
 </file>
@@ -709,19 +709,19 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="2">
-        <v>45327</v>
+        <v>45329</v>
       </c>
       <c r="B2">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C2">
-        <v>108.41</v>
+        <v>121.03</v>
       </c>
       <c r="D2">
-        <v>8.76</v>
+        <v>8.34</v>
       </c>
       <c r="E2">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="F2" t="s">
         <v>6</v>
@@ -729,19 +729,19 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="2">
-        <v>45327</v>
+        <v>45329</v>
       </c>
       <c r="B3">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C3">
-        <v>91.38</v>
+        <v>125.65</v>
       </c>
       <c r="D3">
-        <v>8.32</v>
+        <v>8.4</v>
       </c>
       <c r="E3">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="F3" t="s">
         <v>7</v>
@@ -749,19 +749,19 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="2">
-        <v>45327</v>
+        <v>45329</v>
       </c>
       <c r="B4">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C4">
-        <v>63.85</v>
+        <v>143.96</v>
       </c>
       <c r="D4">
-        <v>7.79</v>
+        <v>8.48</v>
       </c>
       <c r="E4">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="F4" t="s">
         <v>8</v>
@@ -769,19 +769,19 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="2">
-        <v>45327</v>
+        <v>45329</v>
       </c>
       <c r="B5">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C5">
-        <v>29.65</v>
+        <v>132.55</v>
       </c>
       <c r="D5">
-        <v>7.21</v>
+        <v>7.87</v>
       </c>
       <c r="E5">
-        <v>100</v>
+        <v>82</v>
       </c>
       <c r="F5" t="s">
         <v>9</v>
@@ -789,19 +789,19 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="2">
-        <v>45327</v>
+        <v>45329</v>
       </c>
       <c r="B6">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C6">
-        <v>2.69</v>
+        <v>53.41</v>
       </c>
       <c r="D6">
-        <v>6.66</v>
+        <v>6.47</v>
       </c>
       <c r="E6">
-        <v>100</v>
+        <v>72</v>
       </c>
       <c r="F6" t="s">
         <v>10</v>
@@ -809,19 +809,19 @@
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="2">
-        <v>45327</v>
+        <v>45329</v>
       </c>
       <c r="B7">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>3.51</v>
       </c>
       <c r="D7">
-        <v>6.08</v>
+        <v>5.99</v>
       </c>
       <c r="E7">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="F7" t="s">
         <v>11</v>
@@ -829,19 +829,19 @@
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="2">
-        <v>45327</v>
+        <v>45329</v>
       </c>
       <c r="B8">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C8">
         <v>0</v>
       </c>
       <c r="D8">
-        <v>5.84</v>
+        <v>6.04</v>
       </c>
       <c r="E8">
-        <v>100</v>
+        <v>74</v>
       </c>
       <c r="F8" t="s">
         <v>12</v>
@@ -849,19 +849,19 @@
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="2">
-        <v>45327</v>
+        <v>45329</v>
       </c>
       <c r="B9">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C9">
         <v>0</v>
       </c>
       <c r="D9">
-        <v>5.61</v>
+        <v>5.86</v>
       </c>
       <c r="E9">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="F9" t="s">
         <v>13</v>
@@ -869,19 +869,19 @@
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="2">
-        <v>45327</v>
+        <v>45329</v>
       </c>
       <c r="B10">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C10">
         <v>0</v>
       </c>
       <c r="D10">
-        <v>5.3</v>
+        <v>5.7</v>
       </c>
       <c r="E10">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="F10" t="s">
         <v>14</v>
@@ -889,19 +889,19 @@
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="2">
-        <v>45327</v>
+        <v>45329</v>
       </c>
       <c r="B11">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C11">
         <v>0</v>
       </c>
       <c r="D11">
-        <v>5.05</v>
+        <v>5.56</v>
       </c>
       <c r="E11">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="F11" t="s">
         <v>15</v>
@@ -909,19 +909,19 @@
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="2">
-        <v>45327</v>
+        <v>45329</v>
       </c>
       <c r="B12">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C12">
         <v>0</v>
       </c>
       <c r="D12">
-        <v>5.01</v>
+        <v>5.5</v>
       </c>
       <c r="E12">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="F12" t="s">
         <v>16</v>
@@ -929,19 +929,19 @@
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="2">
-        <v>45328</v>
+        <v>45329</v>
       </c>
       <c r="B13">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="C13">
         <v>0</v>
       </c>
       <c r="D13">
-        <v>4.96</v>
+        <v>5.43</v>
       </c>
       <c r="E13">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="F13" t="s">
         <v>17</v>
@@ -949,19 +949,19 @@
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="2">
-        <v>45328</v>
+        <v>45330</v>
       </c>
       <c r="B14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C14">
         <v>0</v>
       </c>
       <c r="D14">
-        <v>4.62</v>
+        <v>5.54</v>
       </c>
       <c r="E14">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="F14" t="s">
         <v>18</v>
@@ -969,19 +969,19 @@
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="2">
-        <v>45328</v>
+        <v>45330</v>
       </c>
       <c r="B15">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C15">
         <v>0</v>
       </c>
       <c r="D15">
-        <v>4.27</v>
+        <v>5.46</v>
       </c>
       <c r="E15">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="F15" t="s">
         <v>19</v>
@@ -989,19 +989,19 @@
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="2">
-        <v>45328</v>
+        <v>45330</v>
       </c>
       <c r="B16">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C16">
         <v>0</v>
       </c>
       <c r="D16">
-        <v>4.13</v>
+        <v>5.42</v>
       </c>
       <c r="E16">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="F16" t="s">
         <v>20</v>
@@ -1009,19 +1009,19 @@
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="2">
-        <v>45328</v>
+        <v>45330</v>
       </c>
       <c r="B17">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C17">
         <v>0</v>
       </c>
       <c r="D17">
-        <v>4.03</v>
+        <v>5.36</v>
       </c>
       <c r="E17">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="F17" t="s">
         <v>21</v>
@@ -1029,19 +1029,19 @@
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="2">
-        <v>45328</v>
+        <v>45330</v>
       </c>
       <c r="B18">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C18">
         <v>0</v>
       </c>
       <c r="D18">
-        <v>3.95</v>
+        <v>5.41</v>
       </c>
       <c r="E18">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="F18" t="s">
         <v>22</v>
@@ -1049,19 +1049,19 @@
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="2">
-        <v>45328</v>
+        <v>45330</v>
       </c>
       <c r="B19">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C19">
         <v>0</v>
       </c>
       <c r="D19">
-        <v>3.3</v>
+        <v>5.31</v>
       </c>
       <c r="E19">
-        <v>93</v>
+        <v>100</v>
       </c>
       <c r="F19" t="s">
         <v>23</v>
@@ -1069,19 +1069,19 @@
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="2">
-        <v>45328</v>
+        <v>45330</v>
       </c>
       <c r="B20">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C20">
-        <v>0.62</v>
+        <v>0</v>
       </c>
       <c r="D20">
-        <v>4.2</v>
+        <v>5.19</v>
       </c>
       <c r="E20">
-        <v>87</v>
+        <v>100</v>
       </c>
       <c r="F20" t="s">
         <v>24</v>
@@ -1089,19 +1089,19 @@
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="2">
-        <v>45328</v>
+        <v>45330</v>
       </c>
       <c r="B21">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C21">
-        <v>36.72</v>
+        <v>0.64</v>
       </c>
       <c r="D21">
-        <v>5.63</v>
+        <v>5.23</v>
       </c>
       <c r="E21">
-        <v>84</v>
+        <v>100</v>
       </c>
       <c r="F21" t="s">
         <v>25</v>
@@ -1109,19 +1109,19 @@
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="2">
-        <v>45328</v>
+        <v>45330</v>
       </c>
       <c r="B22">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C22">
-        <v>117.51</v>
+        <v>21.31</v>
       </c>
       <c r="D22">
-        <v>6.47</v>
+        <v>5.38</v>
       </c>
       <c r="E22">
-        <v>79</v>
+        <v>100</v>
       </c>
       <c r="F22" t="s">
         <v>26</v>
@@ -1129,19 +1129,19 @@
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="2">
-        <v>45328</v>
+        <v>45330</v>
       </c>
       <c r="B23">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C23">
-        <v>200.92</v>
+        <v>55.31</v>
       </c>
       <c r="D23">
-        <v>7.45</v>
+        <v>5.75</v>
       </c>
       <c r="E23">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="F23" t="s">
         <v>27</v>
@@ -1149,19 +1149,19 @@
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="2">
-        <v>45328</v>
+        <v>45330</v>
       </c>
       <c r="B24">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C24">
-        <v>263.89</v>
+        <v>84.70999999999999</v>
       </c>
       <c r="D24">
-        <v>8.52</v>
+        <v>6.11</v>
       </c>
       <c r="E24">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="F24" t="s">
         <v>28</v>
@@ -1169,19 +1169,19 @@
     </row>
     <row r="25" spans="1:6">
       <c r="A25" s="2">
-        <v>45328</v>
+        <v>45330</v>
       </c>
       <c r="B25">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C25">
-        <v>277.56</v>
+        <v>104.57</v>
       </c>
       <c r="D25">
-        <v>8.800000000000001</v>
+        <v>6.56</v>
       </c>
       <c r="E25">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="F25" t="s">
         <v>29</v>
@@ -1189,19 +1189,19 @@
     </row>
     <row r="26" spans="1:6">
       <c r="A26" s="2">
-        <v>45328</v>
+        <v>45330</v>
       </c>
       <c r="B26">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C26">
-        <v>264.77</v>
+        <v>112.57</v>
       </c>
       <c r="D26">
-        <v>8.98</v>
+        <v>6.68</v>
       </c>
       <c r="E26">
-        <v>73</v>
+        <v>100</v>
       </c>
       <c r="F26" t="s">
         <v>30</v>
@@ -1209,19 +1209,19 @@
     </row>
     <row r="27" spans="1:6">
       <c r="A27" s="2">
-        <v>45328</v>
+        <v>45330</v>
       </c>
       <c r="B27">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C27">
-        <v>234.29</v>
+        <v>107.5</v>
       </c>
       <c r="D27">
-        <v>8.25</v>
+        <v>6.62</v>
       </c>
       <c r="E27">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="F27" t="s">
         <v>31</v>
@@ -1229,19 +1229,19 @@
     </row>
     <row r="28" spans="1:6">
       <c r="A28" s="2">
-        <v>45328</v>
+        <v>45330</v>
       </c>
       <c r="B28">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C28">
-        <v>166.71</v>
+        <v>89.31</v>
       </c>
       <c r="D28">
-        <v>7.3</v>
+        <v>6.25</v>
       </c>
       <c r="E28">
-        <v>84</v>
+        <v>100</v>
       </c>
       <c r="F28" t="s">
         <v>32</v>
@@ -1249,19 +1249,19 @@
     </row>
     <row r="29" spans="1:6">
       <c r="A29" s="2">
-        <v>45328</v>
+        <v>45330</v>
       </c>
       <c r="B29">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C29">
-        <v>62.96</v>
+        <v>60.92</v>
       </c>
       <c r="D29">
-        <v>6.3</v>
+        <v>6.22</v>
       </c>
       <c r="E29">
-        <v>87</v>
+        <v>100</v>
       </c>
       <c r="F29" t="s">
         <v>33</v>
@@ -1269,19 +1269,19 @@
     </row>
     <row r="30" spans="1:6">
       <c r="A30" s="2">
-        <v>45328</v>
+        <v>45330</v>
       </c>
       <c r="B30">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C30">
-        <v>3.58</v>
+        <v>27.2</v>
       </c>
       <c r="D30">
-        <v>6.16</v>
+        <v>6.2</v>
       </c>
       <c r="E30">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="F30" t="s">
         <v>34</v>
@@ -1289,19 +1289,19 @@
     </row>
     <row r="31" spans="1:6">
       <c r="A31" s="2">
-        <v>45328</v>
+        <v>45330</v>
       </c>
       <c r="B31">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C31">
-        <v>0</v>
+        <v>2.07</v>
       </c>
       <c r="D31">
-        <v>6.12</v>
+        <v>6.37</v>
       </c>
       <c r="E31">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="F31" t="s">
         <v>35</v>
@@ -1309,19 +1309,19 @@
     </row>
     <row r="32" spans="1:6">
       <c r="A32" s="2">
-        <v>45328</v>
+        <v>45330</v>
       </c>
       <c r="B32">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C32">
         <v>0</v>
       </c>
       <c r="D32">
-        <v>5.79</v>
+        <v>6.68</v>
       </c>
       <c r="E32">
-        <v>89</v>
+        <v>100</v>
       </c>
       <c r="F32" t="s">
         <v>36</v>
@@ -1329,19 +1329,19 @@
     </row>
     <row r="33" spans="1:6">
       <c r="A33" s="2">
-        <v>45328</v>
+        <v>45330</v>
       </c>
       <c r="B33">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C33">
         <v>0</v>
       </c>
       <c r="D33">
-        <v>5.68</v>
+        <v>6.39</v>
       </c>
       <c r="E33">
-        <v>89</v>
+        <v>100</v>
       </c>
       <c r="F33" t="s">
         <v>37</v>
@@ -1349,19 +1349,19 @@
     </row>
     <row r="34" spans="1:6">
       <c r="A34" s="2">
-        <v>45328</v>
+        <v>45330</v>
       </c>
       <c r="B34">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C34">
         <v>0</v>
       </c>
       <c r="D34">
-        <v>5.6</v>
+        <v>6.23</v>
       </c>
       <c r="E34">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="F34" t="s">
         <v>38</v>
@@ -1369,19 +1369,19 @@
     </row>
     <row r="35" spans="1:6">
       <c r="A35" s="2">
-        <v>45328</v>
+        <v>45330</v>
       </c>
       <c r="B35">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C35">
         <v>0</v>
       </c>
       <c r="D35">
-        <v>5.62</v>
+        <v>6.21</v>
       </c>
       <c r="E35">
-        <v>87</v>
+        <v>100</v>
       </c>
       <c r="F35" t="s">
         <v>39</v>
@@ -1389,19 +1389,19 @@
     </row>
     <row r="36" spans="1:6">
       <c r="A36" s="2">
-        <v>45328</v>
+        <v>45330</v>
       </c>
       <c r="B36">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C36">
         <v>0</v>
       </c>
       <c r="D36">
-        <v>5.75</v>
+        <v>6.21</v>
       </c>
       <c r="E36">
-        <v>87</v>
+        <v>100</v>
       </c>
       <c r="F36" t="s">
         <v>40</v>
@@ -1409,19 +1409,19 @@
     </row>
     <row r="37" spans="1:6">
       <c r="A37" s="2">
-        <v>45329</v>
+        <v>45330</v>
       </c>
       <c r="B37">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="C37">
         <v>0</v>
       </c>
       <c r="D37">
-        <v>5.66</v>
+        <v>6.06</v>
       </c>
       <c r="E37">
-        <v>89</v>
+        <v>100</v>
       </c>
       <c r="F37" t="s">
         <v>41</v>
@@ -1429,19 +1429,19 @@
     </row>
     <row r="38" spans="1:6">
       <c r="A38" s="2">
-        <v>45329</v>
+        <v>45331</v>
       </c>
       <c r="B38">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C38">
         <v>0</v>
       </c>
       <c r="D38">
-        <v>5.43</v>
+        <v>6.01</v>
       </c>
       <c r="E38">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="F38" t="s">
         <v>42</v>
@@ -1449,19 +1449,19 @@
     </row>
     <row r="39" spans="1:6">
       <c r="A39" s="2">
-        <v>45329</v>
+        <v>45331</v>
       </c>
       <c r="B39">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C39">
         <v>0</v>
       </c>
       <c r="D39">
-        <v>5.15</v>
+        <v>5.93</v>
       </c>
       <c r="E39">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="F39" t="s">
         <v>43</v>
@@ -1469,19 +1469,19 @@
     </row>
     <row r="40" spans="1:6">
       <c r="A40" s="2">
-        <v>45329</v>
+        <v>45331</v>
       </c>
       <c r="B40">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C40">
         <v>0</v>
       </c>
       <c r="D40">
-        <v>5.16</v>
+        <v>5.91</v>
       </c>
       <c r="E40">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="F40" t="s">
         <v>44</v>
@@ -1489,19 +1489,19 @@
     </row>
     <row r="41" spans="1:6">
       <c r="A41" s="2">
-        <v>45329</v>
+        <v>45331</v>
       </c>
       <c r="B41">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C41">
         <v>0</v>
       </c>
       <c r="D41">
-        <v>4.98</v>
+        <v>5.97</v>
       </c>
       <c r="E41">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="F41" t="s">
         <v>45</v>
@@ -1509,19 +1509,19 @@
     </row>
     <row r="42" spans="1:6">
       <c r="A42" s="2">
-        <v>45329</v>
+        <v>45331</v>
       </c>
       <c r="B42">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C42">
         <v>0</v>
       </c>
       <c r="D42">
-        <v>4.6</v>
+        <v>5.63</v>
       </c>
       <c r="E42">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="F42" t="s">
         <v>46</v>
@@ -1529,19 +1529,19 @@
     </row>
     <row r="43" spans="1:6">
       <c r="A43" s="2">
-        <v>45329</v>
+        <v>45331</v>
       </c>
       <c r="B43">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C43">
         <v>0</v>
       </c>
       <c r="D43">
-        <v>4.65</v>
+        <v>5.97</v>
       </c>
       <c r="E43">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="F43" t="s">
         <v>47</v>
@@ -1549,19 +1549,19 @@
     </row>
     <row r="44" spans="1:6">
       <c r="A44" s="2">
-        <v>45329</v>
+        <v>45331</v>
       </c>
       <c r="B44">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C44">
-        <v>0.73</v>
+        <v>0</v>
       </c>
       <c r="D44">
-        <v>4.99</v>
+        <v>6.03</v>
       </c>
       <c r="E44">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="F44" t="s">
         <v>48</v>
@@ -1569,19 +1569,19 @@
     </row>
     <row r="45" spans="1:6">
       <c r="A45" s="2">
-        <v>45329</v>
+        <v>45331</v>
       </c>
       <c r="B45">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C45">
-        <v>26.79</v>
+        <v>0.82</v>
       </c>
       <c r="D45">
-        <v>5.39</v>
+        <v>6.24</v>
       </c>
       <c r="E45">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="F45" t="s">
         <v>49</v>
@@ -1589,19 +1589,19 @@
     </row>
     <row r="46" spans="1:6">
       <c r="A46" s="2">
-        <v>45329</v>
+        <v>45331</v>
       </c>
       <c r="B46">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C46">
-        <v>69.95</v>
+        <v>22.82</v>
       </c>
       <c r="D46">
-        <v>6.25</v>
+        <v>6.26</v>
       </c>
       <c r="E46">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="F46" t="s">
         <v>50</v>
@@ -1609,19 +1609,19 @@
     </row>
     <row r="47" spans="1:6">
       <c r="A47" s="2">
-        <v>45329</v>
+        <v>45331</v>
       </c>
       <c r="B47">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C47">
-        <v>115.28</v>
+        <v>56.17</v>
       </c>
       <c r="D47">
-        <v>7.55</v>
+        <v>6.33</v>
       </c>
       <c r="E47">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="F47" t="s">
         <v>51</v>
@@ -1629,19 +1629,19 @@
     </row>
     <row r="48" spans="1:6">
       <c r="A48" s="2">
-        <v>45329</v>
+        <v>45331</v>
       </c>
       <c r="B48">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C48">
-        <v>143.85</v>
+        <v>85.78</v>
       </c>
       <c r="D48">
-        <v>8.83</v>
+        <v>6.64</v>
       </c>
       <c r="E48">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="F48" t="s">
         <v>52</v>
@@ -1649,19 +1649,19 @@
     </row>
     <row r="49" spans="1:6">
       <c r="A49" s="2">
-        <v>45329</v>
+        <v>45331</v>
       </c>
       <c r="B49">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C49">
-        <v>156.25</v>
+        <v>105.74</v>
       </c>
       <c r="D49">
-        <v>9.34</v>
+        <v>6.8</v>
       </c>
       <c r="E49">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="F49" t="s">
         <v>53</v>
@@ -1669,19 +1669,19 @@
     </row>
     <row r="50" spans="1:6">
       <c r="A50" s="2">
-        <v>45329</v>
+        <v>45331</v>
       </c>
       <c r="B50">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C50">
-        <v>143.72</v>
+        <v>113.45</v>
       </c>
       <c r="D50">
-        <v>9.369999999999999</v>
+        <v>6.6</v>
       </c>
       <c r="E50">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="F50" t="s">
         <v>54</v>
@@ -1689,19 +1689,19 @@
     </row>
     <row r="51" spans="1:6">
       <c r="A51" s="2">
-        <v>45329</v>
+        <v>45331</v>
       </c>
       <c r="B51">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C51">
-        <v>115.26</v>
+        <v>108.1</v>
       </c>
       <c r="D51">
-        <v>8.93</v>
+        <v>6.48</v>
       </c>
       <c r="E51">
-        <v>93</v>
+        <v>100</v>
       </c>
       <c r="F51" t="s">
         <v>55</v>
@@ -1709,19 +1709,19 @@
     </row>
     <row r="52" spans="1:6">
       <c r="A52" s="2">
-        <v>45329</v>
+        <v>45331</v>
       </c>
       <c r="B52">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C52">
-        <v>84.06999999999999</v>
+        <v>90.28</v>
       </c>
       <c r="D52">
-        <v>8.1</v>
+        <v>6.46</v>
       </c>
       <c r="E52">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="F52" t="s">
         <v>56</v>
@@ -1729,19 +1729,19 @@
     </row>
     <row r="53" spans="1:6">
       <c r="A53" s="2">
-        <v>45329</v>
+        <v>45331</v>
       </c>
       <c r="B53">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C53">
-        <v>43.56</v>
+        <v>62.2</v>
       </c>
       <c r="D53">
-        <v>6.25</v>
+        <v>6.28</v>
       </c>
       <c r="E53">
-        <v>84</v>
+        <v>100</v>
       </c>
       <c r="F53" t="s">
         <v>57</v>
@@ -1749,19 +1749,19 @@
     </row>
     <row r="54" spans="1:6">
       <c r="A54" s="2">
-        <v>45329</v>
+        <v>45331</v>
       </c>
       <c r="B54">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C54">
-        <v>3.16</v>
+        <v>28.26</v>
       </c>
       <c r="D54">
-        <v>5.31</v>
+        <v>6.37</v>
       </c>
       <c r="E54">
-        <v>71</v>
+        <v>100</v>
       </c>
       <c r="F54" t="s">
         <v>58</v>
@@ -1769,19 +1769,19 @@
     </row>
     <row r="55" spans="1:6">
       <c r="A55" s="2">
-        <v>45329</v>
+        <v>45331</v>
       </c>
       <c r="B55">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C55">
-        <v>0</v>
+        <v>2.38</v>
       </c>
       <c r="D55">
-        <v>4.99</v>
+        <v>6.7</v>
       </c>
       <c r="E55">
-        <v>69</v>
+        <v>100</v>
       </c>
       <c r="F55" t="s">
         <v>59</v>
@@ -1789,19 +1789,19 @@
     </row>
     <row r="56" spans="1:6">
       <c r="A56" s="2">
-        <v>45329</v>
+        <v>45331</v>
       </c>
       <c r="B56">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C56">
         <v>0</v>
       </c>
       <c r="D56">
-        <v>4.86</v>
+        <v>6.64</v>
       </c>
       <c r="E56">
-        <v>63</v>
+        <v>100</v>
       </c>
       <c r="F56" t="s">
         <v>60</v>
@@ -1809,19 +1809,19 @@
     </row>
     <row r="57" spans="1:6">
       <c r="A57" s="2">
-        <v>45329</v>
+        <v>45331</v>
       </c>
       <c r="B57">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C57">
         <v>0</v>
       </c>
       <c r="D57">
-        <v>4.55</v>
+        <v>6.68</v>
       </c>
       <c r="E57">
-        <v>53</v>
+        <v>100</v>
       </c>
       <c r="F57" t="s">
         <v>61</v>
@@ -1829,19 +1829,19 @@
     </row>
     <row r="58" spans="1:6">
       <c r="A58" s="2">
-        <v>45329</v>
+        <v>45331</v>
       </c>
       <c r="B58">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C58">
         <v>0</v>
       </c>
       <c r="D58">
-        <v>4.33</v>
+        <v>6.74</v>
       </c>
       <c r="E58">
-        <v>52</v>
+        <v>100</v>
       </c>
       <c r="F58" t="s">
         <v>62</v>
@@ -1849,19 +1849,19 @@
     </row>
     <row r="59" spans="1:6">
       <c r="A59" s="2">
-        <v>45329</v>
+        <v>45331</v>
       </c>
       <c r="B59">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C59">
         <v>0</v>
       </c>
       <c r="D59">
-        <v>4.46</v>
+        <v>6.65</v>
       </c>
       <c r="E59">
-        <v>57</v>
+        <v>100</v>
       </c>
       <c r="F59" t="s">
         <v>63</v>
@@ -1869,19 +1869,19 @@
     </row>
     <row r="60" spans="1:6">
       <c r="A60" s="2">
-        <v>45329</v>
+        <v>45331</v>
       </c>
       <c r="B60">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C60">
         <v>0</v>
       </c>
       <c r="D60">
-        <v>4.67</v>
+        <v>6.58</v>
       </c>
       <c r="E60">
-        <v>63</v>
+        <v>100</v>
       </c>
       <c r="F60" t="s">
         <v>64</v>
@@ -1889,19 +1889,19 @@
     </row>
     <row r="61" spans="1:6">
       <c r="A61" s="2">
-        <v>45330</v>
+        <v>45331</v>
       </c>
       <c r="B61">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="C61">
         <v>0</v>
       </c>
       <c r="D61">
-        <v>4.71</v>
+        <v>6.52</v>
       </c>
       <c r="E61">
-        <v>67</v>
+        <v>100</v>
       </c>
       <c r="F61" t="s">
         <v>65</v>
@@ -1909,19 +1909,19 @@
     </row>
     <row r="62" spans="1:6">
       <c r="A62" s="2">
-        <v>45330</v>
+        <v>45332</v>
       </c>
       <c r="B62">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C62">
         <v>0</v>
       </c>
       <c r="D62">
-        <v>4.66</v>
+        <v>6.39</v>
       </c>
       <c r="E62">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="F62" t="s">
         <v>66</v>
@@ -1929,19 +1929,19 @@
     </row>
     <row r="63" spans="1:6">
       <c r="A63" s="2">
-        <v>45330</v>
+        <v>45332</v>
       </c>
       <c r="B63">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C63">
         <v>0</v>
       </c>
       <c r="D63">
-        <v>4.66</v>
+        <v>6.45</v>
       </c>
       <c r="E63">
-        <v>93</v>
+        <v>100</v>
       </c>
       <c r="F63" t="s">
         <v>67</v>
@@ -1949,19 +1949,19 @@
     </row>
     <row r="64" spans="1:6">
       <c r="A64" s="2">
-        <v>45330</v>
+        <v>45332</v>
       </c>
       <c r="B64">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C64">
         <v>0</v>
       </c>
       <c r="D64">
-        <v>4.83</v>
+        <v>6.59</v>
       </c>
       <c r="E64">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="F64" t="s">
         <v>68</v>
@@ -1969,19 +1969,19 @@
     </row>
     <row r="65" spans="1:6">
       <c r="A65" s="2">
-        <v>45330</v>
+        <v>45332</v>
       </c>
       <c r="B65">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C65">
         <v>0</v>
       </c>
       <c r="D65">
-        <v>4.85</v>
+        <v>6.82</v>
       </c>
       <c r="E65">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="F65" t="s">
         <v>69</v>
@@ -1989,19 +1989,19 @@
     </row>
     <row r="66" spans="1:6">
       <c r="A66" s="2">
-        <v>45330</v>
+        <v>45332</v>
       </c>
       <c r="B66">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C66">
         <v>0</v>
       </c>
       <c r="D66">
-        <v>4.7</v>
+        <v>7</v>
       </c>
       <c r="E66">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="F66" t="s">
         <v>70</v>
@@ -2009,19 +2009,19 @@
     </row>
     <row r="67" spans="1:6">
       <c r="A67" s="2">
-        <v>45330</v>
+        <v>45332</v>
       </c>
       <c r="B67">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C67">
         <v>0</v>
       </c>
       <c r="D67">
-        <v>4.69</v>
+        <v>6.93</v>
       </c>
       <c r="E67">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="F67" t="s">
         <v>71</v>
@@ -2029,19 +2029,19 @@
     </row>
     <row r="68" spans="1:6">
       <c r="A68" s="2">
-        <v>45330</v>
+        <v>45332</v>
       </c>
       <c r="B68">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C68">
-        <v>0.88</v>
+        <v>0</v>
       </c>
       <c r="D68">
-        <v>5.14</v>
+        <v>6.82</v>
       </c>
       <c r="E68">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="F68" t="s">
         <v>72</v>
@@ -2049,19 +2049,19 @@
     </row>
     <row r="69" spans="1:6">
       <c r="A69" s="2">
-        <v>45330</v>
+        <v>45332</v>
       </c>
       <c r="B69">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C69">
-        <v>30.6</v>
+        <v>0.91</v>
       </c>
       <c r="D69">
-        <v>5.8</v>
+        <v>6.95</v>
       </c>
       <c r="E69">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="F69" t="s">
         <v>73</v>
@@ -2069,19 +2069,19 @@
     </row>
     <row r="70" spans="1:6">
       <c r="A70" s="2">
-        <v>45330</v>
+        <v>45332</v>
       </c>
       <c r="B70">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C70">
-        <v>82.94</v>
+        <v>22.97</v>
       </c>
       <c r="D70">
-        <v>5.98</v>
+        <v>7.13</v>
       </c>
       <c r="E70">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="F70" t="s">
         <v>74</v>
@@ -2089,19 +2089,19 @@
     </row>
     <row r="71" spans="1:6">
       <c r="A71" s="2">
-        <v>45330</v>
+        <v>45332</v>
       </c>
       <c r="B71">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C71">
-        <v>122</v>
+        <v>57.38</v>
       </c>
       <c r="D71">
-        <v>6.34</v>
+        <v>7.37</v>
       </c>
       <c r="E71">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="F71" t="s">
         <v>75</v>
@@ -2109,19 +2109,19 @@
     </row>
     <row r="72" spans="1:6">
       <c r="A72" s="2">
-        <v>45330</v>
+        <v>45332</v>
       </c>
       <c r="B72">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C72">
-        <v>142.53</v>
+        <v>87.08</v>
       </c>
       <c r="D72">
-        <v>7.14</v>
+        <v>7.45</v>
       </c>
       <c r="E72">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="F72" t="s">
         <v>76</v>
@@ -2129,19 +2129,19 @@
     </row>
     <row r="73" spans="1:6">
       <c r="A73" s="2">
-        <v>45330</v>
+        <v>45332</v>
       </c>
       <c r="B73">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C73">
-        <v>146.14</v>
+        <v>107.06</v>
       </c>
       <c r="D73">
-        <v>7.8</v>
+        <v>7.49</v>
       </c>
       <c r="E73">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="F73" t="s">
         <v>77</v>
@@ -2149,16 +2149,16 @@
     </row>
     <row r="74" spans="1:6">
       <c r="A74" s="2">
-        <v>45330</v>
+        <v>45332</v>
       </c>
       <c r="B74">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C74">
-        <v>133.21</v>
+        <v>114.81</v>
       </c>
       <c r="D74">
-        <v>7.57</v>
+        <v>8.02</v>
       </c>
       <c r="E74">
         <v>100</v>
@@ -2169,19 +2169,19 @@
     </row>
     <row r="75" spans="1:6">
       <c r="A75" s="2">
-        <v>45330</v>
+        <v>45332</v>
       </c>
       <c r="B75">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C75">
-        <v>101.71</v>
+        <v>109.46</v>
       </c>
       <c r="D75">
-        <v>7.61</v>
+        <v>7.93</v>
       </c>
       <c r="E75">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="F75" t="s">
         <v>79</v>
@@ -2189,16 +2189,16 @@
     </row>
     <row r="76" spans="1:6">
       <c r="A76" s="2">
-        <v>45330</v>
+        <v>45332</v>
       </c>
       <c r="B76">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C76">
-        <v>62.05</v>
+        <v>91.62</v>
       </c>
       <c r="D76">
-        <v>7.26</v>
+        <v>7.77</v>
       </c>
       <c r="E76">
         <v>100</v>
@@ -2209,16 +2209,16 @@
     </row>
     <row r="77" spans="1:6">
       <c r="A77" s="2">
-        <v>45330</v>
+        <v>45332</v>
       </c>
       <c r="B77">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C77">
-        <v>28.56</v>
+        <v>63.46</v>
       </c>
       <c r="D77">
-        <v>6.84</v>
+        <v>7.77</v>
       </c>
       <c r="E77">
         <v>100</v>
@@ -2229,16 +2229,16 @@
     </row>
     <row r="78" spans="1:6">
       <c r="A78" s="2">
-        <v>45330</v>
+        <v>45332</v>
       </c>
       <c r="B78">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C78">
-        <v>2.15</v>
+        <v>29.32</v>
       </c>
       <c r="D78">
-        <v>6.58</v>
+        <v>7.55</v>
       </c>
       <c r="E78">
         <v>100</v>
@@ -2249,16 +2249,16 @@
     </row>
     <row r="79" spans="1:6">
       <c r="A79" s="2">
-        <v>45330</v>
+        <v>45332</v>
       </c>
       <c r="B79">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C79">
-        <v>0</v>
+        <v>2.71</v>
       </c>
       <c r="D79">
-        <v>6.21</v>
+        <v>7.52</v>
       </c>
       <c r="E79">
         <v>100</v>
@@ -2269,16 +2269,16 @@
     </row>
     <row r="80" spans="1:6">
       <c r="A80" s="2">
-        <v>45330</v>
+        <v>45332</v>
       </c>
       <c r="B80">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C80">
         <v>0</v>
       </c>
       <c r="D80">
-        <v>6.08</v>
+        <v>7.55</v>
       </c>
       <c r="E80">
         <v>100</v>
@@ -2289,16 +2289,16 @@
     </row>
     <row r="81" spans="1:6">
       <c r="A81" s="2">
-        <v>45330</v>
+        <v>45332</v>
       </c>
       <c r="B81">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C81">
         <v>0</v>
       </c>
       <c r="D81">
-        <v>6.08</v>
+        <v>7.64</v>
       </c>
       <c r="E81">
         <v>100</v>
@@ -2309,16 +2309,16 @@
     </row>
     <row r="82" spans="1:6">
       <c r="A82" s="2">
-        <v>45330</v>
+        <v>45332</v>
       </c>
       <c r="B82">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C82">
         <v>0</v>
       </c>
       <c r="D82">
-        <v>6.03</v>
+        <v>7.78</v>
       </c>
       <c r="E82">
         <v>100</v>
@@ -2329,16 +2329,16 @@
     </row>
     <row r="83" spans="1:6">
       <c r="A83" s="2">
-        <v>45330</v>
+        <v>45332</v>
       </c>
       <c r="B83">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C83">
         <v>0</v>
       </c>
       <c r="D83">
-        <v>5.98</v>
+        <v>7.93</v>
       </c>
       <c r="E83">
         <v>100</v>
@@ -2349,16 +2349,16 @@
     </row>
     <row r="84" spans="1:6">
       <c r="A84" s="2">
-        <v>45330</v>
+        <v>45332</v>
       </c>
       <c r="B84">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C84">
         <v>0</v>
       </c>
       <c r="D84">
-        <v>5.94</v>
+        <v>7.2</v>
       </c>
       <c r="E84">
         <v>100</v>
@@ -2369,13 +2369,16 @@
     </row>
     <row r="85" spans="1:6">
       <c r="A85" s="2">
-        <v>45331</v>
+        <v>45332</v>
       </c>
       <c r="B85">
+        <v>23</v>
+      </c>
+      <c r="C85">
         <v>0</v>
       </c>
       <c r="D85">
-        <v>5.86</v>
+        <v>7.38</v>
       </c>
       <c r="E85">
         <v>100</v>
@@ -2386,13 +2389,13 @@
     </row>
     <row r="86" spans="1:6">
       <c r="A86" s="2">
-        <v>45331</v>
+        <v>45333</v>
       </c>
       <c r="B86">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D86">
-        <v>5.71</v>
+        <v>7.6</v>
       </c>
       <c r="E86">
         <v>100</v>
@@ -2403,13 +2406,13 @@
     </row>
     <row r="87" spans="1:6">
       <c r="A87" s="2">
-        <v>45331</v>
+        <v>45333</v>
       </c>
       <c r="B87">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D87">
-        <v>5.7</v>
+        <v>7.66</v>
       </c>
       <c r="E87">
         <v>100</v>
@@ -2420,16 +2423,16 @@
     </row>
     <row r="88" spans="1:6">
       <c r="A88" s="2">
-        <v>45331</v>
+        <v>45333</v>
       </c>
       <c r="B88">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D88">
-        <v>5.4</v>
+        <v>7.45</v>
       </c>
       <c r="E88">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="F88" t="s">
         <v>92</v>
@@ -2437,16 +2440,16 @@
     </row>
     <row r="89" spans="1:6">
       <c r="A89" s="2">
-        <v>45331</v>
+        <v>45333</v>
       </c>
       <c r="B89">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D89">
-        <v>5.5</v>
+        <v>7.53</v>
       </c>
       <c r="E89">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="F89" t="s">
         <v>93</v>
@@ -2454,16 +2457,16 @@
     </row>
     <row r="90" spans="1:6">
       <c r="A90" s="2">
-        <v>45331</v>
+        <v>45333</v>
       </c>
       <c r="B90">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D90">
-        <v>5.19</v>
+        <v>7.68</v>
       </c>
       <c r="E90">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="F90" t="s">
         <v>94</v>
@@ -2471,16 +2474,16 @@
     </row>
     <row r="91" spans="1:6">
       <c r="A91" s="2">
-        <v>45331</v>
+        <v>45333</v>
       </c>
       <c r="B91">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D91">
-        <v>5.66</v>
+        <v>7.17</v>
       </c>
       <c r="E91">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="F91" t="s">
         <v>95</v>
@@ -2488,13 +2491,13 @@
     </row>
     <row r="92" spans="1:6">
       <c r="A92" s="2">
-        <v>45331</v>
+        <v>45333</v>
       </c>
       <c r="B92">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D92">
-        <v>6.24</v>
+        <v>7.55</v>
       </c>
       <c r="E92">
         <v>100</v>
@@ -2505,13 +2508,13 @@
     </row>
     <row r="93" spans="1:6">
       <c r="A93" s="2">
-        <v>45331</v>
+        <v>45333</v>
       </c>
       <c r="B93">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D93">
-        <v>7.01</v>
+        <v>8.460000000000001</v>
       </c>
       <c r="E93">
         <v>100</v>
@@ -2522,13 +2525,13 @@
     </row>
     <row r="94" spans="1:6">
       <c r="A94" s="2">
-        <v>45331</v>
+        <v>45333</v>
       </c>
       <c r="B94">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D94">
-        <v>7.6</v>
+        <v>9.94</v>
       </c>
       <c r="E94">
         <v>100</v>
@@ -2539,13 +2542,13 @@
     </row>
     <row r="95" spans="1:6">
       <c r="A95" s="2">
-        <v>45331</v>
+        <v>45333</v>
       </c>
       <c r="B95">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D95">
-        <v>8.01</v>
+        <v>12.3</v>
       </c>
       <c r="E95">
         <v>100</v>
@@ -2556,13 +2559,13 @@
     </row>
     <row r="96" spans="1:6">
       <c r="A96" s="2">
-        <v>45331</v>
+        <v>45333</v>
       </c>
       <c r="B96">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D96">
-        <v>8.33</v>
+        <v>13.19</v>
       </c>
       <c r="E96">
         <v>100</v>
@@ -2573,13 +2576,13 @@
     </row>
     <row r="97" spans="1:6">
       <c r="A97" s="2">
-        <v>45331</v>
+        <v>45333</v>
       </c>
       <c r="B97">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D97">
-        <v>7.99</v>
+        <v>13.67</v>
       </c>
       <c r="E97">
         <v>100</v>

</xml_diff>

<commit_message>
Adding new RAAL model Production
</commit_message>
<xml_diff>
--- a/RAAL/Production/Input.xlsx
+++ b/RAAL/Production/Input.xlsx
@@ -34,292 +34,292 @@
     <t>Lookup</t>
   </si>
   <si>
-    <t>07.02.202412</t>
-  </si>
-  <si>
-    <t>07.02.202413</t>
-  </si>
-  <si>
-    <t>07.02.202414</t>
-  </si>
-  <si>
-    <t>07.02.202415</t>
-  </si>
-  <si>
-    <t>07.02.202416</t>
-  </si>
-  <si>
-    <t>07.02.202417</t>
-  </si>
-  <si>
-    <t>07.02.202418</t>
-  </si>
-  <si>
-    <t>07.02.202419</t>
-  </si>
-  <si>
-    <t>07.02.202420</t>
-  </si>
-  <si>
-    <t>07.02.202421</t>
-  </si>
-  <si>
-    <t>07.02.202422</t>
-  </si>
-  <si>
-    <t>07.02.202423</t>
-  </si>
-  <si>
-    <t>08.02.20240</t>
-  </si>
-  <si>
-    <t>08.02.20241</t>
-  </si>
-  <si>
-    <t>08.02.20242</t>
-  </si>
-  <si>
-    <t>08.02.20243</t>
-  </si>
-  <si>
-    <t>08.02.20244</t>
-  </si>
-  <si>
-    <t>08.02.20245</t>
-  </si>
-  <si>
-    <t>08.02.20246</t>
-  </si>
-  <si>
-    <t>08.02.20247</t>
-  </si>
-  <si>
-    <t>08.02.20248</t>
-  </si>
-  <si>
-    <t>08.02.20249</t>
-  </si>
-  <si>
-    <t>08.02.202410</t>
-  </si>
-  <si>
-    <t>08.02.202411</t>
-  </si>
-  <si>
-    <t>08.02.202412</t>
-  </si>
-  <si>
-    <t>08.02.202413</t>
-  </si>
-  <si>
-    <t>08.02.202414</t>
-  </si>
-  <si>
-    <t>08.02.202415</t>
-  </si>
-  <si>
-    <t>08.02.202416</t>
-  </si>
-  <si>
-    <t>08.02.202417</t>
-  </si>
-  <si>
-    <t>08.02.202418</t>
-  </si>
-  <si>
-    <t>08.02.202419</t>
-  </si>
-  <si>
-    <t>08.02.202420</t>
-  </si>
-  <si>
-    <t>08.02.202421</t>
-  </si>
-  <si>
-    <t>08.02.202422</t>
-  </si>
-  <si>
-    <t>08.02.202423</t>
-  </si>
-  <si>
-    <t>09.02.20240</t>
-  </si>
-  <si>
-    <t>09.02.20241</t>
-  </si>
-  <si>
-    <t>09.02.20242</t>
-  </si>
-  <si>
-    <t>09.02.20243</t>
-  </si>
-  <si>
-    <t>09.02.20244</t>
-  </si>
-  <si>
-    <t>09.02.20245</t>
-  </si>
-  <si>
-    <t>09.02.20246</t>
-  </si>
-  <si>
-    <t>09.02.20247</t>
-  </si>
-  <si>
-    <t>09.02.20248</t>
-  </si>
-  <si>
-    <t>09.02.20249</t>
-  </si>
-  <si>
-    <t>09.02.202410</t>
-  </si>
-  <si>
-    <t>09.02.202411</t>
-  </si>
-  <si>
-    <t>09.02.202412</t>
-  </si>
-  <si>
-    <t>09.02.202413</t>
-  </si>
-  <si>
-    <t>09.02.202414</t>
-  </si>
-  <si>
-    <t>09.02.202415</t>
-  </si>
-  <si>
-    <t>09.02.202416</t>
-  </si>
-  <si>
-    <t>09.02.202417</t>
-  </si>
-  <si>
-    <t>09.02.202418</t>
-  </si>
-  <si>
-    <t>09.02.202419</t>
-  </si>
-  <si>
-    <t>09.02.202420</t>
-  </si>
-  <si>
-    <t>09.02.202421</t>
-  </si>
-  <si>
-    <t>09.02.202422</t>
-  </si>
-  <si>
-    <t>09.02.202423</t>
-  </si>
-  <si>
-    <t>10.02.20240</t>
-  </si>
-  <si>
-    <t>10.02.20241</t>
-  </si>
-  <si>
-    <t>10.02.20242</t>
-  </si>
-  <si>
-    <t>10.02.20243</t>
-  </si>
-  <si>
-    <t>10.02.20244</t>
-  </si>
-  <si>
-    <t>10.02.20245</t>
-  </si>
-  <si>
-    <t>10.02.20246</t>
-  </si>
-  <si>
-    <t>10.02.20247</t>
-  </si>
-  <si>
-    <t>10.02.20248</t>
-  </si>
-  <si>
-    <t>10.02.20249</t>
-  </si>
-  <si>
-    <t>10.02.202410</t>
-  </si>
-  <si>
-    <t>10.02.202411</t>
-  </si>
-  <si>
-    <t>10.02.202412</t>
-  </si>
-  <si>
-    <t>10.02.202413</t>
-  </si>
-  <si>
-    <t>10.02.202414</t>
-  </si>
-  <si>
-    <t>10.02.202415</t>
-  </si>
-  <si>
-    <t>10.02.202416</t>
-  </si>
-  <si>
-    <t>10.02.202417</t>
-  </si>
-  <si>
-    <t>10.02.202418</t>
-  </si>
-  <si>
-    <t>10.02.202419</t>
-  </si>
-  <si>
-    <t>10.02.202420</t>
-  </si>
-  <si>
-    <t>10.02.202421</t>
-  </si>
-  <si>
-    <t>10.02.202422</t>
-  </si>
-  <si>
-    <t>10.02.202423</t>
-  </si>
-  <si>
-    <t>11.02.20240</t>
-  </si>
-  <si>
-    <t>11.02.20241</t>
-  </si>
-  <si>
-    <t>11.02.20242</t>
-  </si>
-  <si>
-    <t>11.02.20243</t>
-  </si>
-  <si>
-    <t>11.02.20244</t>
-  </si>
-  <si>
-    <t>11.02.20245</t>
-  </si>
-  <si>
-    <t>11.02.20246</t>
-  </si>
-  <si>
-    <t>11.02.20247</t>
-  </si>
-  <si>
-    <t>11.02.20248</t>
-  </si>
-  <si>
-    <t>11.02.20249</t>
-  </si>
-  <si>
-    <t>11.02.202410</t>
-  </si>
-  <si>
-    <t>11.02.202411</t>
+    <t>12.02.202414</t>
+  </si>
+  <si>
+    <t>12.02.202415</t>
+  </si>
+  <si>
+    <t>12.02.202416</t>
+  </si>
+  <si>
+    <t>12.02.202417</t>
+  </si>
+  <si>
+    <t>12.02.202418</t>
+  </si>
+  <si>
+    <t>12.02.202419</t>
+  </si>
+  <si>
+    <t>12.02.202420</t>
+  </si>
+  <si>
+    <t>12.02.202421</t>
+  </si>
+  <si>
+    <t>12.02.202422</t>
+  </si>
+  <si>
+    <t>12.02.202423</t>
+  </si>
+  <si>
+    <t>13.02.20240</t>
+  </si>
+  <si>
+    <t>13.02.20241</t>
+  </si>
+  <si>
+    <t>13.02.20242</t>
+  </si>
+  <si>
+    <t>13.02.20243</t>
+  </si>
+  <si>
+    <t>13.02.20244</t>
+  </si>
+  <si>
+    <t>13.02.20245</t>
+  </si>
+  <si>
+    <t>13.02.20246</t>
+  </si>
+  <si>
+    <t>13.02.20247</t>
+  </si>
+  <si>
+    <t>13.02.20248</t>
+  </si>
+  <si>
+    <t>13.02.20249</t>
+  </si>
+  <si>
+    <t>13.02.202410</t>
+  </si>
+  <si>
+    <t>13.02.202411</t>
+  </si>
+  <si>
+    <t>13.02.202412</t>
+  </si>
+  <si>
+    <t>13.02.202413</t>
+  </si>
+  <si>
+    <t>13.02.202414</t>
+  </si>
+  <si>
+    <t>13.02.202415</t>
+  </si>
+  <si>
+    <t>13.02.202416</t>
+  </si>
+  <si>
+    <t>13.02.202417</t>
+  </si>
+  <si>
+    <t>13.02.202418</t>
+  </si>
+  <si>
+    <t>13.02.202419</t>
+  </si>
+  <si>
+    <t>13.02.202420</t>
+  </si>
+  <si>
+    <t>13.02.202421</t>
+  </si>
+  <si>
+    <t>13.02.202422</t>
+  </si>
+  <si>
+    <t>13.02.202423</t>
+  </si>
+  <si>
+    <t>14.02.20240</t>
+  </si>
+  <si>
+    <t>14.02.20241</t>
+  </si>
+  <si>
+    <t>14.02.20242</t>
+  </si>
+  <si>
+    <t>14.02.20243</t>
+  </si>
+  <si>
+    <t>14.02.20244</t>
+  </si>
+  <si>
+    <t>14.02.20245</t>
+  </si>
+  <si>
+    <t>14.02.20246</t>
+  </si>
+  <si>
+    <t>14.02.20247</t>
+  </si>
+  <si>
+    <t>14.02.20248</t>
+  </si>
+  <si>
+    <t>14.02.20249</t>
+  </si>
+  <si>
+    <t>14.02.202410</t>
+  </si>
+  <si>
+    <t>14.02.202411</t>
+  </si>
+  <si>
+    <t>14.02.202412</t>
+  </si>
+  <si>
+    <t>14.02.202413</t>
+  </si>
+  <si>
+    <t>14.02.202414</t>
+  </si>
+  <si>
+    <t>14.02.202415</t>
+  </si>
+  <si>
+    <t>14.02.202416</t>
+  </si>
+  <si>
+    <t>14.02.202417</t>
+  </si>
+  <si>
+    <t>14.02.202418</t>
+  </si>
+  <si>
+    <t>14.02.202419</t>
+  </si>
+  <si>
+    <t>14.02.202420</t>
+  </si>
+  <si>
+    <t>14.02.202421</t>
+  </si>
+  <si>
+    <t>14.02.202422</t>
+  </si>
+  <si>
+    <t>14.02.202423</t>
+  </si>
+  <si>
+    <t>15.02.20240</t>
+  </si>
+  <si>
+    <t>15.02.20241</t>
+  </si>
+  <si>
+    <t>15.02.20242</t>
+  </si>
+  <si>
+    <t>15.02.20243</t>
+  </si>
+  <si>
+    <t>15.02.20244</t>
+  </si>
+  <si>
+    <t>15.02.20245</t>
+  </si>
+  <si>
+    <t>15.02.20246</t>
+  </si>
+  <si>
+    <t>15.02.20247</t>
+  </si>
+  <si>
+    <t>15.02.20248</t>
+  </si>
+  <si>
+    <t>15.02.20249</t>
+  </si>
+  <si>
+    <t>15.02.202410</t>
+  </si>
+  <si>
+    <t>15.02.202411</t>
+  </si>
+  <si>
+    <t>15.02.202412</t>
+  </si>
+  <si>
+    <t>15.02.202413</t>
+  </si>
+  <si>
+    <t>15.02.202414</t>
+  </si>
+  <si>
+    <t>15.02.202415</t>
+  </si>
+  <si>
+    <t>15.02.202416</t>
+  </si>
+  <si>
+    <t>15.02.202417</t>
+  </si>
+  <si>
+    <t>15.02.202418</t>
+  </si>
+  <si>
+    <t>15.02.202419</t>
+  </si>
+  <si>
+    <t>15.02.202420</t>
+  </si>
+  <si>
+    <t>15.02.202421</t>
+  </si>
+  <si>
+    <t>15.02.202422</t>
+  </si>
+  <si>
+    <t>15.02.202423</t>
+  </si>
+  <si>
+    <t>16.02.20240</t>
+  </si>
+  <si>
+    <t>16.02.20241</t>
+  </si>
+  <si>
+    <t>16.02.20242</t>
+  </si>
+  <si>
+    <t>16.02.20243</t>
+  </si>
+  <si>
+    <t>16.02.20244</t>
+  </si>
+  <si>
+    <t>16.02.20245</t>
+  </si>
+  <si>
+    <t>16.02.20246</t>
+  </si>
+  <si>
+    <t>16.02.20247</t>
+  </si>
+  <si>
+    <t>16.02.20248</t>
+  </si>
+  <si>
+    <t>16.02.20249</t>
+  </si>
+  <si>
+    <t>16.02.202410</t>
+  </si>
+  <si>
+    <t>16.02.202411</t>
+  </si>
+  <si>
+    <t>16.02.202412</t>
+  </si>
+  <si>
+    <t>16.02.202413</t>
   </si>
 </sst>
 </file>
@@ -709,19 +709,19 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="2">
-        <v>45329</v>
+        <v>45334</v>
       </c>
       <c r="B2">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C2">
-        <v>121.03</v>
+        <v>99.61</v>
       </c>
       <c r="D2">
-        <v>8.34</v>
+        <v>11.54</v>
       </c>
       <c r="E2">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="F2" t="s">
         <v>6</v>
@@ -729,19 +729,19 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="2">
-        <v>45329</v>
+        <v>45334</v>
       </c>
       <c r="B3">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C3">
-        <v>125.65</v>
+        <v>66.02</v>
       </c>
       <c r="D3">
-        <v>8.4</v>
+        <v>11.32</v>
       </c>
       <c r="E3">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="F3" t="s">
         <v>7</v>
@@ -749,19 +749,19 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="2">
-        <v>45329</v>
+        <v>45334</v>
       </c>
       <c r="B4">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C4">
-        <v>143.96</v>
+        <v>31.49</v>
       </c>
       <c r="D4">
-        <v>8.48</v>
+        <v>10.63</v>
       </c>
       <c r="E4">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="F4" t="s">
         <v>8</v>
@@ -769,19 +769,19 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="2">
-        <v>45329</v>
+        <v>45334</v>
       </c>
       <c r="B5">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C5">
-        <v>132.55</v>
+        <v>3.4</v>
       </c>
       <c r="D5">
-        <v>7.87</v>
+        <v>9.9</v>
       </c>
       <c r="E5">
-        <v>82</v>
+        <v>99</v>
       </c>
       <c r="F5" t="s">
         <v>9</v>
@@ -789,19 +789,19 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="2">
-        <v>45329</v>
+        <v>45334</v>
       </c>
       <c r="B6">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C6">
-        <v>53.41</v>
+        <v>0</v>
       </c>
       <c r="D6">
-        <v>6.47</v>
+        <v>9.18</v>
       </c>
       <c r="E6">
-        <v>72</v>
+        <v>99</v>
       </c>
       <c r="F6" t="s">
         <v>10</v>
@@ -809,19 +809,19 @@
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="2">
-        <v>45329</v>
+        <v>45334</v>
       </c>
       <c r="B7">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C7">
-        <v>3.51</v>
+        <v>0</v>
       </c>
       <c r="D7">
-        <v>5.99</v>
+        <v>9.039999999999999</v>
       </c>
       <c r="E7">
-        <v>70</v>
+        <v>100</v>
       </c>
       <c r="F7" t="s">
         <v>11</v>
@@ -829,19 +829,19 @@
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="2">
-        <v>45329</v>
+        <v>45334</v>
       </c>
       <c r="B8">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C8">
         <v>0</v>
       </c>
       <c r="D8">
-        <v>6.04</v>
+        <v>8.9</v>
       </c>
       <c r="E8">
-        <v>74</v>
+        <v>100</v>
       </c>
       <c r="F8" t="s">
         <v>12</v>
@@ -849,19 +849,19 @@
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="2">
-        <v>45329</v>
+        <v>45334</v>
       </c>
       <c r="B9">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C9">
         <v>0</v>
       </c>
       <c r="D9">
-        <v>5.86</v>
+        <v>8.42</v>
       </c>
       <c r="E9">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="F9" t="s">
         <v>13</v>
@@ -869,19 +869,19 @@
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="2">
-        <v>45329</v>
+        <v>45334</v>
       </c>
       <c r="B10">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C10">
         <v>0</v>
       </c>
       <c r="D10">
-        <v>5.7</v>
+        <v>8.42</v>
       </c>
       <c r="E10">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="F10" t="s">
         <v>14</v>
@@ -889,19 +889,19 @@
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="2">
-        <v>45329</v>
+        <v>45334</v>
       </c>
       <c r="B11">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C11">
         <v>0</v>
       </c>
       <c r="D11">
-        <v>5.56</v>
+        <v>8.27</v>
       </c>
       <c r="E11">
-        <v>93</v>
+        <v>100</v>
       </c>
       <c r="F11" t="s">
         <v>15</v>
@@ -909,19 +909,19 @@
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="2">
-        <v>45329</v>
+        <v>45335</v>
       </c>
       <c r="B12">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="C12">
         <v>0</v>
       </c>
       <c r="D12">
-        <v>5.5</v>
+        <v>8.109999999999999</v>
       </c>
       <c r="E12">
-        <v>93</v>
+        <v>100</v>
       </c>
       <c r="F12" t="s">
         <v>16</v>
@@ -929,19 +929,19 @@
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="2">
-        <v>45329</v>
+        <v>45335</v>
       </c>
       <c r="B13">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="C13">
         <v>0</v>
       </c>
       <c r="D13">
-        <v>5.43</v>
+        <v>7.96</v>
       </c>
       <c r="E13">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="F13" t="s">
         <v>17</v>
@@ -949,19 +949,19 @@
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="2">
-        <v>45330</v>
+        <v>45335</v>
       </c>
       <c r="B14">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C14">
         <v>0</v>
       </c>
       <c r="D14">
-        <v>5.54</v>
+        <v>7.83</v>
       </c>
       <c r="E14">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="F14" t="s">
         <v>18</v>
@@ -969,19 +969,19 @@
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="2">
-        <v>45330</v>
+        <v>45335</v>
       </c>
       <c r="B15">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C15">
         <v>0</v>
       </c>
       <c r="D15">
-        <v>5.46</v>
+        <v>7.65</v>
       </c>
       <c r="E15">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="F15" t="s">
         <v>19</v>
@@ -989,16 +989,16 @@
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="2">
-        <v>45330</v>
+        <v>45335</v>
       </c>
       <c r="B16">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C16">
         <v>0</v>
       </c>
       <c r="D16">
-        <v>5.42</v>
+        <v>7.47</v>
       </c>
       <c r="E16">
         <v>100</v>
@@ -1009,16 +1009,16 @@
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="2">
-        <v>45330</v>
+        <v>45335</v>
       </c>
       <c r="B17">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C17">
         <v>0</v>
       </c>
       <c r="D17">
-        <v>5.36</v>
+        <v>7.25</v>
       </c>
       <c r="E17">
         <v>100</v>
@@ -1029,16 +1029,16 @@
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="2">
-        <v>45330</v>
+        <v>45335</v>
       </c>
       <c r="B18">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C18">
         <v>0</v>
       </c>
       <c r="D18">
-        <v>5.41</v>
+        <v>7.14</v>
       </c>
       <c r="E18">
         <v>100</v>
@@ -1049,16 +1049,16 @@
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="2">
-        <v>45330</v>
+        <v>45335</v>
       </c>
       <c r="B19">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C19">
-        <v>0</v>
+        <v>1.54</v>
       </c>
       <c r="D19">
-        <v>5.31</v>
+        <v>7.09</v>
       </c>
       <c r="E19">
         <v>100</v>
@@ -1069,16 +1069,16 @@
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="2">
-        <v>45330</v>
+        <v>45335</v>
       </c>
       <c r="B20">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C20">
-        <v>0</v>
+        <v>26.02</v>
       </c>
       <c r="D20">
-        <v>5.19</v>
+        <v>6.89</v>
       </c>
       <c r="E20">
         <v>100</v>
@@ -1089,16 +1089,16 @@
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="2">
-        <v>45330</v>
+        <v>45335</v>
       </c>
       <c r="B21">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C21">
-        <v>0.64</v>
+        <v>61.12</v>
       </c>
       <c r="D21">
-        <v>5.23</v>
+        <v>6.86</v>
       </c>
       <c r="E21">
         <v>100</v>
@@ -1109,16 +1109,16 @@
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="2">
-        <v>45330</v>
+        <v>45335</v>
       </c>
       <c r="B22">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C22">
-        <v>21.31</v>
+        <v>91.14</v>
       </c>
       <c r="D22">
-        <v>5.38</v>
+        <v>7.01</v>
       </c>
       <c r="E22">
         <v>100</v>
@@ -1129,16 +1129,16 @@
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="2">
-        <v>45330</v>
+        <v>45335</v>
       </c>
       <c r="B23">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C23">
-        <v>55.31</v>
+        <v>111.28</v>
       </c>
       <c r="D23">
-        <v>5.75</v>
+        <v>7.01</v>
       </c>
       <c r="E23">
         <v>100</v>
@@ -1149,16 +1149,16 @@
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="2">
-        <v>45330</v>
+        <v>45335</v>
       </c>
       <c r="B24">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C24">
-        <v>84.70999999999999</v>
+        <v>119.09</v>
       </c>
       <c r="D24">
-        <v>6.11</v>
+        <v>7.19</v>
       </c>
       <c r="E24">
         <v>100</v>
@@ -1169,16 +1169,16 @@
     </row>
     <row r="25" spans="1:6">
       <c r="A25" s="2">
-        <v>45330</v>
+        <v>45335</v>
       </c>
       <c r="B25">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C25">
-        <v>104.57</v>
+        <v>113.7</v>
       </c>
       <c r="D25">
-        <v>6.56</v>
+        <v>7.47</v>
       </c>
       <c r="E25">
         <v>100</v>
@@ -1189,16 +1189,16 @@
     </row>
     <row r="26" spans="1:6">
       <c r="A26" s="2">
-        <v>45330</v>
+        <v>45335</v>
       </c>
       <c r="B26">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C26">
-        <v>112.57</v>
+        <v>95.70999999999999</v>
       </c>
       <c r="D26">
-        <v>6.68</v>
+        <v>7.48</v>
       </c>
       <c r="E26">
         <v>100</v>
@@ -1209,16 +1209,16 @@
     </row>
     <row r="27" spans="1:6">
       <c r="A27" s="2">
-        <v>45330</v>
+        <v>45335</v>
       </c>
       <c r="B27">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C27">
-        <v>107.5</v>
+        <v>67.26000000000001</v>
       </c>
       <c r="D27">
-        <v>6.62</v>
+        <v>6.91</v>
       </c>
       <c r="E27">
         <v>100</v>
@@ -1229,16 +1229,16 @@
     </row>
     <row r="28" spans="1:6">
       <c r="A28" s="2">
-        <v>45330</v>
+        <v>45335</v>
       </c>
       <c r="B28">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C28">
-        <v>89.31</v>
+        <v>32.55</v>
       </c>
       <c r="D28">
-        <v>6.25</v>
+        <v>5.97</v>
       </c>
       <c r="E28">
         <v>100</v>
@@ -1249,16 +1249,16 @@
     </row>
     <row r="29" spans="1:6">
       <c r="A29" s="2">
-        <v>45330</v>
+        <v>45335</v>
       </c>
       <c r="B29">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C29">
-        <v>60.92</v>
+        <v>3.76</v>
       </c>
       <c r="D29">
-        <v>6.22</v>
+        <v>5.27</v>
       </c>
       <c r="E29">
         <v>100</v>
@@ -1269,16 +1269,16 @@
     </row>
     <row r="30" spans="1:6">
       <c r="A30" s="2">
-        <v>45330</v>
+        <v>45335</v>
       </c>
       <c r="B30">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C30">
-        <v>27.2</v>
+        <v>0</v>
       </c>
       <c r="D30">
-        <v>6.2</v>
+        <v>4.74</v>
       </c>
       <c r="E30">
         <v>100</v>
@@ -1289,16 +1289,16 @@
     </row>
     <row r="31" spans="1:6">
       <c r="A31" s="2">
-        <v>45330</v>
+        <v>45335</v>
       </c>
       <c r="B31">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C31">
-        <v>2.07</v>
+        <v>0</v>
       </c>
       <c r="D31">
-        <v>6.37</v>
+        <v>4.45</v>
       </c>
       <c r="E31">
         <v>100</v>
@@ -1309,16 +1309,16 @@
     </row>
     <row r="32" spans="1:6">
       <c r="A32" s="2">
-        <v>45330</v>
+        <v>45335</v>
       </c>
       <c r="B32">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C32">
         <v>0</v>
       </c>
       <c r="D32">
-        <v>6.68</v>
+        <v>4.26</v>
       </c>
       <c r="E32">
         <v>100</v>
@@ -1329,16 +1329,16 @@
     </row>
     <row r="33" spans="1:6">
       <c r="A33" s="2">
-        <v>45330</v>
+        <v>45335</v>
       </c>
       <c r="B33">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C33">
         <v>0</v>
       </c>
       <c r="D33">
-        <v>6.39</v>
+        <v>4.08</v>
       </c>
       <c r="E33">
         <v>100</v>
@@ -1349,16 +1349,16 @@
     </row>
     <row r="34" spans="1:6">
       <c r="A34" s="2">
-        <v>45330</v>
+        <v>45335</v>
       </c>
       <c r="B34">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C34">
         <v>0</v>
       </c>
       <c r="D34">
-        <v>6.23</v>
+        <v>3.8</v>
       </c>
       <c r="E34">
         <v>100</v>
@@ -1369,16 +1369,16 @@
     </row>
     <row r="35" spans="1:6">
       <c r="A35" s="2">
-        <v>45330</v>
+        <v>45335</v>
       </c>
       <c r="B35">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C35">
         <v>0</v>
       </c>
       <c r="D35">
-        <v>6.21</v>
+        <v>3.75</v>
       </c>
       <c r="E35">
         <v>100</v>
@@ -1389,16 +1389,16 @@
     </row>
     <row r="36" spans="1:6">
       <c r="A36" s="2">
-        <v>45330</v>
+        <v>45336</v>
       </c>
       <c r="B36">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="C36">
         <v>0</v>
       </c>
       <c r="D36">
-        <v>6.21</v>
+        <v>3.66</v>
       </c>
       <c r="E36">
         <v>100</v>
@@ -1409,16 +1409,16 @@
     </row>
     <row r="37" spans="1:6">
       <c r="A37" s="2">
-        <v>45330</v>
+        <v>45336</v>
       </c>
       <c r="B37">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="C37">
         <v>0</v>
       </c>
       <c r="D37">
-        <v>6.06</v>
+        <v>3.49</v>
       </c>
       <c r="E37">
         <v>100</v>
@@ -1429,19 +1429,19 @@
     </row>
     <row r="38" spans="1:6">
       <c r="A38" s="2">
-        <v>45331</v>
+        <v>45336</v>
       </c>
       <c r="B38">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C38">
         <v>0</v>
       </c>
       <c r="D38">
-        <v>6.01</v>
+        <v>3.17</v>
       </c>
       <c r="E38">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F38" t="s">
         <v>42</v>
@@ -1449,19 +1449,19 @@
     </row>
     <row r="39" spans="1:6">
       <c r="A39" s="2">
-        <v>45331</v>
+        <v>45336</v>
       </c>
       <c r="B39">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C39">
         <v>0</v>
       </c>
       <c r="D39">
-        <v>5.93</v>
+        <v>2.79</v>
       </c>
       <c r="E39">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F39" t="s">
         <v>43</v>
@@ -1469,16 +1469,16 @@
     </row>
     <row r="40" spans="1:6">
       <c r="A40" s="2">
-        <v>45331</v>
+        <v>45336</v>
       </c>
       <c r="B40">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C40">
         <v>0</v>
       </c>
       <c r="D40">
-        <v>5.91</v>
+        <v>2.57</v>
       </c>
       <c r="E40">
         <v>99</v>
@@ -1489,16 +1489,16 @@
     </row>
     <row r="41" spans="1:6">
       <c r="A41" s="2">
-        <v>45331</v>
+        <v>45336</v>
       </c>
       <c r="B41">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C41">
         <v>0</v>
       </c>
       <c r="D41">
-        <v>5.97</v>
+        <v>2.3</v>
       </c>
       <c r="E41">
         <v>99</v>
@@ -1509,16 +1509,16 @@
     </row>
     <row r="42" spans="1:6">
       <c r="A42" s="2">
-        <v>45331</v>
+        <v>45336</v>
       </c>
       <c r="B42">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C42">
         <v>0</v>
       </c>
       <c r="D42">
-        <v>5.63</v>
+        <v>2.4</v>
       </c>
       <c r="E42">
         <v>99</v>
@@ -1529,19 +1529,19 @@
     </row>
     <row r="43" spans="1:6">
       <c r="A43" s="2">
-        <v>45331</v>
+        <v>45336</v>
       </c>
       <c r="B43">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C43">
-        <v>0</v>
+        <v>1.96</v>
       </c>
       <c r="D43">
-        <v>5.97</v>
+        <v>3.46</v>
       </c>
       <c r="E43">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="F43" t="s">
         <v>47</v>
@@ -1549,19 +1549,19 @@
     </row>
     <row r="44" spans="1:6">
       <c r="A44" s="2">
-        <v>45331</v>
+        <v>45336</v>
       </c>
       <c r="B44">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C44">
-        <v>0</v>
+        <v>28.7</v>
       </c>
       <c r="D44">
-        <v>6.03</v>
+        <v>4.39</v>
       </c>
       <c r="E44">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="F44" t="s">
         <v>48</v>
@@ -1569,16 +1569,16 @@
     </row>
     <row r="45" spans="1:6">
       <c r="A45" s="2">
-        <v>45331</v>
+        <v>45336</v>
       </c>
       <c r="B45">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C45">
-        <v>0.82</v>
+        <v>63.97</v>
       </c>
       <c r="D45">
-        <v>6.24</v>
+        <v>5.26</v>
       </c>
       <c r="E45">
         <v>100</v>
@@ -1589,16 +1589,16 @@
     </row>
     <row r="46" spans="1:6">
       <c r="A46" s="2">
-        <v>45331</v>
+        <v>45336</v>
       </c>
       <c r="B46">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C46">
-        <v>22.82</v>
+        <v>94.34999999999999</v>
       </c>
       <c r="D46">
-        <v>6.26</v>
+        <v>6.03</v>
       </c>
       <c r="E46">
         <v>100</v>
@@ -1609,16 +1609,16 @@
     </row>
     <row r="47" spans="1:6">
       <c r="A47" s="2">
-        <v>45331</v>
+        <v>45336</v>
       </c>
       <c r="B47">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C47">
-        <v>56.17</v>
+        <v>115.36</v>
       </c>
       <c r="D47">
-        <v>6.33</v>
+        <v>6.61</v>
       </c>
       <c r="E47">
         <v>100</v>
@@ -1629,16 +1629,16 @@
     </row>
     <row r="48" spans="1:6">
       <c r="A48" s="2">
-        <v>45331</v>
+        <v>45336</v>
       </c>
       <c r="B48">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C48">
-        <v>85.78</v>
+        <v>123.66</v>
       </c>
       <c r="D48">
-        <v>6.64</v>
+        <v>7.09</v>
       </c>
       <c r="E48">
         <v>100</v>
@@ -1649,19 +1649,19 @@
     </row>
     <row r="49" spans="1:6">
       <c r="A49" s="2">
-        <v>45331</v>
+        <v>45336</v>
       </c>
       <c r="B49">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C49">
-        <v>105.74</v>
+        <v>118.98</v>
       </c>
       <c r="D49">
-        <v>6.8</v>
+        <v>7.19</v>
       </c>
       <c r="E49">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F49" t="s">
         <v>53</v>
@@ -1669,19 +1669,19 @@
     </row>
     <row r="50" spans="1:6">
       <c r="A50" s="2">
-        <v>45331</v>
+        <v>45336</v>
       </c>
       <c r="B50">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C50">
-        <v>113.45</v>
+        <v>103.58</v>
       </c>
       <c r="D50">
-        <v>6.6</v>
+        <v>6.99</v>
       </c>
       <c r="E50">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="F50" t="s">
         <v>54</v>
@@ -1689,19 +1689,19 @@
     </row>
     <row r="51" spans="1:6">
       <c r="A51" s="2">
-        <v>45331</v>
+        <v>45336</v>
       </c>
       <c r="B51">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C51">
-        <v>108.1</v>
+        <v>86.95</v>
       </c>
       <c r="D51">
-        <v>6.48</v>
+        <v>5.91</v>
       </c>
       <c r="E51">
-        <v>100</v>
+        <v>87</v>
       </c>
       <c r="F51" t="s">
         <v>55</v>
@@ -1709,19 +1709,19 @@
     </row>
     <row r="52" spans="1:6">
       <c r="A52" s="2">
-        <v>45331</v>
+        <v>45336</v>
       </c>
       <c r="B52">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C52">
-        <v>90.28</v>
+        <v>58.21</v>
       </c>
       <c r="D52">
-        <v>6.46</v>
+        <v>4.22</v>
       </c>
       <c r="E52">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="F52" t="s">
         <v>56</v>
@@ -1729,19 +1729,19 @@
     </row>
     <row r="53" spans="1:6">
       <c r="A53" s="2">
-        <v>45331</v>
+        <v>45336</v>
       </c>
       <c r="B53">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C53">
-        <v>62.2</v>
+        <v>8.779999999999999</v>
       </c>
       <c r="D53">
-        <v>6.28</v>
+        <v>3.24</v>
       </c>
       <c r="E53">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="F53" t="s">
         <v>57</v>
@@ -1749,19 +1749,19 @@
     </row>
     <row r="54" spans="1:6">
       <c r="A54" s="2">
-        <v>45331</v>
+        <v>45336</v>
       </c>
       <c r="B54">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C54">
-        <v>28.26</v>
+        <v>0</v>
       </c>
       <c r="D54">
-        <v>6.37</v>
+        <v>2.55</v>
       </c>
       <c r="E54">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="F54" t="s">
         <v>58</v>
@@ -1769,19 +1769,19 @@
     </row>
     <row r="55" spans="1:6">
       <c r="A55" s="2">
-        <v>45331</v>
+        <v>45336</v>
       </c>
       <c r="B55">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C55">
-        <v>2.38</v>
+        <v>0</v>
       </c>
       <c r="D55">
-        <v>6.7</v>
+        <v>2.03</v>
       </c>
       <c r="E55">
-        <v>100</v>
+        <v>68</v>
       </c>
       <c r="F55" t="s">
         <v>59</v>
@@ -1789,19 +1789,19 @@
     </row>
     <row r="56" spans="1:6">
       <c r="A56" s="2">
-        <v>45331</v>
+        <v>45336</v>
       </c>
       <c r="B56">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C56">
         <v>0</v>
       </c>
       <c r="D56">
-        <v>6.64</v>
+        <v>1.53</v>
       </c>
       <c r="E56">
-        <v>100</v>
+        <v>62</v>
       </c>
       <c r="F56" t="s">
         <v>60</v>
@@ -1809,19 +1809,19 @@
     </row>
     <row r="57" spans="1:6">
       <c r="A57" s="2">
-        <v>45331</v>
+        <v>45336</v>
       </c>
       <c r="B57">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C57">
         <v>0</v>
       </c>
       <c r="D57">
-        <v>6.68</v>
+        <v>1.08</v>
       </c>
       <c r="E57">
-        <v>100</v>
+        <v>49</v>
       </c>
       <c r="F57" t="s">
         <v>61</v>
@@ -1829,19 +1829,19 @@
     </row>
     <row r="58" spans="1:6">
       <c r="A58" s="2">
-        <v>45331</v>
+        <v>45336</v>
       </c>
       <c r="B58">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C58">
         <v>0</v>
       </c>
       <c r="D58">
-        <v>6.74</v>
+        <v>0.76</v>
       </c>
       <c r="E58">
-        <v>100</v>
+        <v>42</v>
       </c>
       <c r="F58" t="s">
         <v>62</v>
@@ -1849,19 +1849,19 @@
     </row>
     <row r="59" spans="1:6">
       <c r="A59" s="2">
-        <v>45331</v>
+        <v>45336</v>
       </c>
       <c r="B59">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C59">
         <v>0</v>
       </c>
       <c r="D59">
-        <v>6.65</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="E59">
-        <v>100</v>
+        <v>38</v>
       </c>
       <c r="F59" t="s">
         <v>63</v>
@@ -1869,19 +1869,19 @@
     </row>
     <row r="60" spans="1:6">
       <c r="A60" s="2">
-        <v>45331</v>
+        <v>45337</v>
       </c>
       <c r="B60">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="C60">
         <v>0</v>
       </c>
       <c r="D60">
-        <v>6.58</v>
+        <v>0.47</v>
       </c>
       <c r="E60">
-        <v>100</v>
+        <v>35</v>
       </c>
       <c r="F60" t="s">
         <v>64</v>
@@ -1889,19 +1889,19 @@
     </row>
     <row r="61" spans="1:6">
       <c r="A61" s="2">
-        <v>45331</v>
+        <v>45337</v>
       </c>
       <c r="B61">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="C61">
         <v>0</v>
       </c>
       <c r="D61">
-        <v>6.52</v>
+        <v>0.38</v>
       </c>
       <c r="E61">
-        <v>100</v>
+        <v>24</v>
       </c>
       <c r="F61" t="s">
         <v>65</v>
@@ -1909,19 +1909,19 @@
     </row>
     <row r="62" spans="1:6">
       <c r="A62" s="2">
-        <v>45332</v>
+        <v>45337</v>
       </c>
       <c r="B62">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C62">
         <v>0</v>
       </c>
       <c r="D62">
-        <v>6.39</v>
+        <v>0.33</v>
       </c>
       <c r="E62">
-        <v>100</v>
+        <v>23</v>
       </c>
       <c r="F62" t="s">
         <v>66</v>
@@ -1929,19 +1929,19 @@
     </row>
     <row r="63" spans="1:6">
       <c r="A63" s="2">
-        <v>45332</v>
+        <v>45337</v>
       </c>
       <c r="B63">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C63">
         <v>0</v>
       </c>
       <c r="D63">
-        <v>6.45</v>
+        <v>0.31</v>
       </c>
       <c r="E63">
-        <v>100</v>
+        <v>29</v>
       </c>
       <c r="F63" t="s">
         <v>67</v>
@@ -1949,19 +1949,19 @@
     </row>
     <row r="64" spans="1:6">
       <c r="A64" s="2">
-        <v>45332</v>
+        <v>45337</v>
       </c>
       <c r="B64">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C64">
         <v>0</v>
       </c>
       <c r="D64">
-        <v>6.59</v>
+        <v>0.36</v>
       </c>
       <c r="E64">
-        <v>100</v>
+        <v>41</v>
       </c>
       <c r="F64" t="s">
         <v>68</v>
@@ -1969,19 +1969,19 @@
     </row>
     <row r="65" spans="1:6">
       <c r="A65" s="2">
-        <v>45332</v>
+        <v>45337</v>
       </c>
       <c r="B65">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C65">
         <v>0</v>
       </c>
       <c r="D65">
-        <v>6.82</v>
+        <v>0.32</v>
       </c>
       <c r="E65">
-        <v>100</v>
+        <v>47</v>
       </c>
       <c r="F65" t="s">
         <v>69</v>
@@ -1989,19 +1989,19 @@
     </row>
     <row r="66" spans="1:6">
       <c r="A66" s="2">
-        <v>45332</v>
+        <v>45337</v>
       </c>
       <c r="B66">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C66">
         <v>0</v>
       </c>
       <c r="D66">
-        <v>7</v>
+        <v>0.68</v>
       </c>
       <c r="E66">
-        <v>100</v>
+        <v>52</v>
       </c>
       <c r="F66" t="s">
         <v>70</v>
@@ -2009,19 +2009,19 @@
     </row>
     <row r="67" spans="1:6">
       <c r="A67" s="2">
-        <v>45332</v>
+        <v>45337</v>
       </c>
       <c r="B67">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C67">
-        <v>0</v>
+        <v>7.81</v>
       </c>
       <c r="D67">
-        <v>6.93</v>
+        <v>2.26</v>
       </c>
       <c r="E67">
-        <v>100</v>
+        <v>51</v>
       </c>
       <c r="F67" t="s">
         <v>71</v>
@@ -2029,19 +2029,19 @@
     </row>
     <row r="68" spans="1:6">
       <c r="A68" s="2">
-        <v>45332</v>
+        <v>45337</v>
       </c>
       <c r="B68">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C68">
-        <v>0</v>
+        <v>103.7</v>
       </c>
       <c r="D68">
-        <v>6.82</v>
+        <v>3.92</v>
       </c>
       <c r="E68">
-        <v>100</v>
+        <v>33</v>
       </c>
       <c r="F68" t="s">
         <v>72</v>
@@ -2049,19 +2049,19 @@
     </row>
     <row r="69" spans="1:6">
       <c r="A69" s="2">
-        <v>45332</v>
+        <v>45337</v>
       </c>
       <c r="B69">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C69">
-        <v>0.91</v>
+        <v>242.85</v>
       </c>
       <c r="D69">
-        <v>6.95</v>
+        <v>5.22</v>
       </c>
       <c r="E69">
-        <v>100</v>
+        <v>25</v>
       </c>
       <c r="F69" t="s">
         <v>73</v>
@@ -2069,19 +2069,19 @@
     </row>
     <row r="70" spans="1:6">
       <c r="A70" s="2">
-        <v>45332</v>
+        <v>45337</v>
       </c>
       <c r="B70">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C70">
-        <v>22.97</v>
+        <v>370.55</v>
       </c>
       <c r="D70">
-        <v>7.13</v>
+        <v>5.87</v>
       </c>
       <c r="E70">
-        <v>100</v>
+        <v>22</v>
       </c>
       <c r="F70" t="s">
         <v>74</v>
@@ -2089,19 +2089,19 @@
     </row>
     <row r="71" spans="1:6">
       <c r="A71" s="2">
-        <v>45332</v>
+        <v>45337</v>
       </c>
       <c r="B71">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C71">
-        <v>57.38</v>
+        <v>453.5</v>
       </c>
       <c r="D71">
-        <v>7.37</v>
+        <v>6.3</v>
       </c>
       <c r="E71">
-        <v>100</v>
+        <v>19</v>
       </c>
       <c r="F71" t="s">
         <v>75</v>
@@ -2109,19 +2109,19 @@
     </row>
     <row r="72" spans="1:6">
       <c r="A72" s="2">
-        <v>45332</v>
+        <v>45337</v>
       </c>
       <c r="B72">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C72">
-        <v>87.08</v>
+        <v>485.87</v>
       </c>
       <c r="D72">
-        <v>7.45</v>
+        <v>6.5</v>
       </c>
       <c r="E72">
-        <v>100</v>
+        <v>18</v>
       </c>
       <c r="F72" t="s">
         <v>76</v>
@@ -2129,19 +2129,19 @@
     </row>
     <row r="73" spans="1:6">
       <c r="A73" s="2">
-        <v>45332</v>
+        <v>45337</v>
       </c>
       <c r="B73">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C73">
-        <v>107.06</v>
+        <v>464.75</v>
       </c>
       <c r="D73">
-        <v>7.49</v>
+        <v>6.43</v>
       </c>
       <c r="E73">
-        <v>100</v>
+        <v>33</v>
       </c>
       <c r="F73" t="s">
         <v>77</v>
@@ -2149,19 +2149,19 @@
     </row>
     <row r="74" spans="1:6">
       <c r="A74" s="2">
-        <v>45332</v>
+        <v>45337</v>
       </c>
       <c r="B74">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C74">
-        <v>114.81</v>
+        <v>391.1</v>
       </c>
       <c r="D74">
-        <v>8.02</v>
+        <v>6.08</v>
       </c>
       <c r="E74">
-        <v>100</v>
+        <v>25</v>
       </c>
       <c r="F74" t="s">
         <v>78</v>
@@ -2169,19 +2169,19 @@
     </row>
     <row r="75" spans="1:6">
       <c r="A75" s="2">
-        <v>45332</v>
+        <v>45337</v>
       </c>
       <c r="B75">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C75">
-        <v>109.46</v>
+        <v>275.22</v>
       </c>
       <c r="D75">
-        <v>7.93</v>
+        <v>4.64</v>
       </c>
       <c r="E75">
-        <v>100</v>
+        <v>22</v>
       </c>
       <c r="F75" t="s">
         <v>79</v>
@@ -2189,19 +2189,19 @@
     </row>
     <row r="76" spans="1:6">
       <c r="A76" s="2">
-        <v>45332</v>
+        <v>45337</v>
       </c>
       <c r="B76">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C76">
-        <v>91.62</v>
+        <v>137.98</v>
       </c>
       <c r="D76">
-        <v>7.77</v>
+        <v>2.73</v>
       </c>
       <c r="E76">
-        <v>100</v>
+        <v>18</v>
       </c>
       <c r="F76" t="s">
         <v>80</v>
@@ -2209,19 +2209,19 @@
     </row>
     <row r="77" spans="1:6">
       <c r="A77" s="2">
-        <v>45332</v>
+        <v>45337</v>
       </c>
       <c r="B77">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C77">
-        <v>63.46</v>
+        <v>18.03</v>
       </c>
       <c r="D77">
-        <v>7.77</v>
+        <v>2.16</v>
       </c>
       <c r="E77">
-        <v>100</v>
+        <v>14</v>
       </c>
       <c r="F77" t="s">
         <v>81</v>
@@ -2229,19 +2229,19 @@
     </row>
     <row r="78" spans="1:6">
       <c r="A78" s="2">
-        <v>45332</v>
+        <v>45337</v>
       </c>
       <c r="B78">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C78">
-        <v>29.32</v>
+        <v>0</v>
       </c>
       <c r="D78">
-        <v>7.55</v>
+        <v>1.77</v>
       </c>
       <c r="E78">
-        <v>100</v>
+        <v>12</v>
       </c>
       <c r="F78" t="s">
         <v>82</v>
@@ -2249,19 +2249,19 @@
     </row>
     <row r="79" spans="1:6">
       <c r="A79" s="2">
-        <v>45332</v>
+        <v>45337</v>
       </c>
       <c r="B79">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C79">
-        <v>2.71</v>
+        <v>0</v>
       </c>
       <c r="D79">
-        <v>7.52</v>
+        <v>1.45</v>
       </c>
       <c r="E79">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="F79" t="s">
         <v>83</v>
@@ -2269,19 +2269,19 @@
     </row>
     <row r="80" spans="1:6">
       <c r="A80" s="2">
-        <v>45332</v>
+        <v>45337</v>
       </c>
       <c r="B80">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C80">
         <v>0</v>
       </c>
       <c r="D80">
-        <v>7.55</v>
+        <v>1.29</v>
       </c>
       <c r="E80">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="F80" t="s">
         <v>84</v>
@@ -2289,19 +2289,19 @@
     </row>
     <row r="81" spans="1:6">
       <c r="A81" s="2">
-        <v>45332</v>
+        <v>45337</v>
       </c>
       <c r="B81">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C81">
         <v>0</v>
       </c>
       <c r="D81">
-        <v>7.64</v>
+        <v>1.17</v>
       </c>
       <c r="E81">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="F81" t="s">
         <v>85</v>
@@ -2309,19 +2309,19 @@
     </row>
     <row r="82" spans="1:6">
       <c r="A82" s="2">
-        <v>45332</v>
+        <v>45337</v>
       </c>
       <c r="B82">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C82">
         <v>0</v>
       </c>
       <c r="D82">
-        <v>7.78</v>
+        <v>1.1</v>
       </c>
       <c r="E82">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="F82" t="s">
         <v>86</v>
@@ -2329,19 +2329,19 @@
     </row>
     <row r="83" spans="1:6">
       <c r="A83" s="2">
-        <v>45332</v>
+        <v>45337</v>
       </c>
       <c r="B83">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C83">
         <v>0</v>
       </c>
       <c r="D83">
-        <v>7.93</v>
+        <v>1.02</v>
       </c>
       <c r="E83">
-        <v>100</v>
+        <v>2</v>
       </c>
       <c r="F83" t="s">
         <v>87</v>
@@ -2349,19 +2349,16 @@
     </row>
     <row r="84" spans="1:6">
       <c r="A84" s="2">
-        <v>45332</v>
+        <v>45338</v>
       </c>
       <c r="B84">
-        <v>22</v>
-      </c>
-      <c r="C84">
         <v>0</v>
       </c>
       <c r="D84">
-        <v>7.2</v>
+        <v>0.9399999999999999</v>
       </c>
       <c r="E84">
-        <v>100</v>
+        <v>2</v>
       </c>
       <c r="F84" t="s">
         <v>88</v>
@@ -2369,19 +2366,16 @@
     </row>
     <row r="85" spans="1:6">
       <c r="A85" s="2">
-        <v>45332</v>
+        <v>45338</v>
       </c>
       <c r="B85">
-        <v>23</v>
-      </c>
-      <c r="C85">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D85">
-        <v>7.38</v>
+        <v>0.84</v>
       </c>
       <c r="E85">
-        <v>100</v>
+        <v>6</v>
       </c>
       <c r="F85" t="s">
         <v>89</v>
@@ -2389,16 +2383,16 @@
     </row>
     <row r="86" spans="1:6">
       <c r="A86" s="2">
-        <v>45333</v>
+        <v>45338</v>
       </c>
       <c r="B86">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D86">
-        <v>7.6</v>
+        <v>0.77</v>
       </c>
       <c r="E86">
-        <v>100</v>
+        <v>5</v>
       </c>
       <c r="F86" t="s">
         <v>90</v>
@@ -2406,16 +2400,16 @@
     </row>
     <row r="87" spans="1:6">
       <c r="A87" s="2">
-        <v>45333</v>
+        <v>45338</v>
       </c>
       <c r="B87">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D87">
-        <v>7.66</v>
+        <v>0.7</v>
       </c>
       <c r="E87">
-        <v>100</v>
+        <v>4</v>
       </c>
       <c r="F87" t="s">
         <v>91</v>
@@ -2423,16 +2417,16 @@
     </row>
     <row r="88" spans="1:6">
       <c r="A88" s="2">
-        <v>45333</v>
+        <v>45338</v>
       </c>
       <c r="B88">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D88">
-        <v>7.45</v>
+        <v>0.6</v>
       </c>
       <c r="E88">
-        <v>100</v>
+        <v>3</v>
       </c>
       <c r="F88" t="s">
         <v>92</v>
@@ -2440,16 +2434,16 @@
     </row>
     <row r="89" spans="1:6">
       <c r="A89" s="2">
-        <v>45333</v>
+        <v>45338</v>
       </c>
       <c r="B89">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D89">
-        <v>7.53</v>
+        <v>0.54</v>
       </c>
       <c r="E89">
-        <v>100</v>
+        <v>2</v>
       </c>
       <c r="F89" t="s">
         <v>93</v>
@@ -2457,16 +2451,16 @@
     </row>
     <row r="90" spans="1:6">
       <c r="A90" s="2">
-        <v>45333</v>
+        <v>45338</v>
       </c>
       <c r="B90">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D90">
-        <v>7.68</v>
+        <v>0.87</v>
       </c>
       <c r="E90">
-        <v>100</v>
+        <v>2</v>
       </c>
       <c r="F90" t="s">
         <v>94</v>
@@ -2474,16 +2468,16 @@
     </row>
     <row r="91" spans="1:6">
       <c r="A91" s="2">
-        <v>45333</v>
+        <v>45338</v>
       </c>
       <c r="B91">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D91">
-        <v>7.17</v>
+        <v>2.8</v>
       </c>
       <c r="E91">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="F91" t="s">
         <v>95</v>
@@ -2491,16 +2485,16 @@
     </row>
     <row r="92" spans="1:6">
       <c r="A92" s="2">
-        <v>45333</v>
+        <v>45338</v>
       </c>
       <c r="B92">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D92">
-        <v>7.55</v>
+        <v>4.63</v>
       </c>
       <c r="E92">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="F92" t="s">
         <v>96</v>
@@ -2508,16 +2502,16 @@
     </row>
     <row r="93" spans="1:6">
       <c r="A93" s="2">
-        <v>45333</v>
+        <v>45338</v>
       </c>
       <c r="B93">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D93">
-        <v>8.460000000000001</v>
+        <v>6.02</v>
       </c>
       <c r="E93">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="F93" t="s">
         <v>97</v>
@@ -2525,16 +2519,16 @@
     </row>
     <row r="94" spans="1:6">
       <c r="A94" s="2">
-        <v>45333</v>
+        <v>45338</v>
       </c>
       <c r="B94">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D94">
-        <v>9.94</v>
+        <v>6.94</v>
       </c>
       <c r="E94">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="F94" t="s">
         <v>98</v>
@@ -2542,16 +2536,16 @@
     </row>
     <row r="95" spans="1:6">
       <c r="A95" s="2">
-        <v>45333</v>
+        <v>45338</v>
       </c>
       <c r="B95">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D95">
-        <v>12.3</v>
+        <v>7.49</v>
       </c>
       <c r="E95">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="F95" t="s">
         <v>99</v>
@@ -2559,16 +2553,16 @@
     </row>
     <row r="96" spans="1:6">
       <c r="A96" s="2">
-        <v>45333</v>
+        <v>45338</v>
       </c>
       <c r="B96">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D96">
-        <v>13.19</v>
+        <v>7.72</v>
       </c>
       <c r="E96">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="F96" t="s">
         <v>100</v>
@@ -2576,16 +2570,16 @@
     </row>
     <row r="97" spans="1:6">
       <c r="A97" s="2">
-        <v>45333</v>
+        <v>45338</v>
       </c>
       <c r="B97">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D97">
-        <v>13.67</v>
+        <v>7.63</v>
       </c>
       <c r="E97">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="F97" t="s">
         <v>101</v>

</xml_diff>

<commit_message>
Updating the models with the consideration of the PVPP as feature
</commit_message>
<xml_diff>
--- a/RAAL/Production/Input.xlsx
+++ b/RAAL/Production/Input.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="101">
   <si>
     <t>Data</t>
   </si>
@@ -34,75 +34,6 @@
     <t>Lookup</t>
   </si>
   <si>
-    <t>12.02.202414</t>
-  </si>
-  <si>
-    <t>12.02.202415</t>
-  </si>
-  <si>
-    <t>12.02.202416</t>
-  </si>
-  <si>
-    <t>12.02.202417</t>
-  </si>
-  <si>
-    <t>12.02.202418</t>
-  </si>
-  <si>
-    <t>12.02.202419</t>
-  </si>
-  <si>
-    <t>12.02.202420</t>
-  </si>
-  <si>
-    <t>12.02.202421</t>
-  </si>
-  <si>
-    <t>12.02.202422</t>
-  </si>
-  <si>
-    <t>12.02.202423</t>
-  </si>
-  <si>
-    <t>13.02.20240</t>
-  </si>
-  <si>
-    <t>13.02.20241</t>
-  </si>
-  <si>
-    <t>13.02.20242</t>
-  </si>
-  <si>
-    <t>13.02.20243</t>
-  </si>
-  <si>
-    <t>13.02.20244</t>
-  </si>
-  <si>
-    <t>13.02.20245</t>
-  </si>
-  <si>
-    <t>13.02.20246</t>
-  </si>
-  <si>
-    <t>13.02.20247</t>
-  </si>
-  <si>
-    <t>13.02.20248</t>
-  </si>
-  <si>
-    <t>13.02.20249</t>
-  </si>
-  <si>
-    <t>13.02.202410</t>
-  </si>
-  <si>
-    <t>13.02.202411</t>
-  </si>
-  <si>
-    <t>13.02.202412</t>
-  </si>
-  <si>
     <t>13.02.202413</t>
   </si>
   <si>
@@ -320,6 +251,72 @@
   </si>
   <si>
     <t>16.02.202413</t>
+  </si>
+  <si>
+    <t>16.02.202414</t>
+  </si>
+  <si>
+    <t>16.02.202415</t>
+  </si>
+  <si>
+    <t>16.02.202416</t>
+  </si>
+  <si>
+    <t>16.02.202417</t>
+  </si>
+  <si>
+    <t>16.02.202418</t>
+  </si>
+  <si>
+    <t>16.02.202419</t>
+  </si>
+  <si>
+    <t>16.02.202420</t>
+  </si>
+  <si>
+    <t>16.02.202421</t>
+  </si>
+  <si>
+    <t>16.02.202422</t>
+  </si>
+  <si>
+    <t>16.02.202423</t>
+  </si>
+  <si>
+    <t>17.02.20240</t>
+  </si>
+  <si>
+    <t>17.02.20241</t>
+  </si>
+  <si>
+    <t>17.02.20242</t>
+  </si>
+  <si>
+    <t>17.02.20243</t>
+  </si>
+  <si>
+    <t>17.02.20244</t>
+  </si>
+  <si>
+    <t>17.02.20245</t>
+  </si>
+  <si>
+    <t>17.02.20246</t>
+  </si>
+  <si>
+    <t>17.02.20247</t>
+  </si>
+  <si>
+    <t>17.02.20248</t>
+  </si>
+  <si>
+    <t>17.02.20249</t>
+  </si>
+  <si>
+    <t>17.02.202410</t>
+  </si>
+  <si>
+    <t>17.02.202411</t>
   </si>
 </sst>
 </file>
@@ -709,19 +706,19 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="2">
-        <v>45334</v>
+        <v>45335</v>
       </c>
       <c r="B2">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C2">
-        <v>99.61</v>
+        <v>113.7</v>
       </c>
       <c r="D2">
-        <v>11.54</v>
+        <v>5.81</v>
       </c>
       <c r="E2">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="F2" t="s">
         <v>6</v>
@@ -729,19 +726,19 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="2">
-        <v>45334</v>
+        <v>45335</v>
       </c>
       <c r="B3">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C3">
-        <v>66.02</v>
+        <v>95.70999999999999</v>
       </c>
       <c r="D3">
-        <v>11.32</v>
+        <v>6.14</v>
       </c>
       <c r="E3">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="F3" t="s">
         <v>7</v>
@@ -749,19 +746,19 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="2">
-        <v>45334</v>
+        <v>45335</v>
       </c>
       <c r="B4">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C4">
-        <v>31.49</v>
+        <v>67.26000000000001</v>
       </c>
       <c r="D4">
-        <v>10.63</v>
+        <v>6.07</v>
       </c>
       <c r="E4">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="F4" t="s">
         <v>8</v>
@@ -769,19 +766,19 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="2">
-        <v>45334</v>
+        <v>45335</v>
       </c>
       <c r="B5">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C5">
-        <v>3.4</v>
+        <v>32.55</v>
       </c>
       <c r="D5">
-        <v>9.9</v>
+        <v>5.75</v>
       </c>
       <c r="E5">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="F5" t="s">
         <v>9</v>
@@ -789,19 +786,19 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="2">
-        <v>45334</v>
+        <v>45335</v>
       </c>
       <c r="B6">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>3.76</v>
       </c>
       <c r="D6">
-        <v>9.18</v>
+        <v>5.36</v>
       </c>
       <c r="E6">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="F6" t="s">
         <v>10</v>
@@ -809,16 +806,16 @@
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="2">
-        <v>45334</v>
+        <v>45335</v>
       </c>
       <c r="B7">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C7">
         <v>0</v>
       </c>
       <c r="D7">
-        <v>9.039999999999999</v>
+        <v>5.08</v>
       </c>
       <c r="E7">
         <v>100</v>
@@ -829,16 +826,16 @@
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="2">
-        <v>45334</v>
+        <v>45335</v>
       </c>
       <c r="B8">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C8">
         <v>0</v>
       </c>
       <c r="D8">
-        <v>8.9</v>
+        <v>4.82</v>
       </c>
       <c r="E8">
         <v>100</v>
@@ -849,16 +846,16 @@
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="2">
-        <v>45334</v>
+        <v>45335</v>
       </c>
       <c r="B9">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C9">
         <v>0</v>
       </c>
       <c r="D9">
-        <v>8.42</v>
+        <v>4.59</v>
       </c>
       <c r="E9">
         <v>100</v>
@@ -869,16 +866,16 @@
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="2">
-        <v>45334</v>
+        <v>45335</v>
       </c>
       <c r="B10">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C10">
         <v>0</v>
       </c>
       <c r="D10">
-        <v>8.42</v>
+        <v>4.4</v>
       </c>
       <c r="E10">
         <v>100</v>
@@ -889,16 +886,16 @@
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="2">
-        <v>45334</v>
+        <v>45335</v>
       </c>
       <c r="B11">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C11">
         <v>0</v>
       </c>
       <c r="D11">
-        <v>8.27</v>
+        <v>3.77</v>
       </c>
       <c r="E11">
         <v>100</v>
@@ -912,13 +909,13 @@
         <v>45335</v>
       </c>
       <c r="B12">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="C12">
         <v>0</v>
       </c>
       <c r="D12">
-        <v>8.109999999999999</v>
+        <v>3.26</v>
       </c>
       <c r="E12">
         <v>100</v>
@@ -929,16 +926,16 @@
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="2">
-        <v>45335</v>
+        <v>45336</v>
       </c>
       <c r="B13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C13">
         <v>0</v>
       </c>
       <c r="D13">
-        <v>7.96</v>
+        <v>3.11</v>
       </c>
       <c r="E13">
         <v>100</v>
@@ -949,16 +946,16 @@
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="2">
-        <v>45335</v>
+        <v>45336</v>
       </c>
       <c r="B14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C14">
         <v>0</v>
       </c>
       <c r="D14">
-        <v>7.83</v>
+        <v>2.99</v>
       </c>
       <c r="E14">
         <v>100</v>
@@ -969,16 +966,16 @@
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="2">
-        <v>45335</v>
+        <v>45336</v>
       </c>
       <c r="B15">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C15">
         <v>0</v>
       </c>
       <c r="D15">
-        <v>7.65</v>
+        <v>2.75</v>
       </c>
       <c r="E15">
         <v>100</v>
@@ -989,16 +986,16 @@
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="2">
-        <v>45335</v>
+        <v>45336</v>
       </c>
       <c r="B16">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C16">
         <v>0</v>
       </c>
       <c r="D16">
-        <v>7.47</v>
+        <v>2.69</v>
       </c>
       <c r="E16">
         <v>100</v>
@@ -1009,16 +1006,16 @@
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="2">
-        <v>45335</v>
+        <v>45336</v>
       </c>
       <c r="B17">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C17">
         <v>0</v>
       </c>
       <c r="D17">
-        <v>7.25</v>
+        <v>2.62</v>
       </c>
       <c r="E17">
         <v>100</v>
@@ -1029,16 +1026,16 @@
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="2">
-        <v>45335</v>
+        <v>45336</v>
       </c>
       <c r="B18">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C18">
         <v>0</v>
       </c>
       <c r="D18">
-        <v>7.14</v>
+        <v>2.39</v>
       </c>
       <c r="E18">
         <v>100</v>
@@ -1049,16 +1046,16 @@
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="2">
-        <v>45335</v>
+        <v>45336</v>
       </c>
       <c r="B19">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C19">
-        <v>1.54</v>
+        <v>0</v>
       </c>
       <c r="D19">
-        <v>7.09</v>
+        <v>2.39</v>
       </c>
       <c r="E19">
         <v>100</v>
@@ -1069,19 +1066,19 @@
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="2">
-        <v>45335</v>
+        <v>45336</v>
       </c>
       <c r="B20">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C20">
-        <v>26.02</v>
+        <v>1.81</v>
       </c>
       <c r="D20">
-        <v>6.89</v>
+        <v>3.14</v>
       </c>
       <c r="E20">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F20" t="s">
         <v>24</v>
@@ -1089,16 +1086,16 @@
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="2">
-        <v>45335</v>
+        <v>45336</v>
       </c>
       <c r="B21">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C21">
-        <v>61.12</v>
+        <v>28.08</v>
       </c>
       <c r="D21">
-        <v>6.86</v>
+        <v>3.79</v>
       </c>
       <c r="E21">
         <v>100</v>
@@ -1109,16 +1106,16 @@
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="2">
-        <v>45335</v>
+        <v>45336</v>
       </c>
       <c r="B22">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C22">
-        <v>91.14</v>
+        <v>66.31</v>
       </c>
       <c r="D22">
-        <v>7.01</v>
+        <v>4.72</v>
       </c>
       <c r="E22">
         <v>100</v>
@@ -1129,16 +1126,16 @@
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="2">
-        <v>45335</v>
+        <v>45336</v>
       </c>
       <c r="B23">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C23">
-        <v>111.28</v>
+        <v>95.81</v>
       </c>
       <c r="D23">
-        <v>7.01</v>
+        <v>5.55</v>
       </c>
       <c r="E23">
         <v>100</v>
@@ -1149,16 +1146,16 @@
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="2">
-        <v>45335</v>
+        <v>45336</v>
       </c>
       <c r="B24">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C24">
-        <v>119.09</v>
+        <v>115.85</v>
       </c>
       <c r="D24">
-        <v>7.19</v>
+        <v>6.2</v>
       </c>
       <c r="E24">
         <v>100</v>
@@ -1169,16 +1166,16 @@
     </row>
     <row r="25" spans="1:6">
       <c r="A25" s="2">
-        <v>45335</v>
+        <v>45336</v>
       </c>
       <c r="B25">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C25">
-        <v>113.7</v>
+        <v>123.98</v>
       </c>
       <c r="D25">
-        <v>7.47</v>
+        <v>6.53</v>
       </c>
       <c r="E25">
         <v>100</v>
@@ -1189,16 +1186,16 @@
     </row>
     <row r="26" spans="1:6">
       <c r="A26" s="2">
-        <v>45335</v>
+        <v>45336</v>
       </c>
       <c r="B26">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C26">
-        <v>95.70999999999999</v>
+        <v>118.87</v>
       </c>
       <c r="D26">
-        <v>7.48</v>
+        <v>6.52</v>
       </c>
       <c r="E26">
         <v>100</v>
@@ -1209,16 +1206,16 @@
     </row>
     <row r="27" spans="1:6">
       <c r="A27" s="2">
-        <v>45335</v>
+        <v>45336</v>
       </c>
       <c r="B27">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C27">
-        <v>67.26000000000001</v>
+        <v>99.16</v>
       </c>
       <c r="D27">
-        <v>6.91</v>
+        <v>6.37</v>
       </c>
       <c r="E27">
         <v>100</v>
@@ -1229,19 +1226,19 @@
     </row>
     <row r="28" spans="1:6">
       <c r="A28" s="2">
-        <v>45335</v>
+        <v>45336</v>
       </c>
       <c r="B28">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C28">
-        <v>32.55</v>
+        <v>68.48</v>
       </c>
       <c r="D28">
-        <v>5.97</v>
+        <v>5.89</v>
       </c>
       <c r="E28">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F28" t="s">
         <v>32</v>
@@ -1249,19 +1246,19 @@
     </row>
     <row r="29" spans="1:6">
       <c r="A29" s="2">
-        <v>45335</v>
+        <v>45336</v>
       </c>
       <c r="B29">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C29">
-        <v>3.76</v>
+        <v>35.03</v>
       </c>
       <c r="D29">
-        <v>5.27</v>
+        <v>4.47</v>
       </c>
       <c r="E29">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="F29" t="s">
         <v>33</v>
@@ -1269,19 +1266,19 @@
     </row>
     <row r="30" spans="1:6">
       <c r="A30" s="2">
-        <v>45335</v>
+        <v>45336</v>
       </c>
       <c r="B30">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C30">
-        <v>0</v>
+        <v>4.83</v>
       </c>
       <c r="D30">
-        <v>4.74</v>
+        <v>3.32</v>
       </c>
       <c r="E30">
-        <v>100</v>
+        <v>85</v>
       </c>
       <c r="F30" t="s">
         <v>34</v>
@@ -1289,19 +1286,19 @@
     </row>
     <row r="31" spans="1:6">
       <c r="A31" s="2">
-        <v>45335</v>
+        <v>45336</v>
       </c>
       <c r="B31">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C31">
         <v>0</v>
       </c>
       <c r="D31">
-        <v>4.45</v>
+        <v>2.57</v>
       </c>
       <c r="E31">
-        <v>100</v>
+        <v>79</v>
       </c>
       <c r="F31" t="s">
         <v>35</v>
@@ -1309,19 +1306,19 @@
     </row>
     <row r="32" spans="1:6">
       <c r="A32" s="2">
-        <v>45335</v>
+        <v>45336</v>
       </c>
       <c r="B32">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C32">
         <v>0</v>
       </c>
       <c r="D32">
-        <v>4.26</v>
+        <v>2.13</v>
       </c>
       <c r="E32">
-        <v>100</v>
+        <v>73</v>
       </c>
       <c r="F32" t="s">
         <v>36</v>
@@ -1329,19 +1326,19 @@
     </row>
     <row r="33" spans="1:6">
       <c r="A33" s="2">
-        <v>45335</v>
+        <v>45336</v>
       </c>
       <c r="B33">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C33">
         <v>0</v>
       </c>
       <c r="D33">
-        <v>4.08</v>
+        <v>1.85</v>
       </c>
       <c r="E33">
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="F33" t="s">
         <v>37</v>
@@ -1349,19 +1346,19 @@
     </row>
     <row r="34" spans="1:6">
       <c r="A34" s="2">
-        <v>45335</v>
+        <v>45336</v>
       </c>
       <c r="B34">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C34">
         <v>0</v>
       </c>
       <c r="D34">
-        <v>3.8</v>
+        <v>1.47</v>
       </c>
       <c r="E34">
-        <v>100</v>
+        <v>59</v>
       </c>
       <c r="F34" t="s">
         <v>38</v>
@@ -1369,19 +1366,19 @@
     </row>
     <row r="35" spans="1:6">
       <c r="A35" s="2">
-        <v>45335</v>
+        <v>45336</v>
       </c>
       <c r="B35">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C35">
         <v>0</v>
       </c>
       <c r="D35">
-        <v>3.75</v>
+        <v>1.31</v>
       </c>
       <c r="E35">
-        <v>100</v>
+        <v>59</v>
       </c>
       <c r="F35" t="s">
         <v>39</v>
@@ -1392,16 +1389,16 @@
         <v>45336</v>
       </c>
       <c r="B36">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="C36">
         <v>0</v>
       </c>
       <c r="D36">
-        <v>3.66</v>
+        <v>1.24</v>
       </c>
       <c r="E36">
-        <v>100</v>
+        <v>61</v>
       </c>
       <c r="F36" t="s">
         <v>40</v>
@@ -1409,19 +1406,19 @@
     </row>
     <row r="37" spans="1:6">
       <c r="A37" s="2">
-        <v>45336</v>
+        <v>45337</v>
       </c>
       <c r="B37">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C37">
         <v>0</v>
       </c>
       <c r="D37">
-        <v>3.49</v>
+        <v>1.25</v>
       </c>
       <c r="E37">
-        <v>100</v>
+        <v>63</v>
       </c>
       <c r="F37" t="s">
         <v>41</v>
@@ -1429,19 +1426,19 @@
     </row>
     <row r="38" spans="1:6">
       <c r="A38" s="2">
-        <v>45336</v>
+        <v>45337</v>
       </c>
       <c r="B38">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C38">
         <v>0</v>
       </c>
       <c r="D38">
-        <v>3.17</v>
+        <v>0.88</v>
       </c>
       <c r="E38">
-        <v>99</v>
+        <v>58</v>
       </c>
       <c r="F38" t="s">
         <v>42</v>
@@ -1449,19 +1446,19 @@
     </row>
     <row r="39" spans="1:6">
       <c r="A39" s="2">
-        <v>45336</v>
+        <v>45337</v>
       </c>
       <c r="B39">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C39">
         <v>0</v>
       </c>
       <c r="D39">
-        <v>2.79</v>
+        <v>0.71</v>
       </c>
       <c r="E39">
-        <v>99</v>
+        <v>44</v>
       </c>
       <c r="F39" t="s">
         <v>43</v>
@@ -1469,19 +1466,19 @@
     </row>
     <row r="40" spans="1:6">
       <c r="A40" s="2">
-        <v>45336</v>
+        <v>45337</v>
       </c>
       <c r="B40">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C40">
         <v>0</v>
       </c>
       <c r="D40">
-        <v>2.57</v>
+        <v>0.64</v>
       </c>
       <c r="E40">
-        <v>99</v>
+        <v>37</v>
       </c>
       <c r="F40" t="s">
         <v>44</v>
@@ -1489,19 +1486,19 @@
     </row>
     <row r="41" spans="1:6">
       <c r="A41" s="2">
-        <v>45336</v>
+        <v>45337</v>
       </c>
       <c r="B41">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C41">
         <v>0</v>
       </c>
       <c r="D41">
-        <v>2.3</v>
+        <v>0.61</v>
       </c>
       <c r="E41">
-        <v>99</v>
+        <v>33</v>
       </c>
       <c r="F41" t="s">
         <v>45</v>
@@ -1509,19 +1506,19 @@
     </row>
     <row r="42" spans="1:6">
       <c r="A42" s="2">
-        <v>45336</v>
+        <v>45337</v>
       </c>
       <c r="B42">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C42">
         <v>0</v>
       </c>
       <c r="D42">
-        <v>2.4</v>
+        <v>0.61</v>
       </c>
       <c r="E42">
-        <v>99</v>
+        <v>31</v>
       </c>
       <c r="F42" t="s">
         <v>46</v>
@@ -1529,19 +1526,19 @@
     </row>
     <row r="43" spans="1:6">
       <c r="A43" s="2">
-        <v>45336</v>
+        <v>45337</v>
       </c>
       <c r="B43">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C43">
-        <v>1.96</v>
+        <v>0</v>
       </c>
       <c r="D43">
-        <v>3.46</v>
+        <v>0.93</v>
       </c>
       <c r="E43">
-        <v>100</v>
+        <v>28</v>
       </c>
       <c r="F43" t="s">
         <v>47</v>
@@ -1549,19 +1546,19 @@
     </row>
     <row r="44" spans="1:6">
       <c r="A44" s="2">
-        <v>45336</v>
+        <v>45337</v>
       </c>
       <c r="B44">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C44">
-        <v>28.7</v>
+        <v>8.34</v>
       </c>
       <c r="D44">
-        <v>4.39</v>
+        <v>2.55</v>
       </c>
       <c r="E44">
-        <v>100</v>
+        <v>17</v>
       </c>
       <c r="F44" t="s">
         <v>48</v>
@@ -1569,19 +1566,19 @@
     </row>
     <row r="45" spans="1:6">
       <c r="A45" s="2">
-        <v>45336</v>
+        <v>45337</v>
       </c>
       <c r="B45">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C45">
-        <v>63.97</v>
+        <v>111.86</v>
       </c>
       <c r="D45">
-        <v>5.26</v>
+        <v>4.13</v>
       </c>
       <c r="E45">
-        <v>100</v>
+        <v>15</v>
       </c>
       <c r="F45" t="s">
         <v>49</v>
@@ -1589,19 +1586,19 @@
     </row>
     <row r="46" spans="1:6">
       <c r="A46" s="2">
-        <v>45336</v>
+        <v>45337</v>
       </c>
       <c r="B46">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C46">
-        <v>94.34999999999999</v>
+        <v>254.06</v>
       </c>
       <c r="D46">
-        <v>6.03</v>
+        <v>5.41</v>
       </c>
       <c r="E46">
-        <v>100</v>
+        <v>14</v>
       </c>
       <c r="F46" t="s">
         <v>50</v>
@@ -1609,19 +1606,19 @@
     </row>
     <row r="47" spans="1:6">
       <c r="A47" s="2">
-        <v>45336</v>
+        <v>45337</v>
       </c>
       <c r="B47">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C47">
-        <v>115.36</v>
+        <v>374.87</v>
       </c>
       <c r="D47">
-        <v>6.61</v>
+        <v>6.22</v>
       </c>
       <c r="E47">
-        <v>100</v>
+        <v>13</v>
       </c>
       <c r="F47" t="s">
         <v>51</v>
@@ -1629,19 +1626,19 @@
     </row>
     <row r="48" spans="1:6">
       <c r="A48" s="2">
-        <v>45336</v>
+        <v>45337</v>
       </c>
       <c r="B48">
+        <v>11</v>
+      </c>
+      <c r="C48">
+        <v>455.85</v>
+      </c>
+      <c r="D48">
+        <v>6.72</v>
+      </c>
+      <c r="E48">
         <v>12</v>
-      </c>
-      <c r="C48">
-        <v>123.66</v>
-      </c>
-      <c r="D48">
-        <v>7.09</v>
-      </c>
-      <c r="E48">
-        <v>100</v>
       </c>
       <c r="F48" t="s">
         <v>52</v>
@@ -1649,19 +1646,19 @@
     </row>
     <row r="49" spans="1:6">
       <c r="A49" s="2">
-        <v>45336</v>
+        <v>45337</v>
       </c>
       <c r="B49">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C49">
-        <v>118.98</v>
+        <v>487.28</v>
       </c>
       <c r="D49">
-        <v>7.19</v>
+        <v>6.96</v>
       </c>
       <c r="E49">
-        <v>99</v>
+        <v>12</v>
       </c>
       <c r="F49" t="s">
         <v>53</v>
@@ -1669,202 +1666,148 @@
     </row>
     <row r="50" spans="1:6">
       <c r="A50" s="2">
-        <v>45336</v>
+        <v>45337</v>
       </c>
       <c r="B50">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C50">
-        <v>103.58</v>
+        <v>487.28</v>
       </c>
       <c r="D50">
-        <v>6.99</v>
+        <v>6.96</v>
       </c>
       <c r="E50">
-        <v>94</v>
+        <v>12</v>
       </c>
       <c r="F50" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="51" spans="1:6">
       <c r="A51" s="2">
-        <v>45336</v>
+        <v>45337</v>
       </c>
       <c r="B51">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C51">
-        <v>86.95</v>
-      </c>
-      <c r="D51">
-        <v>5.91</v>
-      </c>
-      <c r="E51">
-        <v>87</v>
+        <v>465.63</v>
       </c>
       <c r="F51" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="52" spans="1:6">
       <c r="A52" s="2">
-        <v>45336</v>
+        <v>45337</v>
       </c>
       <c r="B52">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C52">
-        <v>58.21</v>
-      </c>
-      <c r="D52">
-        <v>4.22</v>
-      </c>
-      <c r="E52">
-        <v>90</v>
+        <v>392.43</v>
       </c>
       <c r="F52" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="53" spans="1:6">
       <c r="A53" s="2">
-        <v>45336</v>
+        <v>45337</v>
       </c>
       <c r="B53">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C53">
-        <v>8.779999999999999</v>
-      </c>
-      <c r="D53">
-        <v>3.24</v>
-      </c>
-      <c r="E53">
-        <v>92</v>
+        <v>275.97</v>
       </c>
       <c r="F53" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="54" spans="1:6">
       <c r="A54" s="2">
-        <v>45336</v>
+        <v>45337</v>
       </c>
       <c r="B54">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C54">
-        <v>0</v>
-      </c>
-      <c r="D54">
-        <v>2.55</v>
-      </c>
-      <c r="E54">
-        <v>91</v>
+        <v>137.13</v>
       </c>
       <c r="F54" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="55" spans="1:6">
       <c r="A55" s="2">
-        <v>45336</v>
+        <v>45337</v>
       </c>
       <c r="B55">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C55">
-        <v>0</v>
-      </c>
-      <c r="D55">
-        <v>2.03</v>
-      </c>
-      <c r="E55">
-        <v>68</v>
+        <v>17.85</v>
       </c>
       <c r="F55" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="56" spans="1:6">
       <c r="A56" s="2">
-        <v>45336</v>
+        <v>45337</v>
       </c>
       <c r="B56">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C56">
         <v>0</v>
       </c>
-      <c r="D56">
-        <v>1.53</v>
-      </c>
-      <c r="E56">
-        <v>62</v>
-      </c>
       <c r="F56" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="57" spans="1:6">
       <c r="A57" s="2">
-        <v>45336</v>
+        <v>45337</v>
       </c>
       <c r="B57">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C57">
         <v>0</v>
       </c>
-      <c r="D57">
-        <v>1.08</v>
-      </c>
-      <c r="E57">
-        <v>49</v>
-      </c>
       <c r="F57" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="58" spans="1:6">
       <c r="A58" s="2">
-        <v>45336</v>
+        <v>45337</v>
       </c>
       <c r="B58">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C58">
         <v>0</v>
       </c>
-      <c r="D58">
-        <v>0.76</v>
-      </c>
-      <c r="E58">
-        <v>42</v>
-      </c>
       <c r="F58" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="59" spans="1:6">
       <c r="A59" s="2">
-        <v>45336</v>
+        <v>45337</v>
       </c>
       <c r="B59">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C59">
         <v>0</v>
       </c>
-      <c r="D59">
-        <v>0.5600000000000001</v>
-      </c>
-      <c r="E59">
-        <v>38</v>
-      </c>
       <c r="F59" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="60" spans="1:6">
@@ -1872,19 +1815,13 @@
         <v>45337</v>
       </c>
       <c r="B60">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="C60">
         <v>0</v>
       </c>
-      <c r="D60">
-        <v>0.47</v>
-      </c>
-      <c r="E60">
-        <v>35</v>
-      </c>
       <c r="F60" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="61" spans="1:6">
@@ -1892,459 +1829,321 @@
         <v>45337</v>
       </c>
       <c r="B61">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="C61">
         <v>0</v>
       </c>
-      <c r="D61">
-        <v>0.38</v>
-      </c>
-      <c r="E61">
-        <v>24</v>
-      </c>
       <c r="F61" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="62" spans="1:6">
       <c r="A62" s="2">
-        <v>45337</v>
+        <v>45338</v>
       </c>
       <c r="B62">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C62">
         <v>0</v>
       </c>
-      <c r="D62">
-        <v>0.33</v>
-      </c>
-      <c r="E62">
-        <v>23</v>
-      </c>
       <c r="F62" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="63" spans="1:6">
       <c r="A63" s="2">
-        <v>45337</v>
+        <v>45338</v>
       </c>
       <c r="B63">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C63">
         <v>0</v>
       </c>
-      <c r="D63">
-        <v>0.31</v>
-      </c>
-      <c r="E63">
-        <v>29</v>
-      </c>
       <c r="F63" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="64" spans="1:6">
       <c r="A64" s="2">
-        <v>45337</v>
+        <v>45338</v>
       </c>
       <c r="B64">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C64">
         <v>0</v>
       </c>
-      <c r="D64">
-        <v>0.36</v>
-      </c>
-      <c r="E64">
-        <v>41</v>
-      </c>
       <c r="F64" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="65" spans="1:6">
       <c r="A65" s="2">
-        <v>45337</v>
+        <v>45338</v>
       </c>
       <c r="B65">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C65">
         <v>0</v>
       </c>
-      <c r="D65">
-        <v>0.32</v>
-      </c>
-      <c r="E65">
-        <v>47</v>
-      </c>
       <c r="F65" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="66" spans="1:6">
       <c r="A66" s="2">
-        <v>45337</v>
+        <v>45338</v>
       </c>
       <c r="B66">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C66">
         <v>0</v>
       </c>
-      <c r="D66">
-        <v>0.68</v>
-      </c>
-      <c r="E66">
-        <v>52</v>
-      </c>
       <c r="F66" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="67" spans="1:6">
       <c r="A67" s="2">
-        <v>45337</v>
+        <v>45338</v>
       </c>
       <c r="B67">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C67">
-        <v>7.81</v>
-      </c>
-      <c r="D67">
-        <v>2.26</v>
-      </c>
-      <c r="E67">
-        <v>51</v>
+        <v>0</v>
       </c>
       <c r="F67" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="68" spans="1:6">
       <c r="A68" s="2">
-        <v>45337</v>
+        <v>45338</v>
       </c>
       <c r="B68">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C68">
-        <v>103.7</v>
-      </c>
-      <c r="D68">
-        <v>3.92</v>
-      </c>
-      <c r="E68">
-        <v>33</v>
+        <v>0</v>
       </c>
       <c r="F68" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="69" spans="1:6">
       <c r="A69" s="2">
-        <v>45337</v>
+        <v>45338</v>
       </c>
       <c r="B69">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C69">
-        <v>242.85</v>
-      </c>
-      <c r="D69">
-        <v>5.22</v>
-      </c>
-      <c r="E69">
-        <v>25</v>
+        <v>9.74</v>
       </c>
       <c r="F69" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="70" spans="1:6">
       <c r="A70" s="2">
-        <v>45337</v>
+        <v>45338</v>
       </c>
       <c r="B70">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C70">
-        <v>370.55</v>
-      </c>
-      <c r="D70">
-        <v>5.87</v>
-      </c>
-      <c r="E70">
-        <v>22</v>
+        <v>116.88</v>
       </c>
       <c r="F70" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="71" spans="1:6">
       <c r="A71" s="2">
-        <v>45337</v>
+        <v>45338</v>
       </c>
       <c r="B71">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C71">
-        <v>453.5</v>
-      </c>
-      <c r="D71">
-        <v>6.3</v>
-      </c>
-      <c r="E71">
-        <v>19</v>
+        <v>259.58</v>
       </c>
       <c r="F71" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="72" spans="1:6">
       <c r="A72" s="2">
-        <v>45337</v>
+        <v>45338</v>
       </c>
       <c r="B72">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C72">
-        <v>485.87</v>
-      </c>
-      <c r="D72">
-        <v>6.5</v>
-      </c>
-      <c r="E72">
-        <v>18</v>
+        <v>380.66</v>
       </c>
       <c r="F72" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="73" spans="1:6">
       <c r="A73" s="2">
-        <v>45337</v>
+        <v>45338</v>
       </c>
       <c r="B73">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C73">
-        <v>464.75</v>
-      </c>
-      <c r="D73">
-        <v>6.43</v>
-      </c>
-      <c r="E73">
-        <v>33</v>
+        <v>461.51</v>
       </c>
       <c r="F73" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="74" spans="1:6">
       <c r="A74" s="2">
-        <v>45337</v>
+        <v>45338</v>
       </c>
       <c r="B74">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C74">
-        <v>391.1</v>
-      </c>
-      <c r="D74">
-        <v>6.08</v>
-      </c>
-      <c r="E74">
-        <v>25</v>
+        <v>492.89</v>
       </c>
       <c r="F74" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="75" spans="1:6">
       <c r="A75" s="2">
-        <v>45337</v>
+        <v>45338</v>
       </c>
       <c r="B75">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C75">
-        <v>275.22</v>
-      </c>
-      <c r="D75">
-        <v>4.64</v>
-      </c>
-      <c r="E75">
-        <v>22</v>
+        <v>471.25</v>
       </c>
       <c r="F75" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="76" spans="1:6">
       <c r="A76" s="2">
-        <v>45337</v>
+        <v>45338</v>
       </c>
       <c r="B76">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C76">
-        <v>137.98</v>
-      </c>
-      <c r="D76">
-        <v>2.73</v>
-      </c>
-      <c r="E76">
-        <v>18</v>
+        <v>398.87</v>
       </c>
       <c r="F76" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="77" spans="1:6">
       <c r="A77" s="2">
-        <v>45337</v>
+        <v>45338</v>
       </c>
       <c r="B77">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C77">
-        <v>18.03</v>
-      </c>
-      <c r="D77">
-        <v>2.16</v>
-      </c>
-      <c r="E77">
-        <v>14</v>
+        <v>284.12</v>
       </c>
       <c r="F77" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="78" spans="1:6">
       <c r="A78" s="2">
-        <v>45337</v>
+        <v>45338</v>
       </c>
       <c r="B78">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C78">
-        <v>0</v>
-      </c>
-      <c r="D78">
-        <v>1.77</v>
-      </c>
-      <c r="E78">
-        <v>12</v>
+        <v>143.28</v>
       </c>
       <c r="F78" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="79" spans="1:6">
       <c r="A79" s="2">
-        <v>45337</v>
+        <v>45338</v>
       </c>
       <c r="B79">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C79">
-        <v>0</v>
-      </c>
-      <c r="D79">
-        <v>1.45</v>
-      </c>
-      <c r="E79">
-        <v>0</v>
+        <v>20.45</v>
       </c>
       <c r="F79" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="80" spans="1:6">
       <c r="A80" s="2">
-        <v>45337</v>
+        <v>45338</v>
       </c>
       <c r="B80">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C80">
         <v>0</v>
       </c>
-      <c r="D80">
-        <v>1.29</v>
-      </c>
-      <c r="E80">
-        <v>0</v>
-      </c>
       <c r="F80" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="81" spans="1:6">
       <c r="A81" s="2">
-        <v>45337</v>
+        <v>45338</v>
       </c>
       <c r="B81">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C81">
         <v>0</v>
       </c>
-      <c r="D81">
-        <v>1.17</v>
-      </c>
-      <c r="E81">
-        <v>0</v>
-      </c>
       <c r="F81" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="82" spans="1:6">
       <c r="A82" s="2">
-        <v>45337</v>
+        <v>45338</v>
       </c>
       <c r="B82">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C82">
         <v>0</v>
       </c>
-      <c r="D82">
-        <v>1.1</v>
-      </c>
-      <c r="E82">
-        <v>1</v>
-      </c>
       <c r="F82" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="83" spans="1:6">
       <c r="A83" s="2">
-        <v>45337</v>
+        <v>45338</v>
       </c>
       <c r="B83">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C83">
         <v>0</v>
       </c>
-      <c r="D83">
-        <v>1.02</v>
-      </c>
-      <c r="E83">
-        <v>2</v>
-      </c>
       <c r="F83" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="84" spans="1:6">
@@ -2352,16 +2151,13 @@
         <v>45338</v>
       </c>
       <c r="B84">
-        <v>0</v>
-      </c>
-      <c r="D84">
-        <v>0.9399999999999999</v>
-      </c>
-      <c r="E84">
-        <v>2</v>
+        <v>22</v>
+      </c>
+      <c r="C84">
+        <v>0</v>
       </c>
       <c r="F84" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="85" spans="1:6">
@@ -2369,220 +2165,181 @@
         <v>45338</v>
       </c>
       <c r="B85">
-        <v>1</v>
-      </c>
-      <c r="D85">
-        <v>0.84</v>
-      </c>
-      <c r="E85">
-        <v>6</v>
+        <v>23</v>
+      </c>
+      <c r="C85">
+        <v>0</v>
       </c>
       <c r="F85" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="86" spans="1:6">
       <c r="A86" s="2">
-        <v>45338</v>
+        <v>45339</v>
       </c>
       <c r="B86">
-        <v>2</v>
-      </c>
-      <c r="D86">
-        <v>0.77</v>
-      </c>
-      <c r="E86">
-        <v>5</v>
+        <v>0</v>
+      </c>
+      <c r="C86">
+        <v>0</v>
       </c>
       <c r="F86" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="87" spans="1:6">
       <c r="A87" s="2">
-        <v>45338</v>
+        <v>45339</v>
       </c>
       <c r="B87">
-        <v>3</v>
-      </c>
-      <c r="D87">
-        <v>0.7</v>
-      </c>
-      <c r="E87">
-        <v>4</v>
+        <v>1</v>
+      </c>
+      <c r="C87">
+        <v>0</v>
       </c>
       <c r="F87" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="88" spans="1:6">
       <c r="A88" s="2">
-        <v>45338</v>
+        <v>45339</v>
       </c>
       <c r="B88">
-        <v>4</v>
-      </c>
-      <c r="D88">
-        <v>0.6</v>
-      </c>
-      <c r="E88">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="C88">
+        <v>0</v>
       </c>
       <c r="F88" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="89" spans="1:6">
       <c r="A89" s="2">
-        <v>45338</v>
+        <v>45339</v>
       </c>
       <c r="B89">
-        <v>5</v>
-      </c>
-      <c r="D89">
-        <v>0.54</v>
-      </c>
-      <c r="E89">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="C89">
+        <v>0</v>
       </c>
       <c r="F89" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="90" spans="1:6">
       <c r="A90" s="2">
-        <v>45338</v>
+        <v>45339</v>
       </c>
       <c r="B90">
-        <v>6</v>
-      </c>
-      <c r="D90">
-        <v>0.87</v>
-      </c>
-      <c r="E90">
-        <v>2</v>
+        <v>4</v>
+      </c>
+      <c r="C90">
+        <v>0</v>
       </c>
       <c r="F90" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="91" spans="1:6">
       <c r="A91" s="2">
-        <v>45338</v>
+        <v>45339</v>
       </c>
       <c r="B91">
-        <v>7</v>
-      </c>
-      <c r="D91">
-        <v>2.8</v>
-      </c>
-      <c r="E91">
+        <v>5</v>
+      </c>
+      <c r="C91">
         <v>0</v>
       </c>
       <c r="F91" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="92" spans="1:6">
       <c r="A92" s="2">
-        <v>45338</v>
+        <v>45339</v>
       </c>
       <c r="B92">
-        <v>8</v>
-      </c>
-      <c r="D92">
-        <v>4.63</v>
-      </c>
-      <c r="E92">
+        <v>6</v>
+      </c>
+      <c r="C92">
         <v>0</v>
       </c>
       <c r="F92" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="93" spans="1:6">
       <c r="A93" s="2">
-        <v>45338</v>
+        <v>45339</v>
       </c>
       <c r="B93">
-        <v>9</v>
-      </c>
-      <c r="D93">
-        <v>6.02</v>
-      </c>
-      <c r="E93">
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="C93">
+        <v>11.15</v>
       </c>
       <c r="F93" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="94" spans="1:6">
       <c r="A94" s="2">
-        <v>45338</v>
+        <v>45339</v>
       </c>
       <c r="B94">
-        <v>10</v>
-      </c>
-      <c r="D94">
-        <v>6.94</v>
-      </c>
-      <c r="E94">
-        <v>0</v>
+        <v>8</v>
+      </c>
+      <c r="C94">
+        <v>121.51</v>
       </c>
       <c r="F94" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="95" spans="1:6">
       <c r="A95" s="2">
-        <v>45338</v>
+        <v>45339</v>
       </c>
       <c r="B95">
-        <v>11</v>
-      </c>
-      <c r="D95">
-        <v>7.49</v>
-      </c>
-      <c r="E95">
-        <v>0</v>
+        <v>9</v>
+      </c>
+      <c r="C95">
+        <v>265.09</v>
       </c>
       <c r="F95" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="96" spans="1:6">
       <c r="A96" s="2">
-        <v>45338</v>
+        <v>45339</v>
       </c>
       <c r="B96">
-        <v>12</v>
-      </c>
-      <c r="D96">
-        <v>7.72</v>
-      </c>
-      <c r="E96">
-        <v>0</v>
+        <v>10</v>
+      </c>
+      <c r="C96">
+        <v>386.67</v>
       </c>
       <c r="F96" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="97" spans="1:6">
       <c r="A97" s="2">
-        <v>45338</v>
+        <v>45339</v>
       </c>
       <c r="B97">
-        <v>13</v>
-      </c>
-      <c r="D97">
-        <v>7.63</v>
-      </c>
-      <c r="E97">
-        <v>0</v>
+        <v>11</v>
+      </c>
+      <c r="C97">
+        <v>467.97</v>
       </c>
       <c r="F97" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Aligning the prediction values to the dates and intervals
</commit_message>
<xml_diff>
--- a/RAAL/Production/Input.xlsx
+++ b/RAAL/Production/Input.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="102">
   <si>
     <t>Data</t>
   </si>
@@ -34,289 +34,292 @@
     <t>Lookup</t>
   </si>
   <si>
-    <t>13.02.202413</t>
-  </si>
-  <si>
-    <t>13.02.202414</t>
-  </si>
-  <si>
-    <t>13.02.202415</t>
-  </si>
-  <si>
-    <t>13.02.202416</t>
-  </si>
-  <si>
-    <t>13.02.202417</t>
-  </si>
-  <si>
-    <t>13.02.202418</t>
-  </si>
-  <si>
-    <t>13.02.202419</t>
-  </si>
-  <si>
-    <t>13.02.202420</t>
-  </si>
-  <si>
-    <t>13.02.202421</t>
-  </si>
-  <si>
-    <t>13.02.202422</t>
-  </si>
-  <si>
-    <t>13.02.202423</t>
-  </si>
-  <si>
-    <t>14.02.20240</t>
-  </si>
-  <si>
-    <t>14.02.20241</t>
-  </si>
-  <si>
-    <t>14.02.20242</t>
-  </si>
-  <si>
-    <t>14.02.20243</t>
-  </si>
-  <si>
-    <t>14.02.20244</t>
-  </si>
-  <si>
-    <t>14.02.20245</t>
-  </si>
-  <si>
-    <t>14.02.20246</t>
-  </si>
-  <si>
-    <t>14.02.20247</t>
-  </si>
-  <si>
-    <t>14.02.20248</t>
-  </si>
-  <si>
-    <t>14.02.20249</t>
-  </si>
-  <si>
-    <t>14.02.202410</t>
-  </si>
-  <si>
-    <t>14.02.202411</t>
-  </si>
-  <si>
-    <t>14.02.202412</t>
-  </si>
-  <si>
-    <t>14.02.202413</t>
-  </si>
-  <si>
-    <t>14.02.202414</t>
-  </si>
-  <si>
-    <t>14.02.202415</t>
-  </si>
-  <si>
-    <t>14.02.202416</t>
-  </si>
-  <si>
-    <t>14.02.202417</t>
-  </si>
-  <si>
-    <t>14.02.202418</t>
-  </si>
-  <si>
-    <t>14.02.202419</t>
-  </si>
-  <si>
-    <t>14.02.202420</t>
-  </si>
-  <si>
-    <t>14.02.202421</t>
-  </si>
-  <si>
-    <t>14.02.202422</t>
-  </si>
-  <si>
-    <t>14.02.202423</t>
-  </si>
-  <si>
-    <t>15.02.20240</t>
-  </si>
-  <si>
-    <t>15.02.20241</t>
-  </si>
-  <si>
-    <t>15.02.20242</t>
-  </si>
-  <si>
-    <t>15.02.20243</t>
-  </si>
-  <si>
-    <t>15.02.20244</t>
-  </si>
-  <si>
-    <t>15.02.20245</t>
-  </si>
-  <si>
-    <t>15.02.20246</t>
-  </si>
-  <si>
-    <t>15.02.20247</t>
-  </si>
-  <si>
-    <t>15.02.20248</t>
-  </si>
-  <si>
-    <t>15.02.20249</t>
-  </si>
-  <si>
-    <t>15.02.202410</t>
-  </si>
-  <si>
-    <t>15.02.202411</t>
-  </si>
-  <si>
-    <t>15.02.202412</t>
-  </si>
-  <si>
-    <t>15.02.202413</t>
-  </si>
-  <si>
-    <t>15.02.202414</t>
-  </si>
-  <si>
-    <t>15.02.202415</t>
-  </si>
-  <si>
-    <t>15.02.202416</t>
-  </si>
-  <si>
-    <t>15.02.202417</t>
-  </si>
-  <si>
-    <t>15.02.202418</t>
-  </si>
-  <si>
-    <t>15.02.202419</t>
-  </si>
-  <si>
-    <t>15.02.202420</t>
-  </si>
-  <si>
-    <t>15.02.202421</t>
-  </si>
-  <si>
-    <t>15.02.202422</t>
-  </si>
-  <si>
-    <t>15.02.202423</t>
-  </si>
-  <si>
-    <t>16.02.20240</t>
-  </si>
-  <si>
-    <t>16.02.20241</t>
-  </si>
-  <si>
-    <t>16.02.20242</t>
-  </si>
-  <si>
-    <t>16.02.20243</t>
-  </si>
-  <si>
-    <t>16.02.20244</t>
-  </si>
-  <si>
-    <t>16.02.20245</t>
-  </si>
-  <si>
-    <t>16.02.20246</t>
-  </si>
-  <si>
-    <t>16.02.20247</t>
-  </si>
-  <si>
-    <t>16.02.20248</t>
-  </si>
-  <si>
-    <t>16.02.20249</t>
-  </si>
-  <si>
-    <t>16.02.202410</t>
-  </si>
-  <si>
-    <t>16.02.202411</t>
-  </si>
-  <si>
-    <t>16.02.202412</t>
-  </si>
-  <si>
-    <t>16.02.202413</t>
-  </si>
-  <si>
-    <t>16.02.202414</t>
-  </si>
-  <si>
-    <t>16.02.202415</t>
-  </si>
-  <si>
-    <t>16.02.202416</t>
-  </si>
-  <si>
-    <t>16.02.202417</t>
-  </si>
-  <si>
-    <t>16.02.202418</t>
-  </si>
-  <si>
-    <t>16.02.202419</t>
-  </si>
-  <si>
-    <t>16.02.202420</t>
-  </si>
-  <si>
-    <t>16.02.202421</t>
-  </si>
-  <si>
-    <t>16.02.202422</t>
-  </si>
-  <si>
-    <t>16.02.202423</t>
-  </si>
-  <si>
-    <t>17.02.20240</t>
-  </si>
-  <si>
-    <t>17.02.20241</t>
-  </si>
-  <si>
-    <t>17.02.20242</t>
-  </si>
-  <si>
-    <t>17.02.20243</t>
-  </si>
-  <si>
-    <t>17.02.20244</t>
-  </si>
-  <si>
-    <t>17.02.20245</t>
-  </si>
-  <si>
-    <t>17.02.20246</t>
-  </si>
-  <si>
-    <t>17.02.20247</t>
-  </si>
-  <si>
-    <t>17.02.20248</t>
-  </si>
-  <si>
-    <t>17.02.20249</t>
-  </si>
-  <si>
-    <t>17.02.202410</t>
-  </si>
-  <si>
-    <t>17.02.202411</t>
+    <t>19.02.202415</t>
+  </si>
+  <si>
+    <t>19.02.202416</t>
+  </si>
+  <si>
+    <t>19.02.202417</t>
+  </si>
+  <si>
+    <t>19.02.202418</t>
+  </si>
+  <si>
+    <t>19.02.202419</t>
+  </si>
+  <si>
+    <t>19.02.202420</t>
+  </si>
+  <si>
+    <t>19.02.202421</t>
+  </si>
+  <si>
+    <t>19.02.202422</t>
+  </si>
+  <si>
+    <t>19.02.202423</t>
+  </si>
+  <si>
+    <t>20.02.20240</t>
+  </si>
+  <si>
+    <t>20.02.20241</t>
+  </si>
+  <si>
+    <t>20.02.20242</t>
+  </si>
+  <si>
+    <t>20.02.20243</t>
+  </si>
+  <si>
+    <t>20.02.20244</t>
+  </si>
+  <si>
+    <t>20.02.20245</t>
+  </si>
+  <si>
+    <t>20.02.20246</t>
+  </si>
+  <si>
+    <t>20.02.20247</t>
+  </si>
+  <si>
+    <t>20.02.20248</t>
+  </si>
+  <si>
+    <t>20.02.20249</t>
+  </si>
+  <si>
+    <t>20.02.202410</t>
+  </si>
+  <si>
+    <t>20.02.202411</t>
+  </si>
+  <si>
+    <t>20.02.202412</t>
+  </si>
+  <si>
+    <t>20.02.202413</t>
+  </si>
+  <si>
+    <t>20.02.202414</t>
+  </si>
+  <si>
+    <t>20.02.202415</t>
+  </si>
+  <si>
+    <t>20.02.202416</t>
+  </si>
+  <si>
+    <t>20.02.202417</t>
+  </si>
+  <si>
+    <t>20.02.202418</t>
+  </si>
+  <si>
+    <t>20.02.202419</t>
+  </si>
+  <si>
+    <t>20.02.202420</t>
+  </si>
+  <si>
+    <t>20.02.202421</t>
+  </si>
+  <si>
+    <t>20.02.202422</t>
+  </si>
+  <si>
+    <t>20.02.202423</t>
+  </si>
+  <si>
+    <t>21.02.20240</t>
+  </si>
+  <si>
+    <t>21.02.20241</t>
+  </si>
+  <si>
+    <t>21.02.20242</t>
+  </si>
+  <si>
+    <t>21.02.20243</t>
+  </si>
+  <si>
+    <t>21.02.20244</t>
+  </si>
+  <si>
+    <t>21.02.20245</t>
+  </si>
+  <si>
+    <t>21.02.20246</t>
+  </si>
+  <si>
+    <t>21.02.20247</t>
+  </si>
+  <si>
+    <t>21.02.20248</t>
+  </si>
+  <si>
+    <t>21.02.20249</t>
+  </si>
+  <si>
+    <t>21.02.202410</t>
+  </si>
+  <si>
+    <t>21.02.202411</t>
+  </si>
+  <si>
+    <t>21.02.202412</t>
+  </si>
+  <si>
+    <t>21.02.202413</t>
+  </si>
+  <si>
+    <t>21.02.202414</t>
+  </si>
+  <si>
+    <t>21.02.202415</t>
+  </si>
+  <si>
+    <t>21.02.202416</t>
+  </si>
+  <si>
+    <t>21.02.202417</t>
+  </si>
+  <si>
+    <t>21.02.202418</t>
+  </si>
+  <si>
+    <t>21.02.202419</t>
+  </si>
+  <si>
+    <t>21.02.202420</t>
+  </si>
+  <si>
+    <t>21.02.202421</t>
+  </si>
+  <si>
+    <t>21.02.202422</t>
+  </si>
+  <si>
+    <t>21.02.202423</t>
+  </si>
+  <si>
+    <t>22.02.20240</t>
+  </si>
+  <si>
+    <t>22.02.20241</t>
+  </si>
+  <si>
+    <t>22.02.20242</t>
+  </si>
+  <si>
+    <t>22.02.20243</t>
+  </si>
+  <si>
+    <t>22.02.20244</t>
+  </si>
+  <si>
+    <t>22.02.20245</t>
+  </si>
+  <si>
+    <t>22.02.20246</t>
+  </si>
+  <si>
+    <t>22.02.20247</t>
+  </si>
+  <si>
+    <t>22.02.20248</t>
+  </si>
+  <si>
+    <t>22.02.20249</t>
+  </si>
+  <si>
+    <t>22.02.202410</t>
+  </si>
+  <si>
+    <t>22.02.202411</t>
+  </si>
+  <si>
+    <t>22.02.202412</t>
+  </si>
+  <si>
+    <t>22.02.202413</t>
+  </si>
+  <si>
+    <t>22.02.202414</t>
+  </si>
+  <si>
+    <t>22.02.202415</t>
+  </si>
+  <si>
+    <t>22.02.202416</t>
+  </si>
+  <si>
+    <t>22.02.202417</t>
+  </si>
+  <si>
+    <t>22.02.202418</t>
+  </si>
+  <si>
+    <t>22.02.202419</t>
+  </si>
+  <si>
+    <t>22.02.202420</t>
+  </si>
+  <si>
+    <t>22.02.202421</t>
+  </si>
+  <si>
+    <t>22.02.202422</t>
+  </si>
+  <si>
+    <t>22.02.202423</t>
+  </si>
+  <si>
+    <t>23.02.20240</t>
+  </si>
+  <si>
+    <t>23.02.20241</t>
+  </si>
+  <si>
+    <t>23.02.20242</t>
+  </si>
+  <si>
+    <t>23.02.20243</t>
+  </si>
+  <si>
+    <t>23.02.20244</t>
+  </si>
+  <si>
+    <t>23.02.20245</t>
+  </si>
+  <si>
+    <t>23.02.20246</t>
+  </si>
+  <si>
+    <t>23.02.20247</t>
+  </si>
+  <si>
+    <t>23.02.20248</t>
+  </si>
+  <si>
+    <t>23.02.20249</t>
+  </si>
+  <si>
+    <t>23.02.202410</t>
+  </si>
+  <si>
+    <t>23.02.202411</t>
+  </si>
+  <si>
+    <t>23.02.202412</t>
+  </si>
+  <si>
+    <t>23.02.202413</t>
+  </si>
+  <si>
+    <t>23.02.202414</t>
   </si>
 </sst>
 </file>
@@ -706,19 +709,16 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="2">
-        <v>45335</v>
+        <v>45341</v>
       </c>
       <c r="B2">
-        <v>13</v>
-      </c>
-      <c r="C2">
-        <v>113.7</v>
+        <v>15</v>
       </c>
       <c r="D2">
-        <v>5.81</v>
+        <v>5.98</v>
       </c>
       <c r="E2">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="F2" t="s">
         <v>6</v>
@@ -726,19 +726,16 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="2">
-        <v>45335</v>
+        <v>45341</v>
       </c>
       <c r="B3">
-        <v>14</v>
-      </c>
-      <c r="C3">
-        <v>95.70999999999999</v>
+        <v>16</v>
       </c>
       <c r="D3">
-        <v>6.14</v>
+        <v>5.52</v>
       </c>
       <c r="E3">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="F3" t="s">
         <v>7</v>
@@ -746,19 +743,16 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="2">
-        <v>45335</v>
+        <v>45341</v>
       </c>
       <c r="B4">
-        <v>15</v>
-      </c>
-      <c r="C4">
-        <v>67.26000000000001</v>
+        <v>17</v>
       </c>
       <c r="D4">
-        <v>6.07</v>
+        <v>4.96</v>
       </c>
       <c r="E4">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="F4" t="s">
         <v>8</v>
@@ -766,19 +760,16 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="2">
-        <v>45335</v>
+        <v>45341</v>
       </c>
       <c r="B5">
-        <v>16</v>
-      </c>
-      <c r="C5">
-        <v>32.55</v>
+        <v>18</v>
       </c>
       <c r="D5">
-        <v>5.75</v>
+        <v>4.35</v>
       </c>
       <c r="E5">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="F5" t="s">
         <v>9</v>
@@ -786,19 +777,16 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="2">
-        <v>45335</v>
+        <v>45341</v>
       </c>
       <c r="B6">
-        <v>17</v>
-      </c>
-      <c r="C6">
-        <v>3.76</v>
+        <v>19</v>
       </c>
       <c r="D6">
-        <v>5.36</v>
+        <v>3.56</v>
       </c>
       <c r="E6">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F6" t="s">
         <v>10</v>
@@ -806,16 +794,13 @@
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="2">
-        <v>45335</v>
+        <v>45341</v>
       </c>
       <c r="B7">
-        <v>18</v>
-      </c>
-      <c r="C7">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="D7">
-        <v>5.08</v>
+        <v>2.71</v>
       </c>
       <c r="E7">
         <v>100</v>
@@ -826,16 +811,13 @@
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="2">
-        <v>45335</v>
+        <v>45341</v>
       </c>
       <c r="B8">
-        <v>19</v>
-      </c>
-      <c r="C8">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="D8">
-        <v>4.82</v>
+        <v>2.62</v>
       </c>
       <c r="E8">
         <v>100</v>
@@ -846,19 +828,16 @@
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="2">
-        <v>45335</v>
+        <v>45341</v>
       </c>
       <c r="B9">
-        <v>20</v>
-      </c>
-      <c r="C9">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="D9">
-        <v>4.59</v>
+        <v>2.34</v>
       </c>
       <c r="E9">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F9" t="s">
         <v>13</v>
@@ -866,19 +845,16 @@
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="2">
-        <v>45335</v>
+        <v>45341</v>
       </c>
       <c r="B10">
-        <v>21</v>
-      </c>
-      <c r="C10">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="D10">
-        <v>4.4</v>
+        <v>2.5</v>
       </c>
       <c r="E10">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="F10" t="s">
         <v>14</v>
@@ -886,19 +862,19 @@
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="2">
-        <v>45335</v>
+        <v>45342</v>
       </c>
       <c r="B11">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="C11">
         <v>0</v>
       </c>
       <c r="D11">
-        <v>3.77</v>
+        <v>3.07</v>
       </c>
       <c r="E11">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="F11" t="s">
         <v>15</v>
@@ -906,16 +882,16 @@
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="2">
-        <v>45335</v>
+        <v>45342</v>
       </c>
       <c r="B12">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="C12">
         <v>0</v>
       </c>
       <c r="D12">
-        <v>3.26</v>
+        <v>2.54</v>
       </c>
       <c r="E12">
         <v>100</v>
@@ -926,16 +902,16 @@
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="2">
-        <v>45336</v>
+        <v>45342</v>
       </c>
       <c r="B13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C13">
         <v>0</v>
       </c>
       <c r="D13">
-        <v>3.11</v>
+        <v>2.65</v>
       </c>
       <c r="E13">
         <v>100</v>
@@ -946,16 +922,16 @@
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="2">
-        <v>45336</v>
+        <v>45342</v>
       </c>
       <c r="B14">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C14">
         <v>0</v>
       </c>
       <c r="D14">
-        <v>2.99</v>
+        <v>2.8</v>
       </c>
       <c r="E14">
         <v>100</v>
@@ -966,16 +942,16 @@
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="2">
-        <v>45336</v>
+        <v>45342</v>
       </c>
       <c r="B15">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C15">
         <v>0</v>
       </c>
       <c r="D15">
-        <v>2.75</v>
+        <v>2.83</v>
       </c>
       <c r="E15">
         <v>100</v>
@@ -986,16 +962,16 @@
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="2">
-        <v>45336</v>
+        <v>45342</v>
       </c>
       <c r="B16">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C16">
         <v>0</v>
       </c>
       <c r="D16">
-        <v>2.69</v>
+        <v>2.8</v>
       </c>
       <c r="E16">
         <v>100</v>
@@ -1006,16 +982,16 @@
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="2">
-        <v>45336</v>
+        <v>45342</v>
       </c>
       <c r="B17">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C17">
         <v>0</v>
       </c>
       <c r="D17">
-        <v>2.62</v>
+        <v>2.84</v>
       </c>
       <c r="E17">
         <v>100</v>
@@ -1026,16 +1002,16 @@
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="2">
-        <v>45336</v>
+        <v>45342</v>
       </c>
       <c r="B18">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C18">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D18">
-        <v>2.39</v>
+        <v>2.97</v>
       </c>
       <c r="E18">
         <v>100</v>
@@ -1046,16 +1022,16 @@
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="2">
-        <v>45336</v>
+        <v>45342</v>
       </c>
       <c r="B19">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C19">
-        <v>0</v>
+        <v>33.99</v>
       </c>
       <c r="D19">
-        <v>2.39</v>
+        <v>3.06</v>
       </c>
       <c r="E19">
         <v>100</v>
@@ -1066,19 +1042,19 @@
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="2">
-        <v>45336</v>
+        <v>45342</v>
       </c>
       <c r="B20">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C20">
-        <v>1.81</v>
+        <v>70.47</v>
       </c>
       <c r="D20">
-        <v>3.14</v>
+        <v>3.15</v>
       </c>
       <c r="E20">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="F20" t="s">
         <v>24</v>
@@ -1086,16 +1062,16 @@
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="2">
-        <v>45336</v>
+        <v>45342</v>
       </c>
       <c r="B21">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C21">
-        <v>28.08</v>
+        <v>101.13</v>
       </c>
       <c r="D21">
-        <v>3.79</v>
+        <v>3.31</v>
       </c>
       <c r="E21">
         <v>100</v>
@@ -1106,16 +1082,16 @@
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="2">
-        <v>45336</v>
+        <v>45342</v>
       </c>
       <c r="B22">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C22">
-        <v>66.31</v>
+        <v>121.56</v>
       </c>
       <c r="D22">
-        <v>4.72</v>
+        <v>3.44</v>
       </c>
       <c r="E22">
         <v>100</v>
@@ -1126,16 +1102,16 @@
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="2">
-        <v>45336</v>
+        <v>45342</v>
       </c>
       <c r="B23">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C23">
-        <v>95.81</v>
+        <v>129.41</v>
       </c>
       <c r="D23">
-        <v>5.55</v>
+        <v>3.55</v>
       </c>
       <c r="E23">
         <v>100</v>
@@ -1146,16 +1122,16 @@
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="2">
-        <v>45336</v>
+        <v>45342</v>
       </c>
       <c r="B24">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C24">
-        <v>115.85</v>
+        <v>123.84</v>
       </c>
       <c r="D24">
-        <v>6.2</v>
+        <v>3.64</v>
       </c>
       <c r="E24">
         <v>100</v>
@@ -1166,16 +1142,16 @@
     </row>
     <row r="25" spans="1:6">
       <c r="A25" s="2">
-        <v>45336</v>
+        <v>45342</v>
       </c>
       <c r="B25">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C25">
-        <v>123.98</v>
+        <v>105.93</v>
       </c>
       <c r="D25">
-        <v>6.53</v>
+        <v>3.72</v>
       </c>
       <c r="E25">
         <v>100</v>
@@ -1186,16 +1162,16 @@
     </row>
     <row r="26" spans="1:6">
       <c r="A26" s="2">
-        <v>45336</v>
+        <v>45342</v>
       </c>
       <c r="B26">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C26">
-        <v>118.87</v>
+        <v>77.31</v>
       </c>
       <c r="D26">
-        <v>6.52</v>
+        <v>3.65</v>
       </c>
       <c r="E26">
         <v>100</v>
@@ -1206,19 +1182,19 @@
     </row>
     <row r="27" spans="1:6">
       <c r="A27" s="2">
-        <v>45336</v>
+        <v>45342</v>
       </c>
       <c r="B27">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C27">
-        <v>99.16</v>
+        <v>40.89</v>
       </c>
       <c r="D27">
-        <v>6.37</v>
+        <v>2.76</v>
       </c>
       <c r="E27">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="F27" t="s">
         <v>31</v>
@@ -1226,19 +1202,19 @@
     </row>
     <row r="28" spans="1:6">
       <c r="A28" s="2">
-        <v>45336</v>
+        <v>45342</v>
       </c>
       <c r="B28">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C28">
-        <v>68.48</v>
+        <v>7.94</v>
       </c>
       <c r="D28">
-        <v>5.89</v>
+        <v>2.13</v>
       </c>
       <c r="E28">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="F28" t="s">
         <v>32</v>
@@ -1246,19 +1222,19 @@
     </row>
     <row r="29" spans="1:6">
       <c r="A29" s="2">
-        <v>45336</v>
+        <v>45342</v>
       </c>
       <c r="B29">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C29">
-        <v>35.03</v>
+        <v>0</v>
       </c>
       <c r="D29">
-        <v>4.47</v>
+        <v>1.96</v>
       </c>
       <c r="E29">
-        <v>95</v>
+        <v>78</v>
       </c>
       <c r="F29" t="s">
         <v>33</v>
@@ -1266,19 +1242,19 @@
     </row>
     <row r="30" spans="1:6">
       <c r="A30" s="2">
-        <v>45336</v>
+        <v>45342</v>
       </c>
       <c r="B30">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C30">
-        <v>4.83</v>
+        <v>0</v>
       </c>
       <c r="D30">
-        <v>3.32</v>
+        <v>1.7</v>
       </c>
       <c r="E30">
-        <v>85</v>
+        <v>32</v>
       </c>
       <c r="F30" t="s">
         <v>34</v>
@@ -1286,19 +1262,19 @@
     </row>
     <row r="31" spans="1:6">
       <c r="A31" s="2">
-        <v>45336</v>
+        <v>45342</v>
       </c>
       <c r="B31">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C31">
         <v>0</v>
       </c>
       <c r="D31">
-        <v>2.57</v>
+        <v>1.66</v>
       </c>
       <c r="E31">
-        <v>79</v>
+        <v>37</v>
       </c>
       <c r="F31" t="s">
         <v>35</v>
@@ -1306,19 +1282,19 @@
     </row>
     <row r="32" spans="1:6">
       <c r="A32" s="2">
-        <v>45336</v>
+        <v>45342</v>
       </c>
       <c r="B32">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C32">
         <v>0</v>
       </c>
       <c r="D32">
-        <v>2.13</v>
+        <v>1.81</v>
       </c>
       <c r="E32">
-        <v>73</v>
+        <v>49</v>
       </c>
       <c r="F32" t="s">
         <v>36</v>
@@ -1326,19 +1302,19 @@
     </row>
     <row r="33" spans="1:6">
       <c r="A33" s="2">
-        <v>45336</v>
+        <v>45342</v>
       </c>
       <c r="B33">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C33">
         <v>0</v>
       </c>
       <c r="D33">
-        <v>1.85</v>
+        <v>2.03</v>
       </c>
       <c r="E33">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="F33" t="s">
         <v>37</v>
@@ -1346,19 +1322,19 @@
     </row>
     <row r="34" spans="1:6">
       <c r="A34" s="2">
-        <v>45336</v>
+        <v>45342</v>
       </c>
       <c r="B34">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C34">
         <v>0</v>
       </c>
       <c r="D34">
-        <v>1.47</v>
+        <v>2</v>
       </c>
       <c r="E34">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="F34" t="s">
         <v>38</v>
@@ -1366,19 +1342,19 @@
     </row>
     <row r="35" spans="1:6">
       <c r="A35" s="2">
-        <v>45336</v>
+        <v>45343</v>
       </c>
       <c r="B35">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="C35">
         <v>0</v>
       </c>
       <c r="D35">
-        <v>1.31</v>
+        <v>2.14</v>
       </c>
       <c r="E35">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="F35" t="s">
         <v>39</v>
@@ -1386,19 +1362,19 @@
     </row>
     <row r="36" spans="1:6">
       <c r="A36" s="2">
-        <v>45336</v>
+        <v>45343</v>
       </c>
       <c r="B36">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="C36">
         <v>0</v>
       </c>
       <c r="D36">
-        <v>1.24</v>
+        <v>2.66</v>
       </c>
       <c r="E36">
-        <v>61</v>
+        <v>100</v>
       </c>
       <c r="F36" t="s">
         <v>40</v>
@@ -1406,19 +1382,19 @@
     </row>
     <row r="37" spans="1:6">
       <c r="A37" s="2">
-        <v>45337</v>
+        <v>45343</v>
       </c>
       <c r="B37">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C37">
         <v>0</v>
       </c>
       <c r="D37">
-        <v>1.25</v>
+        <v>2.82</v>
       </c>
       <c r="E37">
-        <v>63</v>
+        <v>100</v>
       </c>
       <c r="F37" t="s">
         <v>41</v>
@@ -1426,19 +1402,19 @@
     </row>
     <row r="38" spans="1:6">
       <c r="A38" s="2">
-        <v>45337</v>
+        <v>45343</v>
       </c>
       <c r="B38">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C38">
         <v>0</v>
       </c>
       <c r="D38">
-        <v>0.88</v>
+        <v>2.8</v>
       </c>
       <c r="E38">
-        <v>58</v>
+        <v>100</v>
       </c>
       <c r="F38" t="s">
         <v>42</v>
@@ -1446,19 +1422,19 @@
     </row>
     <row r="39" spans="1:6">
       <c r="A39" s="2">
-        <v>45337</v>
+        <v>45343</v>
       </c>
       <c r="B39">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C39">
         <v>0</v>
       </c>
       <c r="D39">
-        <v>0.71</v>
+        <v>2.82</v>
       </c>
       <c r="E39">
-        <v>44</v>
+        <v>100</v>
       </c>
       <c r="F39" t="s">
         <v>43</v>
@@ -1466,19 +1442,19 @@
     </row>
     <row r="40" spans="1:6">
       <c r="A40" s="2">
-        <v>45337</v>
+        <v>45343</v>
       </c>
       <c r="B40">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C40">
         <v>0</v>
       </c>
       <c r="D40">
-        <v>0.64</v>
+        <v>2.88</v>
       </c>
       <c r="E40">
-        <v>37</v>
+        <v>100</v>
       </c>
       <c r="F40" t="s">
         <v>44</v>
@@ -1486,19 +1462,19 @@
     </row>
     <row r="41" spans="1:6">
       <c r="A41" s="2">
-        <v>45337</v>
+        <v>45343</v>
       </c>
       <c r="B41">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C41">
         <v>0</v>
       </c>
       <c r="D41">
-        <v>0.61</v>
+        <v>3.13</v>
       </c>
       <c r="E41">
-        <v>33</v>
+        <v>100</v>
       </c>
       <c r="F41" t="s">
         <v>45</v>
@@ -1506,19 +1482,19 @@
     </row>
     <row r="42" spans="1:6">
       <c r="A42" s="2">
-        <v>45337</v>
+        <v>45343</v>
       </c>
       <c r="B42">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C42">
-        <v>0</v>
+        <v>4.6</v>
       </c>
       <c r="D42">
-        <v>0.61</v>
+        <v>3.96</v>
       </c>
       <c r="E42">
-        <v>31</v>
+        <v>99</v>
       </c>
       <c r="F42" t="s">
         <v>46</v>
@@ -1526,19 +1502,19 @@
     </row>
     <row r="43" spans="1:6">
       <c r="A43" s="2">
-        <v>45337</v>
+        <v>45343</v>
       </c>
       <c r="B43">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C43">
-        <v>0</v>
+        <v>37.75</v>
       </c>
       <c r="D43">
-        <v>0.93</v>
+        <v>4.53</v>
       </c>
       <c r="E43">
-        <v>28</v>
+        <v>99</v>
       </c>
       <c r="F43" t="s">
         <v>47</v>
@@ -1546,19 +1522,19 @@
     </row>
     <row r="44" spans="1:6">
       <c r="A44" s="2">
-        <v>45337</v>
+        <v>45343</v>
       </c>
       <c r="B44">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C44">
-        <v>8.34</v>
+        <v>78.94</v>
       </c>
       <c r="D44">
-        <v>2.55</v>
+        <v>4.96</v>
       </c>
       <c r="E44">
-        <v>17</v>
+        <v>100</v>
       </c>
       <c r="F44" t="s">
         <v>48</v>
@@ -1566,19 +1542,19 @@
     </row>
     <row r="45" spans="1:6">
       <c r="A45" s="2">
-        <v>45337</v>
+        <v>45343</v>
       </c>
       <c r="B45">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C45">
-        <v>111.86</v>
+        <v>109.24</v>
       </c>
       <c r="D45">
-        <v>4.13</v>
+        <v>5.58</v>
       </c>
       <c r="E45">
-        <v>15</v>
+        <v>100</v>
       </c>
       <c r="F45" t="s">
         <v>49</v>
@@ -1586,19 +1562,19 @@
     </row>
     <row r="46" spans="1:6">
       <c r="A46" s="2">
-        <v>45337</v>
+        <v>45343</v>
       </c>
       <c r="B46">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C46">
-        <v>254.06</v>
+        <v>128.51</v>
       </c>
       <c r="D46">
-        <v>5.41</v>
+        <v>5.52</v>
       </c>
       <c r="E46">
-        <v>14</v>
+        <v>100</v>
       </c>
       <c r="F46" t="s">
         <v>50</v>
@@ -1606,19 +1582,19 @@
     </row>
     <row r="47" spans="1:6">
       <c r="A47" s="2">
-        <v>45337</v>
+        <v>45343</v>
       </c>
       <c r="B47">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C47">
-        <v>374.87</v>
+        <v>135.62</v>
       </c>
       <c r="D47">
-        <v>6.22</v>
+        <v>4.74</v>
       </c>
       <c r="E47">
-        <v>13</v>
+        <v>100</v>
       </c>
       <c r="F47" t="s">
         <v>51</v>
@@ -1626,19 +1602,19 @@
     </row>
     <row r="48" spans="1:6">
       <c r="A48" s="2">
-        <v>45337</v>
+        <v>45343</v>
       </c>
       <c r="B48">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C48">
-        <v>455.85</v>
+        <v>129.17</v>
       </c>
       <c r="D48">
-        <v>6.72</v>
+        <v>4.64</v>
       </c>
       <c r="E48">
-        <v>12</v>
+        <v>100</v>
       </c>
       <c r="F48" t="s">
         <v>52</v>
@@ -1646,19 +1622,19 @@
     </row>
     <row r="49" spans="1:6">
       <c r="A49" s="2">
-        <v>45337</v>
+        <v>45343</v>
       </c>
       <c r="B49">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C49">
-        <v>487.28</v>
+        <v>109.32</v>
       </c>
       <c r="D49">
-        <v>6.96</v>
+        <v>4.9</v>
       </c>
       <c r="E49">
-        <v>12</v>
+        <v>95</v>
       </c>
       <c r="F49" t="s">
         <v>53</v>
@@ -1666,680 +1642,917 @@
     </row>
     <row r="50" spans="1:6">
       <c r="A50" s="2">
-        <v>45337</v>
+        <v>45343</v>
       </c>
       <c r="B50">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C50">
-        <v>487.28</v>
+        <v>91.27</v>
       </c>
       <c r="D50">
-        <v>6.96</v>
+        <v>4.57</v>
       </c>
       <c r="E50">
-        <v>12</v>
+        <v>93</v>
       </c>
       <c r="F50" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="51" spans="1:6">
       <c r="A51" s="2">
-        <v>45337</v>
+        <v>45343</v>
       </c>
       <c r="B51">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C51">
-        <v>465.63</v>
+        <v>64.03</v>
+      </c>
+      <c r="D51">
+        <v>3.08</v>
+      </c>
+      <c r="E51">
+        <v>90</v>
       </c>
       <c r="F51" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="52" spans="1:6">
       <c r="A52" s="2">
-        <v>45337</v>
+        <v>45343</v>
       </c>
       <c r="B52">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C52">
-        <v>392.43</v>
+        <v>13.47</v>
+      </c>
+      <c r="D52">
+        <v>3.66</v>
+      </c>
+      <c r="E52">
+        <v>92</v>
       </c>
       <c r="F52" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="53" spans="1:6">
       <c r="A53" s="2">
-        <v>45337</v>
+        <v>45343</v>
       </c>
       <c r="B53">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C53">
-        <v>275.97</v>
+        <v>0</v>
+      </c>
+      <c r="D53">
+        <v>3.69</v>
+      </c>
+      <c r="E53">
+        <v>93</v>
       </c>
       <c r="F53" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="54" spans="1:6">
       <c r="A54" s="2">
-        <v>45337</v>
+        <v>45343</v>
       </c>
       <c r="B54">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C54">
-        <v>137.13</v>
+        <v>0</v>
+      </c>
+      <c r="D54">
+        <v>3.58</v>
+      </c>
+      <c r="E54">
+        <v>100</v>
       </c>
       <c r="F54" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="55" spans="1:6">
       <c r="A55" s="2">
-        <v>45337</v>
+        <v>45343</v>
       </c>
       <c r="B55">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C55">
-        <v>17.85</v>
+        <v>0</v>
+      </c>
+      <c r="D55">
+        <v>3.53</v>
+      </c>
+      <c r="E55">
+        <v>100</v>
       </c>
       <c r="F55" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="56" spans="1:6">
       <c r="A56" s="2">
-        <v>45337</v>
+        <v>45343</v>
       </c>
       <c r="B56">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C56">
         <v>0</v>
       </c>
+      <c r="D56">
+        <v>3.49</v>
+      </c>
+      <c r="E56">
+        <v>100</v>
+      </c>
       <c r="F56" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="57" spans="1:6">
       <c r="A57" s="2">
-        <v>45337</v>
+        <v>45343</v>
       </c>
       <c r="B57">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C57">
         <v>0</v>
       </c>
+      <c r="D57">
+        <v>3.43</v>
+      </c>
+      <c r="E57">
+        <v>100</v>
+      </c>
       <c r="F57" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="58" spans="1:6">
       <c r="A58" s="2">
-        <v>45337</v>
+        <v>45343</v>
       </c>
       <c r="B58">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C58">
         <v>0</v>
       </c>
+      <c r="D58">
+        <v>2.62</v>
+      </c>
+      <c r="E58">
+        <v>100</v>
+      </c>
       <c r="F58" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="59" spans="1:6">
       <c r="A59" s="2">
-        <v>45337</v>
+        <v>45344</v>
       </c>
       <c r="B59">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="C59">
         <v>0</v>
       </c>
+      <c r="D59">
+        <v>2.87</v>
+      </c>
+      <c r="E59">
+        <v>100</v>
+      </c>
       <c r="F59" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="60" spans="1:6">
       <c r="A60" s="2">
-        <v>45337</v>
+        <v>45344</v>
       </c>
       <c r="B60">
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="C60">
         <v>0</v>
       </c>
+      <c r="D60">
+        <v>3.03</v>
+      </c>
+      <c r="E60">
+        <v>100</v>
+      </c>
       <c r="F60" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="61" spans="1:6">
       <c r="A61" s="2">
-        <v>45337</v>
+        <v>45344</v>
       </c>
       <c r="B61">
-        <v>23</v>
+        <v>2</v>
       </c>
       <c r="C61">
         <v>0</v>
       </c>
+      <c r="D61">
+        <v>2.96</v>
+      </c>
+      <c r="E61">
+        <v>100</v>
+      </c>
       <c r="F61" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="62" spans="1:6">
       <c r="A62" s="2">
-        <v>45338</v>
+        <v>45344</v>
       </c>
       <c r="B62">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C62">
         <v>0</v>
       </c>
+      <c r="D62">
+        <v>2.92</v>
+      </c>
+      <c r="E62">
+        <v>100</v>
+      </c>
       <c r="F62" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="63" spans="1:6">
       <c r="A63" s="2">
-        <v>45338</v>
+        <v>45344</v>
       </c>
       <c r="B63">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C63">
         <v>0</v>
       </c>
+      <c r="D63">
+        <v>2.87</v>
+      </c>
+      <c r="E63">
+        <v>100</v>
+      </c>
       <c r="F63" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="64" spans="1:6">
       <c r="A64" s="2">
-        <v>45338</v>
+        <v>45344</v>
       </c>
       <c r="B64">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C64">
         <v>0</v>
       </c>
+      <c r="D64">
+        <v>2.76</v>
+      </c>
+      <c r="E64">
+        <v>100</v>
+      </c>
       <c r="F64" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="65" spans="1:6">
       <c r="A65" s="2">
-        <v>45338</v>
+        <v>45344</v>
       </c>
       <c r="B65">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C65">
         <v>0</v>
       </c>
+      <c r="D65">
+        <v>2.85</v>
+      </c>
+      <c r="E65">
+        <v>100</v>
+      </c>
       <c r="F65" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="66" spans="1:6">
       <c r="A66" s="2">
-        <v>45338</v>
+        <v>45344</v>
       </c>
       <c r="B66">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C66">
-        <v>0</v>
+        <v>5.15</v>
+      </c>
+      <c r="D66">
+        <v>3.42</v>
+      </c>
+      <c r="E66">
+        <v>99</v>
       </c>
       <c r="F66" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="67" spans="1:6">
       <c r="A67" s="2">
-        <v>45338</v>
+        <v>45344</v>
       </c>
       <c r="B67">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C67">
-        <v>0</v>
+        <v>38.22</v>
+      </c>
+      <c r="D67">
+        <v>4.48</v>
+      </c>
+      <c r="E67">
+        <v>100</v>
       </c>
       <c r="F67" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="68" spans="1:6">
       <c r="A68" s="2">
-        <v>45338</v>
+        <v>45344</v>
       </c>
       <c r="B68">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C68">
-        <v>0</v>
+        <v>77.43000000000001</v>
+      </c>
+      <c r="D68">
+        <v>5.63</v>
+      </c>
+      <c r="E68">
+        <v>100</v>
       </c>
       <c r="F68" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="69" spans="1:6">
       <c r="A69" s="2">
-        <v>45338</v>
+        <v>45344</v>
       </c>
       <c r="B69">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C69">
-        <v>9.74</v>
+        <v>107.36</v>
+      </c>
+      <c r="D69">
+        <v>6.69</v>
+      </c>
+      <c r="E69">
+        <v>100</v>
       </c>
       <c r="F69" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="70" spans="1:6">
       <c r="A70" s="2">
-        <v>45338</v>
+        <v>45344</v>
       </c>
       <c r="B70">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C70">
-        <v>116.88</v>
+        <v>127.31</v>
+      </c>
+      <c r="D70">
+        <v>7.28</v>
+      </c>
+      <c r="E70">
+        <v>100</v>
       </c>
       <c r="F70" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="71" spans="1:6">
       <c r="A71" s="2">
-        <v>45338</v>
+        <v>45344</v>
       </c>
       <c r="B71">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C71">
-        <v>259.58</v>
+        <v>134.71</v>
+      </c>
+      <c r="D71">
+        <v>7.78</v>
+      </c>
+      <c r="E71">
+        <v>100</v>
       </c>
       <c r="F71" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="72" spans="1:6">
       <c r="A72" s="2">
-        <v>45338</v>
+        <v>45344</v>
       </c>
       <c r="B72">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C72">
-        <v>380.66</v>
+        <v>128.66</v>
+      </c>
+      <c r="D72">
+        <v>8.220000000000001</v>
+      </c>
+      <c r="E72">
+        <v>90</v>
       </c>
       <c r="F72" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="73" spans="1:6">
       <c r="A73" s="2">
-        <v>45338</v>
+        <v>45344</v>
       </c>
       <c r="B73">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C73">
-        <v>461.51</v>
+        <v>147.39</v>
+      </c>
+      <c r="D73">
+        <v>8.26</v>
+      </c>
+      <c r="E73">
+        <v>85</v>
       </c>
       <c r="F73" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="74" spans="1:6">
       <c r="A74" s="2">
-        <v>45338</v>
+        <v>45344</v>
       </c>
       <c r="B74">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C74">
-        <v>492.89</v>
+        <v>162.45</v>
+      </c>
+      <c r="D74">
+        <v>7.44</v>
+      </c>
+      <c r="E74">
+        <v>88</v>
       </c>
       <c r="F74" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="75" spans="1:6">
       <c r="A75" s="2">
-        <v>45338</v>
+        <v>45344</v>
       </c>
       <c r="B75">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C75">
-        <v>471.25</v>
+        <v>94.28</v>
+      </c>
+      <c r="D75">
+        <v>5.82</v>
+      </c>
+      <c r="E75">
+        <v>91</v>
       </c>
       <c r="F75" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="76" spans="1:6">
       <c r="A76" s="2">
-        <v>45338</v>
+        <v>45344</v>
       </c>
       <c r="B76">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C76">
-        <v>398.87</v>
+        <v>17.03</v>
+      </c>
+      <c r="D76">
+        <v>4.83</v>
+      </c>
+      <c r="E76">
+        <v>93</v>
       </c>
       <c r="F76" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="77" spans="1:6">
       <c r="A77" s="2">
-        <v>45338</v>
+        <v>45344</v>
       </c>
       <c r="B77">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C77">
-        <v>284.12</v>
+        <v>0</v>
+      </c>
+      <c r="D77">
+        <v>4.22</v>
+      </c>
+      <c r="E77">
+        <v>94</v>
       </c>
       <c r="F77" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="78" spans="1:6">
       <c r="A78" s="2">
-        <v>45338</v>
+        <v>45344</v>
       </c>
       <c r="B78">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C78">
-        <v>143.28</v>
+        <v>0</v>
+      </c>
+      <c r="D78">
+        <v>4.37</v>
+      </c>
+      <c r="E78">
+        <v>100</v>
       </c>
       <c r="F78" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="79" spans="1:6">
       <c r="A79" s="2">
-        <v>45338</v>
+        <v>45344</v>
       </c>
       <c r="B79">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C79">
-        <v>20.45</v>
+        <v>0</v>
+      </c>
+      <c r="D79">
+        <v>4.4</v>
+      </c>
+      <c r="E79">
+        <v>99</v>
       </c>
       <c r="F79" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="80" spans="1:6">
       <c r="A80" s="2">
-        <v>45338</v>
+        <v>45344</v>
       </c>
       <c r="B80">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C80">
         <v>0</v>
       </c>
+      <c r="D80">
+        <v>4.07</v>
+      </c>
+      <c r="E80">
+        <v>99</v>
+      </c>
       <c r="F80" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="81" spans="1:6">
       <c r="A81" s="2">
-        <v>45338</v>
+        <v>45344</v>
       </c>
       <c r="B81">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C81">
         <v>0</v>
       </c>
+      <c r="D81">
+        <v>3.94</v>
+      </c>
+      <c r="E81">
+        <v>95</v>
+      </c>
       <c r="F81" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="82" spans="1:6">
       <c r="A82" s="2">
-        <v>45338</v>
+        <v>45344</v>
       </c>
       <c r="B82">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C82">
         <v>0</v>
       </c>
+      <c r="D82">
+        <v>3.9</v>
+      </c>
+      <c r="E82">
+        <v>95</v>
+      </c>
       <c r="F82" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="83" spans="1:6">
       <c r="A83" s="2">
-        <v>45338</v>
+        <v>45345</v>
       </c>
       <c r="B83">
-        <v>21</v>
-      </c>
-      <c r="C83">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="D83">
+        <v>4</v>
+      </c>
+      <c r="E83">
+        <v>96</v>
       </c>
       <c r="F83" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="84" spans="1:6">
       <c r="A84" s="2">
-        <v>45338</v>
+        <v>45345</v>
       </c>
       <c r="B84">
-        <v>22</v>
-      </c>
-      <c r="C84">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="D84">
+        <v>4.2</v>
+      </c>
+      <c r="E84">
+        <v>100</v>
       </c>
       <c r="F84" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="85" spans="1:6">
       <c r="A85" s="2">
-        <v>45338</v>
+        <v>45345</v>
       </c>
       <c r="B85">
-        <v>23</v>
-      </c>
-      <c r="C85">
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="D85">
+        <v>4.05</v>
+      </c>
+      <c r="E85">
+        <v>100</v>
       </c>
       <c r="F85" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="86" spans="1:6">
       <c r="A86" s="2">
-        <v>45339</v>
+        <v>45345</v>
       </c>
       <c r="B86">
-        <v>0</v>
-      </c>
-      <c r="C86">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="D86">
+        <v>4.23</v>
+      </c>
+      <c r="E86">
+        <v>100</v>
       </c>
       <c r="F86" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="87" spans="1:6">
       <c r="A87" s="2">
-        <v>45339</v>
+        <v>45345</v>
       </c>
       <c r="B87">
-        <v>1</v>
-      </c>
-      <c r="C87">
-        <v>0</v>
+        <v>4</v>
+      </c>
+      <c r="D87">
+        <v>4.17</v>
+      </c>
+      <c r="E87">
+        <v>100</v>
       </c>
       <c r="F87" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="88" spans="1:6">
       <c r="A88" s="2">
-        <v>45339</v>
+        <v>45345</v>
       </c>
       <c r="B88">
-        <v>2</v>
-      </c>
-      <c r="C88">
-        <v>0</v>
+        <v>5</v>
+      </c>
+      <c r="D88">
+        <v>3.95</v>
+      </c>
+      <c r="E88">
+        <v>100</v>
       </c>
       <c r="F88" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="89" spans="1:6">
       <c r="A89" s="2">
-        <v>45339</v>
+        <v>45345</v>
       </c>
       <c r="B89">
-        <v>3</v>
-      </c>
-      <c r="C89">
-        <v>0</v>
+        <v>6</v>
+      </c>
+      <c r="D89">
+        <v>4.77</v>
+      </c>
+      <c r="E89">
+        <v>100</v>
       </c>
       <c r="F89" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="90" spans="1:6">
       <c r="A90" s="2">
-        <v>45339</v>
+        <v>45345</v>
       </c>
       <c r="B90">
-        <v>4</v>
-      </c>
-      <c r="C90">
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="D90">
+        <v>6.04</v>
+      </c>
+      <c r="E90">
+        <v>100</v>
       </c>
       <c r="F90" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="91" spans="1:6">
       <c r="A91" s="2">
-        <v>45339</v>
+        <v>45345</v>
       </c>
       <c r="B91">
-        <v>5</v>
-      </c>
-      <c r="C91">
-        <v>0</v>
+        <v>8</v>
+      </c>
+      <c r="D91">
+        <v>6.95</v>
+      </c>
+      <c r="E91">
+        <v>100</v>
       </c>
       <c r="F91" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="92" spans="1:6">
       <c r="A92" s="2">
-        <v>45339</v>
+        <v>45345</v>
       </c>
       <c r="B92">
-        <v>6</v>
-      </c>
-      <c r="C92">
-        <v>0</v>
+        <v>9</v>
+      </c>
+      <c r="D92">
+        <v>8.5</v>
+      </c>
+      <c r="E92">
+        <v>100</v>
       </c>
       <c r="F92" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="93" spans="1:6">
       <c r="A93" s="2">
-        <v>45339</v>
+        <v>45345</v>
       </c>
       <c r="B93">
-        <v>7</v>
-      </c>
-      <c r="C93">
-        <v>11.15</v>
+        <v>10</v>
+      </c>
+      <c r="D93">
+        <v>9.69</v>
+      </c>
+      <c r="E93">
+        <v>100</v>
       </c>
       <c r="F93" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="94" spans="1:6">
       <c r="A94" s="2">
-        <v>45339</v>
+        <v>45345</v>
       </c>
       <c r="B94">
-        <v>8</v>
-      </c>
-      <c r="C94">
-        <v>121.51</v>
+        <v>11</v>
+      </c>
+      <c r="D94">
+        <v>10.99</v>
+      </c>
+      <c r="E94">
+        <v>100</v>
       </c>
       <c r="F94" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="95" spans="1:6">
       <c r="A95" s="2">
-        <v>45339</v>
+        <v>45345</v>
       </c>
       <c r="B95">
-        <v>9</v>
-      </c>
-      <c r="C95">
-        <v>265.09</v>
+        <v>12</v>
+      </c>
+      <c r="D95">
+        <v>11.54</v>
+      </c>
+      <c r="E95">
+        <v>100</v>
       </c>
       <c r="F95" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="96" spans="1:6">
       <c r="A96" s="2">
-        <v>45339</v>
+        <v>45345</v>
       </c>
       <c r="B96">
-        <v>10</v>
-      </c>
-      <c r="C96">
-        <v>386.67</v>
+        <v>13</v>
+      </c>
+      <c r="D96">
+        <v>11.74</v>
+      </c>
+      <c r="E96">
+        <v>89</v>
       </c>
       <c r="F96" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="97" spans="1:6">
       <c r="A97" s="2">
-        <v>45339</v>
+        <v>45345</v>
       </c>
       <c r="B97">
-        <v>11</v>
-      </c>
-      <c r="C97">
-        <v>467.97</v>
+        <v>14</v>
+      </c>
+      <c r="D97">
+        <v>11.52</v>
+      </c>
+      <c r="E97">
+        <v>89</v>
       </c>
       <c r="F97" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>

</xml_diff>